<commit_message>
Major cleanup on executing a round
Also added the beginnings of damage calculations to be able to simulate basic, STR-based combat.
</commit_message>
<xml_diff>
--- a/Battle Log.xlsx
+++ b/Battle Log.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scrummel\source\repos\pillar\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="75" windowWidth="24915" windowHeight="12840"/>
   </bookViews>
@@ -10,12 +15,12 @@
     <sheet name="Battle 1" sheetId="1" r:id="rId1"/>
     <sheet name="Battle 2" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="25">
   <si>
     <t>NAME</t>
   </si>
@@ -26,18 +31,12 @@
     <t>MONS</t>
   </si>
   <si>
-    <t>ROBO</t>
-  </si>
-  <si>
     <t>LongSword</t>
   </si>
   <si>
     <t>Nail</t>
   </si>
   <si>
-    <t>Colt</t>
-  </si>
-  <si>
     <t>Goblin</t>
   </si>
   <si>
@@ -96,16 +95,13 @@
   </si>
   <si>
     <t>Index</t>
-  </si>
-  <si>
-    <t>DarkRose</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -144,6 +140,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -192,7 +191,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -224,9 +223,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -258,6 +258,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -433,14 +434,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="5" width="11.7109375" customWidth="1"/>
     <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
@@ -451,54 +452,54 @@
     <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" t="s">
+      <c r="H1" t="s">
         <v>14</v>
       </c>
-      <c r="E1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>15</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>16</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>17</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>18</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>19</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O1" t="s">
         <v>20</v>
       </c>
-      <c r="M1" t="s">
-        <v>21</v>
-      </c>
-      <c r="N1" t="s">
-        <v>25</v>
-      </c>
-      <c r="O1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15">
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="str">
         <f>B2</f>
         <v>HUME</v>
@@ -507,102 +508,78 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="L2" t="s">
         <v>3</v>
       </c>
-      <c r="L2" t="s">
-        <v>4</v>
-      </c>
       <c r="M2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
-        <f t="shared" ref="A3:A6" si="0">B3</f>
+        <f t="shared" ref="A3:A5" si="0">B3</f>
         <v>MONS</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L3" t="s">
+        <v>4</v>
+      </c>
+      <c r="M3" t="s">
         <v>5</v>
       </c>
-      <c r="M3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15">
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="str">
         <f t="shared" si="0"/>
-        <v>ROBO</v>
+        <v>Goblin</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="L4" t="s">
-        <v>6</v>
-      </c>
-      <c r="M4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="str">
         <f t="shared" si="0"/>
-        <v>Goblin</v>
+        <v>Jaguar</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15">
-      <c r="A6" t="str">
-        <f t="shared" si="0"/>
-        <v>DarkRose</v>
-      </c>
-      <c r="B6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L3">
       <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>
@@ -611,75 +588,75 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" t="s">
+      <c r="H1" t="s">
         <v>14</v>
       </c>
-      <c r="E1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>15</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>16</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>17</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>18</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>19</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O1" t="s">
         <v>20</v>
       </c>
-      <c r="M1" t="s">
-        <v>21</v>
-      </c>
-      <c r="N1" t="s">
-        <v>25</v>
-      </c>
-      <c r="O1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15">
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="str">
         <f>B2</f>
         <v>MUTE</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -688,16 +665,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
         <f>B3</f>
         <v>Spider</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D3">
         <v>1</v>

</xml_diff>

<commit_message>
Added flags for status effects
</commit_message>
<xml_diff>
--- a/Battle Log.xlsx
+++ b/Battle Log.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="33">
   <si>
     <t>NAME</t>
   </si>
@@ -95,6 +95,30 @@
   </si>
   <si>
     <t>Index</t>
+  </si>
+  <si>
+    <t>Cursed</t>
+  </si>
+  <si>
+    <t>Stunned</t>
+  </si>
+  <si>
+    <t>Paralyzed</t>
+  </si>
+  <si>
+    <t>Poisoned</t>
+  </si>
+  <si>
+    <t>Confused</t>
+  </si>
+  <si>
+    <t>Blinded</t>
+  </si>
+  <si>
+    <t>Stoned</t>
+  </si>
+  <si>
+    <t>Dead</t>
   </si>
 </sst>
 </file>
@@ -435,10 +459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O5"/>
+  <dimension ref="A1:V5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -450,9 +474,10 @@
     <col min="10" max="10" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -493,13 +518,34 @@
         <v>19</v>
       </c>
       <c r="N1" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="O1" t="s">
+        <v>25</v>
+      </c>
+      <c r="P1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>26</v>
+      </c>
+      <c r="R1" t="s">
+        <v>27</v>
+      </c>
+      <c r="S1" t="s">
+        <v>28</v>
+      </c>
+      <c r="T1" t="s">
+        <v>29</v>
+      </c>
+      <c r="U1" t="s">
+        <v>32</v>
+      </c>
+      <c r="V1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" t="str">
         <f>B2</f>
         <v>HUME</v>
@@ -523,7 +569,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
         <f t="shared" ref="A3:A5" si="0">B3</f>
         <v>MONS</v>
@@ -547,7 +593,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4" t="str">
         <f t="shared" si="0"/>
         <v>Goblin</v>
@@ -559,10 +605,10 @@
         <v>22</v>
       </c>
       <c r="D4">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5" t="str">
         <f t="shared" si="0"/>
         <v>Jaguar</v>
@@ -574,7 +620,7 @@
         <v>22</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adjustments made for Dead status
</commit_message>
<xml_diff>
--- a/Battle Log.xlsx
+++ b/Battle Log.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="32">
   <si>
     <t>NAME</t>
   </si>
@@ -116,9 +116,6 @@
   </si>
   <si>
     <t>Stoned</t>
-  </si>
-  <si>
-    <t>Dead</t>
   </si>
 </sst>
 </file>
@@ -459,10 +456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V5"/>
+  <dimension ref="A1:U5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="U1" sqref="U1:U1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -474,10 +471,10 @@
     <col min="10" max="10" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -539,13 +536,10 @@
         <v>29</v>
       </c>
       <c r="U1" t="s">
-        <v>32</v>
-      </c>
-      <c r="V1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" t="str">
         <f>B2</f>
         <v>HUME</v>
@@ -569,7 +563,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
         <f t="shared" ref="A3:A5" si="0">B3</f>
         <v>MONS</v>
@@ -593,7 +587,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" t="str">
         <f t="shared" si="0"/>
         <v>Goblin</v>
@@ -608,7 +602,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" t="str">
         <f t="shared" si="0"/>
         <v>Jaguar</v>

</xml_diff>

<commit_message>
Get master back to current
Messed up the branching. Need to merge good code back into master.
</commit_message>
<xml_diff>
--- a/Battle Log.xlsx
+++ b/Battle Log.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scrummel\source\repos\pillar\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="75" windowWidth="24915" windowHeight="12840"/>
   </bookViews>
@@ -15,12 +10,12 @@
     <sheet name="Battle 1" sheetId="1" r:id="rId1"/>
     <sheet name="Battle 2" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="31">
   <si>
     <t>NAME</t>
   </si>
@@ -38,9 +33,6 @@
   </si>
   <si>
     <t>Goblin</t>
-  </si>
-  <si>
-    <t>Jaguar</t>
   </si>
   <si>
     <t>Position</t>
@@ -121,8 +113,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -212,7 +204,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -244,10 +236,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -279,7 +270,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -455,14 +445,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:U4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="U1" sqref="U1:U1048576"/>
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="4" max="5" width="11.7109375" customWidth="1"/>
     <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
@@ -474,72 +464,72 @@
     <col min="21" max="21" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
         <v>12</v>
       </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>13</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>14</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>15</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>16</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>17</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>18</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>25</v>
+      </c>
+      <c r="R1" t="s">
+        <v>26</v>
+      </c>
+      <c r="S1" t="s">
+        <v>27</v>
+      </c>
+      <c r="T1" t="s">
+        <v>28</v>
+      </c>
+      <c r="U1" t="s">
         <v>19</v>
       </c>
-      <c r="N1" t="s">
-        <v>31</v>
-      </c>
-      <c r="O1" t="s">
-        <v>25</v>
-      </c>
-      <c r="P1" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>26</v>
-      </c>
-      <c r="R1" t="s">
-        <v>27</v>
-      </c>
-      <c r="S1" t="s">
-        <v>28</v>
-      </c>
-      <c r="T1" t="s">
-        <v>29</v>
-      </c>
-      <c r="U1" t="s">
-        <v>20</v>
-      </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21">
       <c r="A2" t="str">
         <f>B2</f>
         <v>HUME</v>
@@ -548,7 +538,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -560,19 +550,19 @@
         <v>3</v>
       </c>
       <c r="M2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21">
       <c r="A3" t="str">
-        <f t="shared" ref="A3:A5" si="0">B3</f>
+        <f t="shared" ref="A3:A4" si="0">B3</f>
         <v>MONS</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -587,7 +577,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21">
       <c r="A4" t="str">
         <f t="shared" si="0"/>
         <v>Goblin</v>
@@ -596,25 +586,10 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A5" t="str">
-        <f t="shared" si="0"/>
-        <v>Jaguar</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -628,75 +603,75 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
         <v>12</v>
       </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>13</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>14</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>15</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>16</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>17</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>18</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O1" t="s">
         <v>19</v>
       </c>
-      <c r="N1" t="s">
-        <v>23</v>
-      </c>
-      <c r="O1" t="s">
-        <v>20</v>
-      </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15">
       <c r="A2" t="str">
         <f>B2</f>
         <v>MUTE</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -705,16 +680,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15">
       <c r="A3" t="str">
         <f>B3</f>
         <v>Spider</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D3">
         <v>1</v>

</xml_diff>

<commit_message>
Added Group attack capability (mana only)
</commit_message>
<xml_diff>
--- a/Battle Log.xlsx
+++ b/Battle Log.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="24915" windowHeight="12840" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="24915" windowHeight="12840" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Battle 1" sheetId="1" r:id="rId1"/>
     <sheet name="Battle 2" sheetId="3" r:id="rId2"/>
     <sheet name="Battle 3" sheetId="7" r:id="rId3"/>
+    <sheet name="Battle 4" sheetId="9" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="35">
   <si>
     <t>NAME</t>
   </si>
@@ -115,6 +116,12 @@
   </si>
   <si>
     <t>Rapier</t>
+  </si>
+  <si>
+    <t>Zappo</t>
+  </si>
+  <si>
+    <t>Fire</t>
   </si>
 </sst>
 </file>
@@ -457,7 +464,7 @@
   <dimension ref="A1:U4"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -739,7 +746,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
@@ -859,4 +866,132 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:U3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>23</v>
+      </c>
+      <c r="R1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S1" t="s">
+        <v>25</v>
+      </c>
+      <c r="T1" t="s">
+        <v>26</v>
+      </c>
+      <c r="U1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21">
+      <c r="A2" t="str">
+        <f>B2</f>
+        <v>Zappo</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="L2" t="s">
+        <v>34</v>
+      </c>
+      <c r="M2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21">
+      <c r="A3" t="str">
+        <f>B3</f>
+        <v>Goblin</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Basic All Enemies working
</commit_message>
<xml_diff>
--- a/Battle Log.xlsx
+++ b/Battle Log.xlsx
@@ -4,20 +4,22 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="24915" windowHeight="12840" activeTab="3"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="24915" windowHeight="12840" activeTab="5"/>
   </bookViews>
   <sheets>
-    <sheet name="Battle 1" sheetId="1" r:id="rId1"/>
-    <sheet name="Battle 2" sheetId="3" r:id="rId2"/>
-    <sheet name="Battle 3" sheetId="7" r:id="rId3"/>
-    <sheet name="Battle 4" sheetId="9" r:id="rId4"/>
+    <sheet name="Single STR" sheetId="1" r:id="rId1"/>
+    <sheet name="Single AGL" sheetId="3" r:id="rId2"/>
+    <sheet name="Shield" sheetId="7" r:id="rId3"/>
+    <sheet name="Group MANA - PC" sheetId="9" r:id="rId4"/>
+    <sheet name="Group MANA - Enemy" sheetId="11" r:id="rId5"/>
+    <sheet name="All Enemies - PC" sheetId="13" r:id="rId6"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="40">
   <si>
     <t>NAME</t>
   </si>
@@ -122,6 +124,21 @@
   </si>
   <si>
     <t>Fire</t>
+  </si>
+  <si>
+    <t>ROBO</t>
+  </si>
+  <si>
+    <t>Jerk</t>
+  </si>
+  <si>
+    <t>ColtGun</t>
+  </si>
+  <si>
+    <t>Flammie</t>
+  </si>
+  <si>
+    <t>Flame</t>
   </si>
 </sst>
 </file>
@@ -872,7 +889,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
@@ -994,4 +1011,359 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:U6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>23</v>
+      </c>
+      <c r="R1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S1" t="s">
+        <v>25</v>
+      </c>
+      <c r="T1" t="s">
+        <v>26</v>
+      </c>
+      <c r="U1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21">
+      <c r="A2" t="str">
+        <f>B2</f>
+        <v>HUME</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="L2" t="s">
+        <v>3</v>
+      </c>
+      <c r="M2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21">
+      <c r="A3" t="str">
+        <f>B3</f>
+        <v>MUTE</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="L3" t="s">
+        <v>32</v>
+      </c>
+      <c r="M3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21">
+      <c r="A4" t="str">
+        <f t="shared" ref="A4:A6" si="0">B4</f>
+        <v>MONS</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="L4" t="s">
+        <v>4</v>
+      </c>
+      <c r="M4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21">
+      <c r="A5" t="str">
+        <f t="shared" si="0"/>
+        <v>ROBO</v>
+      </c>
+      <c r="B5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="L5" t="s">
+        <v>37</v>
+      </c>
+      <c r="M5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21">
+      <c r="A6" t="str">
+        <f t="shared" si="0"/>
+        <v>Jerk</v>
+      </c>
+      <c r="B6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:U5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>23</v>
+      </c>
+      <c r="R1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S1" t="s">
+        <v>25</v>
+      </c>
+      <c r="T1" t="s">
+        <v>26</v>
+      </c>
+      <c r="U1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21">
+      <c r="A2" t="str">
+        <f>B2</f>
+        <v>Flammie</v>
+      </c>
+      <c r="B2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="L2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21">
+      <c r="A3" t="str">
+        <f>B3</f>
+        <v>Goblin</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21">
+      <c r="A4" t="str">
+        <f t="shared" ref="A4:A6" si="0">B4</f>
+        <v>Jaguar</v>
+      </c>
+      <c r="B4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21">
+      <c r="A5" t="str">
+        <f t="shared" si="0"/>
+        <v>Eagle</v>
+      </c>
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Revised combat,py to use command class
</commit_message>
<xml_diff>
--- a/Battle Log.xlsx
+++ b/Battle Log.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="24915" windowHeight="12840" activeTab="5"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="24915" windowHeight="12840" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Single STR" sheetId="1" r:id="rId1"/>
@@ -13,13 +13,14 @@
     <sheet name="Group MANA - PC" sheetId="9" r:id="rId4"/>
     <sheet name="Group MANA - Enemy" sheetId="11" r:id="rId5"/>
     <sheet name="All Enemies - PC" sheetId="13" r:id="rId6"/>
+    <sheet name="Static DMG" sheetId="14" r:id="rId7"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="40">
   <si>
     <t>NAME</t>
   </si>
@@ -132,13 +133,13 @@
     <t>Jerk</t>
   </si>
   <si>
-    <t>ColtGun</t>
-  </si>
-  <si>
     <t>Flammie</t>
   </si>
   <si>
     <t>Flame</t>
+  </si>
+  <si>
+    <t>Colt</t>
   </si>
 </sst>
 </file>
@@ -1018,7 +1019,7 @@
   <dimension ref="A1:U6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1187,7 +1188,7 @@
         <v>4</v>
       </c>
       <c r="L5" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="M5" t="s">
         <v>36</v>
@@ -1217,7 +1218,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:U5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -1303,7 +1304,7 @@
         <v>Flammie</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
         <v>19</v>
@@ -1315,7 +1316,7 @@
         <v>1</v>
       </c>
       <c r="L2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:21">
@@ -1335,7 +1336,7 @@
     </row>
     <row r="4" spans="1:21">
       <c r="A4" t="str">
-        <f t="shared" ref="A4:A6" si="0">B4</f>
+        <f t="shared" ref="A4:A5" si="0">B4</f>
         <v>Jaguar</v>
       </c>
       <c r="B4" t="s">
@@ -1366,4 +1367,133 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:U3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="4" max="5" width="11.7109375" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>23</v>
+      </c>
+      <c r="R1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S1" t="s">
+        <v>25</v>
+      </c>
+      <c r="T1" t="s">
+        <v>26</v>
+      </c>
+      <c r="U1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21">
+      <c r="A2" t="str">
+        <f>B2</f>
+        <v>ROBO</v>
+      </c>
+      <c r="B2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="L2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21">
+      <c r="A3" t="str">
+        <f t="shared" ref="A3" si="0">B3</f>
+        <v>Goblin</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added stubs for other targets. DB cleanup
</commit_message>
<xml_diff>
--- a/Battle Log.xlsx
+++ b/Battle Log.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="24915" windowHeight="12840" activeTab="6"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="24915" windowHeight="12840" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Single STR" sheetId="1" r:id="rId1"/>
@@ -14,13 +14,14 @@
     <sheet name="Group MANA - Enemy" sheetId="11" r:id="rId5"/>
     <sheet name="All Enemies - PC" sheetId="13" r:id="rId6"/>
     <sheet name="Static DMG" sheetId="14" r:id="rId7"/>
+    <sheet name="Group Static" sheetId="15" r:id="rId8"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="41">
   <si>
     <t>NAME</t>
   </si>
@@ -140,6 +141,9 @@
   </si>
   <si>
     <t>Colt</t>
+  </si>
+  <si>
+    <t>SMG</t>
   </si>
 </sst>
 </file>
@@ -1373,7 +1377,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
@@ -1496,4 +1500,132 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:U3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>23</v>
+      </c>
+      <c r="R1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S1" t="s">
+        <v>25</v>
+      </c>
+      <c r="T1" t="s">
+        <v>26</v>
+      </c>
+      <c r="U1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21">
+      <c r="A2" t="str">
+        <f>B2</f>
+        <v>ROBO</v>
+      </c>
+      <c r="B2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="L2" t="s">
+        <v>40</v>
+      </c>
+      <c r="M2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21">
+      <c r="A3" t="str">
+        <f>B3</f>
+        <v>Goblin</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added Self effects and more Ally effects
</commit_message>
<xml_diff>
--- a/Battle Log.xlsx
+++ b/Battle Log.xlsx
@@ -1,27 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21029"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Action IV\Documents\GitHub\pillar\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{438CE05C-2FF6-4E67-BCEA-217481883518}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="24915" windowHeight="12840" activeTab="7"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="24915" windowHeight="12840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Single STR" sheetId="1" r:id="rId1"/>
-    <sheet name="Single AGL" sheetId="3" r:id="rId2"/>
-    <sheet name="Shield" sheetId="7" r:id="rId3"/>
-    <sheet name="Group MANA - PC" sheetId="9" r:id="rId4"/>
-    <sheet name="Group MANA - Enemy" sheetId="11" r:id="rId5"/>
-    <sheet name="All Enemies - PC" sheetId="13" r:id="rId6"/>
-    <sheet name="Static DMG" sheetId="14" r:id="rId7"/>
-    <sheet name="Group Static" sheetId="15" r:id="rId8"/>
+    <sheet name="Players" sheetId="16" r:id="rId1"/>
+    <sheet name="Single STR" sheetId="1" r:id="rId2"/>
+    <sheet name="Single AGL" sheetId="3" r:id="rId3"/>
+    <sheet name="Shield" sheetId="7" r:id="rId4"/>
+    <sheet name="Group MANA - PC" sheetId="9" r:id="rId5"/>
+    <sheet name="Group MANA - Enemy" sheetId="11" r:id="rId6"/>
+    <sheet name="All Enemies - PC" sheetId="13" r:id="rId7"/>
+    <sheet name="Static DMG" sheetId="14" r:id="rId8"/>
+    <sheet name="Group Static" sheetId="15" r:id="rId9"/>
+    <sheet name="PC Cure - Magic" sheetId="17" r:id="rId10"/>
+    <sheet name="PC Cure - Item" sheetId="18" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="67">
   <si>
     <t>NAME</t>
   </si>
@@ -32,9 +41,6 @@
     <t>MONS</t>
   </si>
   <si>
-    <t>LongSword</t>
-  </si>
-  <si>
     <t>Nail</t>
   </si>
   <si>
@@ -116,9 +122,6 @@
     <t>Jaguar</t>
   </si>
   <si>
-    <t>DragonShield</t>
-  </si>
-  <si>
     <t>Rapier</t>
   </si>
   <si>
@@ -143,19 +146,124 @@
     <t>Colt</t>
   </si>
   <si>
-    <t>SMG</t>
+    <t>BabyD</t>
+  </si>
+  <si>
+    <t>Mutant</t>
+  </si>
+  <si>
+    <t>Robot</t>
+  </si>
+  <si>
+    <t>Human</t>
+  </si>
+  <si>
+    <t>S7</t>
+  </si>
+  <si>
+    <t>S6</t>
+  </si>
+  <si>
+    <t>S5</t>
+  </si>
+  <si>
+    <t>S4</t>
+  </si>
+  <si>
+    <t>S3</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>S0</t>
+  </si>
+  <si>
+    <t>MANA</t>
+  </si>
+  <si>
+    <t>AGL</t>
+  </si>
+  <si>
+    <t>DEF</t>
+  </si>
+  <si>
+    <t>STR</t>
+  </si>
+  <si>
+    <t>HP</t>
+  </si>
+  <si>
+    <t>TYPE</t>
+  </si>
+  <si>
+    <t>CLASS</t>
+  </si>
+  <si>
+    <t>PLAYER</t>
+  </si>
+  <si>
+    <t>CHARACTER</t>
+  </si>
+  <si>
+    <t>Long Sword</t>
+  </si>
+  <si>
+    <t>Bronze Armor</t>
+  </si>
+  <si>
+    <t>Dragon Shield</t>
+  </si>
+  <si>
+    <t>Gold Armor</t>
+  </si>
+  <si>
+    <t>SMG Gun</t>
+  </si>
+  <si>
+    <t>Colt Gun</t>
+  </si>
+  <si>
+    <t>Cure</t>
+  </si>
+  <si>
+    <t>Cure Potion</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -175,14 +283,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{9DABA29D-F777-47A0-A48E-1316C9ED2915}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -240,7 +353,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -272,9 +385,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -306,6 +437,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -481,15 +630,641 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D5ADEB8-F7B1-46C0-9957-CEA833A44FA7}">
+  <dimension ref="A1:R7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="10" width="9.140625" style="1"/>
+    <col min="11" max="11" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" style="1"/>
+    <col min="15" max="15" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="str">
+        <f t="shared" ref="A2:A7" si="0">B2</f>
+        <v>HUME</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" s="1">
+        <f t="shared" ref="E2:E7" si="1">IF(D2="Human",0,IF(D2="Mutant",1,IF(D2="Robot",3,2)))</f>
+        <v>0</v>
+      </c>
+      <c r="F2" s="1">
+        <v>59</v>
+      </c>
+      <c r="G2" s="1">
+        <v>6</v>
+      </c>
+      <c r="H2" s="1">
+        <v>3</v>
+      </c>
+      <c r="I2" s="1">
+        <v>5</v>
+      </c>
+      <c r="J2" s="1">
+        <v>3</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>MUTE</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F3" s="1">
+        <v>45</v>
+      </c>
+      <c r="G3" s="1">
+        <v>4</v>
+      </c>
+      <c r="H3" s="1">
+        <v>10</v>
+      </c>
+      <c r="I3" s="1">
+        <v>5</v>
+      </c>
+      <c r="J3" s="1">
+        <v>6</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>MONS</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="1">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="F4" s="1">
+        <v>45</v>
+      </c>
+      <c r="G4" s="1">
+        <v>5</v>
+      </c>
+      <c r="H4" s="1">
+        <v>5</v>
+      </c>
+      <c r="I4" s="1">
+        <v>2</v>
+      </c>
+      <c r="J4" s="1">
+        <v>6</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>ROBO</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="1">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="F5" s="1">
+        <v>60</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0</v>
+      </c>
+      <c r="H5" s="1">
+        <v>6</v>
+      </c>
+      <c r="I5" s="1">
+        <v>5</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M5" s="3"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Zappo</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F6" s="1">
+        <v>200</v>
+      </c>
+      <c r="G6" s="1">
+        <v>4</v>
+      </c>
+      <c r="H6" s="1">
+        <v>99</v>
+      </c>
+      <c r="I6" s="1">
+        <v>5</v>
+      </c>
+      <c r="J6" s="1">
+        <v>6</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Flammie</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="1">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="F7" s="1">
+        <v>999</v>
+      </c>
+      <c r="G7" s="1">
+        <v>2</v>
+      </c>
+      <c r="H7" s="1">
+        <v>99</v>
+      </c>
+      <c r="I7" s="1">
+        <v>50</v>
+      </c>
+      <c r="J7" s="1">
+        <v>10</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1006FC48-2C9E-47D4-B181-3EF632118273}">
+  <dimension ref="A1:U4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" t="s">
+        <v>27</v>
+      </c>
+      <c r="O1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R1" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1" t="s">
+        <v>24</v>
+      </c>
+      <c r="T1" t="s">
+        <v>25</v>
+      </c>
+      <c r="U1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A2" t="str">
+        <f>B2</f>
+        <v>Zappo</v>
+      </c>
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="L2" t="s">
+        <v>65</v>
+      </c>
+      <c r="M2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A3" t="str">
+        <f>B3</f>
+        <v>Flammie</v>
+      </c>
+      <c r="B3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="G3">
+        <v>900</v>
+      </c>
+      <c r="L3" t="s">
+        <v>3</v>
+      </c>
+      <c r="M3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A4" t="str">
+        <f>B4</f>
+        <v>Goblin</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{867063E5-FD23-4605-BAE9-258F8B0EFA4D}">
+  <dimension ref="A1:U4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" t="s">
+        <v>27</v>
+      </c>
+      <c r="O1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R1" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1" t="s">
+        <v>24</v>
+      </c>
+      <c r="T1" t="s">
+        <v>25</v>
+      </c>
+      <c r="U1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A2" t="str">
+        <f>B2</f>
+        <v>Zappo</v>
+      </c>
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>150</v>
+      </c>
+      <c r="L2" t="s">
+        <v>30</v>
+      </c>
+      <c r="M2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A3" t="str">
+        <f>B3</f>
+        <v>Flammie</v>
+      </c>
+      <c r="B3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="L3" t="s">
+        <v>66</v>
+      </c>
+      <c r="M3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A4" t="str">
+        <f>B4</f>
+        <v>Goblin</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:U4"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="5" width="11.7109375" customWidth="1"/>
     <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
@@ -501,72 +1276,72 @@
     <col min="21" max="21" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
         <v>10</v>
       </c>
-      <c r="E1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>11</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>12</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>13</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>14</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>15</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>16</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
+        <v>27</v>
+      </c>
+      <c r="O1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R1" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1" t="s">
+        <v>24</v>
+      </c>
+      <c r="T1" t="s">
+        <v>25</v>
+      </c>
+      <c r="U1" t="s">
         <v>17</v>
       </c>
-      <c r="N1" t="s">
-        <v>28</v>
-      </c>
-      <c r="O1" t="s">
-        <v>22</v>
-      </c>
-      <c r="P1" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>23</v>
-      </c>
-      <c r="R1" t="s">
-        <v>24</v>
-      </c>
-      <c r="S1" t="s">
-        <v>25</v>
-      </c>
-      <c r="T1" t="s">
-        <v>26</v>
-      </c>
-      <c r="U1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21">
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" t="str">
         <f>B2</f>
         <v>HUME</v>
@@ -575,7 +1350,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -584,13 +1359,13 @@
         <v>2</v>
       </c>
       <c r="L2" t="s">
-        <v>3</v>
+        <v>59</v>
       </c>
       <c r="M2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
         <f t="shared" ref="A3:A4" si="0">B3</f>
         <v>MONS</v>
@@ -599,7 +1374,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -608,22 +1383,22 @@
         <v>1</v>
       </c>
       <c r="L3" t="s">
+        <v>3</v>
+      </c>
+      <c r="M3" t="s">
         <v>4</v>
       </c>
-      <c r="M3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21">
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" t="str">
         <f t="shared" si="0"/>
         <v>Goblin</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -634,8 +1409,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:U3"/>
   <sheetViews>
@@ -643,7 +1418,7 @@
       <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
@@ -654,81 +1429,81 @@
     <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
         <v>10</v>
       </c>
-      <c r="E1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>11</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>12</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>13</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>14</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>15</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>16</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
+        <v>27</v>
+      </c>
+      <c r="O1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R1" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1" t="s">
+        <v>24</v>
+      </c>
+      <c r="T1" t="s">
+        <v>25</v>
+      </c>
+      <c r="U1" t="s">
         <v>17</v>
       </c>
-      <c r="N1" t="s">
-        <v>28</v>
-      </c>
-      <c r="O1" t="s">
-        <v>22</v>
-      </c>
-      <c r="P1" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>23</v>
-      </c>
-      <c r="R1" t="s">
-        <v>24</v>
-      </c>
-      <c r="S1" t="s">
-        <v>25</v>
-      </c>
-      <c r="T1" t="s">
-        <v>26</v>
-      </c>
-      <c r="U1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21">
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" t="str">
         <f>B2</f>
         <v>MUTE</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -737,22 +1512,22 @@
         <v>1</v>
       </c>
       <c r="L2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="M2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
         <f>B3</f>
         <v>Eagle</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -763,16 +1538,16 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="5" width="11.7109375" customWidth="1"/>
     <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
@@ -784,72 +1559,72 @@
     <col min="21" max="21" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
         <v>10</v>
       </c>
-      <c r="E1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>11</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>12</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>13</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>14</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>15</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>16</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
+        <v>27</v>
+      </c>
+      <c r="O1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R1" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1" t="s">
+        <v>24</v>
+      </c>
+      <c r="T1" t="s">
+        <v>25</v>
+      </c>
+      <c r="U1" t="s">
         <v>17</v>
       </c>
-      <c r="N1" t="s">
-        <v>28</v>
-      </c>
-      <c r="O1" t="s">
-        <v>22</v>
-      </c>
-      <c r="P1" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>23</v>
-      </c>
-      <c r="R1" t="s">
-        <v>24</v>
-      </c>
-      <c r="S1" t="s">
-        <v>25</v>
-      </c>
-      <c r="T1" t="s">
-        <v>26</v>
-      </c>
-      <c r="U1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21">
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" t="str">
         <f>B2</f>
         <v>HUME</v>
@@ -858,7 +1633,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -867,19 +1642,19 @@
         <v>1</v>
       </c>
       <c r="L2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
         <f t="shared" ref="A3" si="0">B3</f>
         <v>Jaguar</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -890,15 +1665,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
@@ -909,81 +1684,81 @@
     <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
         <v>10</v>
       </c>
-      <c r="E1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>11</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>12</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>13</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>14</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>15</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>16</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
+        <v>27</v>
+      </c>
+      <c r="O1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R1" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1" t="s">
+        <v>24</v>
+      </c>
+      <c r="T1" t="s">
+        <v>25</v>
+      </c>
+      <c r="U1" t="s">
         <v>17</v>
       </c>
-      <c r="N1" t="s">
-        <v>28</v>
-      </c>
-      <c r="O1" t="s">
-        <v>22</v>
-      </c>
-      <c r="P1" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>23</v>
-      </c>
-      <c r="R1" t="s">
-        <v>24</v>
-      </c>
-      <c r="S1" t="s">
-        <v>25</v>
-      </c>
-      <c r="T1" t="s">
-        <v>26</v>
-      </c>
-      <c r="U1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21">
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" t="str">
         <f>B2</f>
         <v>Zappo</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -992,22 +1767,22 @@
         <v>1</v>
       </c>
       <c r="L2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="M2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
         <f>B3</f>
         <v>Goblin</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D3">
         <v>8</v>
@@ -1018,15 +1793,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:U6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
@@ -1037,72 +1812,72 @@
     <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
         <v>10</v>
       </c>
-      <c r="E1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>11</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>12</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>13</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>14</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>15</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>16</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
+        <v>27</v>
+      </c>
+      <c r="O1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R1" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1" t="s">
+        <v>24</v>
+      </c>
+      <c r="T1" t="s">
+        <v>25</v>
+      </c>
+      <c r="U1" t="s">
         <v>17</v>
       </c>
-      <c r="N1" t="s">
-        <v>28</v>
-      </c>
-      <c r="O1" t="s">
-        <v>22</v>
-      </c>
-      <c r="P1" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>23</v>
-      </c>
-      <c r="R1" t="s">
-        <v>24</v>
-      </c>
-      <c r="S1" t="s">
-        <v>25</v>
-      </c>
-      <c r="T1" t="s">
-        <v>26</v>
-      </c>
-      <c r="U1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21">
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" t="str">
         <f>B2</f>
         <v>HUME</v>
@@ -1111,7 +1886,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1120,22 +1895,22 @@
         <v>1</v>
       </c>
       <c r="L2" t="s">
-        <v>3</v>
+        <v>59</v>
       </c>
       <c r="M2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
         <f>B3</f>
         <v>MUTE</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -1144,13 +1919,13 @@
         <v>2</v>
       </c>
       <c r="L3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="M3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" t="str">
         <f t="shared" ref="A4:A6" si="0">B4</f>
         <v>MONS</v>
@@ -1159,7 +1934,7 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -1168,22 +1943,22 @@
         <v>3</v>
       </c>
       <c r="L4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" t="str">
         <f t="shared" si="0"/>
         <v>ROBO</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -1192,22 +1967,22 @@
         <v>4</v>
       </c>
       <c r="L5" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="M5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" t="str">
         <f t="shared" si="0"/>
         <v>Jerk</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -1218,15 +1993,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:U5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
@@ -1237,81 +2012,81 @@
     <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
         <v>10</v>
       </c>
-      <c r="E1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>11</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>12</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>13</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>14</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>15</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>16</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
+        <v>27</v>
+      </c>
+      <c r="O1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R1" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1" t="s">
+        <v>24</v>
+      </c>
+      <c r="T1" t="s">
+        <v>25</v>
+      </c>
+      <c r="U1" t="s">
         <v>17</v>
       </c>
-      <c r="N1" t="s">
-        <v>28</v>
-      </c>
-      <c r="O1" t="s">
-        <v>22</v>
-      </c>
-      <c r="P1" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>23</v>
-      </c>
-      <c r="R1" t="s">
-        <v>24</v>
-      </c>
-      <c r="S1" t="s">
-        <v>25</v>
-      </c>
-      <c r="T1" t="s">
-        <v>26</v>
-      </c>
-      <c r="U1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21">
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" t="str">
         <f>B2</f>
         <v>Flammie</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1320,49 +2095,49 @@
         <v>1</v>
       </c>
       <c r="L2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
         <f>B3</f>
         <v>Goblin</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D3">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" t="str">
         <f t="shared" ref="A4:A5" si="0">B4</f>
         <v>Jaguar</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D4">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" t="str">
         <f t="shared" si="0"/>
         <v>Eagle</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D5">
         <v>4</v>
@@ -1373,15 +2148,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="5" width="11.7109375" customWidth="1"/>
     <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
@@ -1393,81 +2168,81 @@
     <col min="21" max="21" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
         <v>10</v>
       </c>
-      <c r="E1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>11</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>12</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>13</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>14</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>15</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>16</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
+        <v>27</v>
+      </c>
+      <c r="O1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R1" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1" t="s">
+        <v>24</v>
+      </c>
+      <c r="T1" t="s">
+        <v>25</v>
+      </c>
+      <c r="U1" t="s">
         <v>17</v>
       </c>
-      <c r="N1" t="s">
-        <v>28</v>
-      </c>
-      <c r="O1" t="s">
-        <v>22</v>
-      </c>
-      <c r="P1" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>23</v>
-      </c>
-      <c r="R1" t="s">
-        <v>24</v>
-      </c>
-      <c r="S1" t="s">
-        <v>25</v>
-      </c>
-      <c r="T1" t="s">
-        <v>26</v>
-      </c>
-      <c r="U1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21">
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" t="str">
         <f>B2</f>
         <v>ROBO</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1476,22 +2251,22 @@
         <v>1</v>
       </c>
       <c r="L2" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="M2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
         <f t="shared" ref="A3" si="0">B3</f>
         <v>Goblin</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -1502,15 +2277,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
@@ -1521,81 +2296,81 @@
     <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
         <v>10</v>
       </c>
-      <c r="E1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>11</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>12</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>13</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>14</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>15</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>16</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
+        <v>27</v>
+      </c>
+      <c r="O1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R1" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1" t="s">
+        <v>24</v>
+      </c>
+      <c r="T1" t="s">
+        <v>25</v>
+      </c>
+      <c r="U1" t="s">
         <v>17</v>
       </c>
-      <c r="N1" t="s">
-        <v>28</v>
-      </c>
-      <c r="O1" t="s">
-        <v>22</v>
-      </c>
-      <c r="P1" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>23</v>
-      </c>
-      <c r="R1" t="s">
-        <v>24</v>
-      </c>
-      <c r="S1" t="s">
-        <v>25</v>
-      </c>
-      <c r="T1" t="s">
-        <v>26</v>
-      </c>
-      <c r="U1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21">
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" t="str">
         <f>B2</f>
         <v>ROBO</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1604,22 +2379,22 @@
         <v>1</v>
       </c>
       <c r="L2" t="s">
-        <v>40</v>
+        <v>63</v>
       </c>
       <c r="M2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
         <f>B3</f>
         <v>Goblin</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D3">
         <v>8</v>

</xml_diff>

<commit_message>
"Allies" effects now working
Including group heals and buffs
</commit_message>
<xml_diff>
--- a/Battle Log.xlsx
+++ b/Battle Log.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Action IV\Documents\GitHub\pillar\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scrummel\source\repos\pillar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{438CE05C-2FF6-4E67-BCEA-217481883518}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="24915" windowHeight="12840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="24915" windowHeight="12840" tabRatio="838" firstSheet="2" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Players" sheetId="16" r:id="rId1"/>
@@ -24,13 +23,14 @@
     <sheet name="Group Static" sheetId="15" r:id="rId9"/>
     <sheet name="PC Cure - Magic" sheetId="17" r:id="rId10"/>
     <sheet name="PC Cure - Item" sheetId="18" r:id="rId11"/>
+    <sheet name="PC All Heal" sheetId="19" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="69">
   <si>
     <t>NAME</t>
   </si>
@@ -231,12 +231,18 @@
   </si>
   <si>
     <t>Cure Potion</t>
+  </si>
+  <si>
+    <t>Asleep</t>
+  </si>
+  <si>
+    <t>Heal Staff</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -295,7 +301,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{9DABA29D-F777-47A0-A48E-1316C9ED2915}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -386,23 +392,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -438,23 +427,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -630,11 +602,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D5ADEB8-F7B1-46C0-9957-CEA833A44FA7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -899,6 +871,9 @@
       <c r="M6" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="N6" s="3" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="str">
@@ -946,11 +921,11 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1006FC48-2C9E-47D4-B181-3EF632118273}">
-  <dimension ref="A1:U4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="R1" sqref="R1:R1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -964,7 +939,7 @@
     <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -1017,19 +992,22 @@
         <v>22</v>
       </c>
       <c r="R1" t="s">
+        <v>67</v>
+      </c>
+      <c r="S1" t="s">
         <v>23</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>24</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>25</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" t="str">
         <f>B2</f>
         <v>Zappo</v>
@@ -1053,7 +1031,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
         <f>B3</f>
         <v>Flammie</v>
@@ -1080,7 +1058,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4" t="str">
         <f>B4</f>
         <v>Goblin</v>
@@ -1101,11 +1079,11 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{867063E5-FD23-4605-BAE9-258F8B0EFA4D}">
-  <dimension ref="A1:U4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1119,7 +1097,7 @@
     <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -1172,19 +1150,22 @@
         <v>22</v>
       </c>
       <c r="R1" t="s">
+        <v>67</v>
+      </c>
+      <c r="S1" t="s">
         <v>23</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>24</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>25</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" t="str">
         <f>B2</f>
         <v>Zappo</v>
@@ -1211,7 +1192,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
         <f>B3</f>
         <v>Flammie</v>
@@ -1235,7 +1216,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4" t="str">
         <f>B4</f>
         <v>Goblin</v>
@@ -1255,13 +1236,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:U4"/>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V4"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1273,10 +1253,10 @@
     <col min="10" max="10" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -1329,19 +1309,22 @@
         <v>22</v>
       </c>
       <c r="R1" t="s">
+        <v>67</v>
+      </c>
+      <c r="S1" t="s">
         <v>23</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>24</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>25</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" t="str">
         <f>B2</f>
         <v>HUME</v>
@@ -1356,6 +1339,163 @@
         <v>1</v>
       </c>
       <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>30</v>
+      </c>
+      <c r="L2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A3" t="str">
+        <f t="shared" ref="A3:A4" si="0">B3</f>
+        <v>Jaguar</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A4" t="str">
+        <f t="shared" si="0"/>
+        <v>Zappo</v>
+      </c>
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>100</v>
+      </c>
+      <c r="L4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:V4"/>
+  <sheetViews>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="R1" sqref="R1:R1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="5" width="11.7109375" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" t="s">
+        <v>27</v>
+      </c>
+      <c r="O1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R1" t="s">
+        <v>67</v>
+      </c>
+      <c r="S1" t="s">
+        <v>23</v>
+      </c>
+      <c r="T1" t="s">
+        <v>24</v>
+      </c>
+      <c r="U1" t="s">
+        <v>25</v>
+      </c>
+      <c r="V1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A2" t="str">
+        <f>B2</f>
+        <v>HUME</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
         <v>2</v>
       </c>
       <c r="L2" t="s">
@@ -1365,7 +1505,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
         <f t="shared" ref="A3:A4" si="0">B3</f>
         <v>MONS</v>
@@ -1389,7 +1529,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4" t="str">
         <f t="shared" si="0"/>
         <v>Goblin</v>
@@ -1410,12 +1550,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:U3"/>
+  <dimension ref="A1:V3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="R1" sqref="R1:R1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1429,7 +1569,7 @@
     <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -1482,19 +1622,22 @@
         <v>22</v>
       </c>
       <c r="R1" t="s">
+        <v>67</v>
+      </c>
+      <c r="S1" t="s">
         <v>23</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>24</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>25</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" t="str">
         <f>B2</f>
         <v>MUTE</v>
@@ -1518,7 +1661,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
         <f>B3</f>
         <v>Eagle</v>
@@ -1539,12 +1682,12 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:U3"/>
+  <dimension ref="A1:V3"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="R1" sqref="R1:R1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1556,10 +1699,10 @@
     <col min="10" max="10" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -1612,19 +1755,22 @@
         <v>22</v>
       </c>
       <c r="R1" t="s">
+        <v>67</v>
+      </c>
+      <c r="S1" t="s">
         <v>23</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>24</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>25</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" t="str">
         <f>B2</f>
         <v>HUME</v>
@@ -1645,7 +1791,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
         <f t="shared" ref="A3" si="0">B3</f>
         <v>Jaguar</v>
@@ -1666,11 +1812,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:U3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="R1" sqref="R1:R1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1684,7 +1830,7 @@
     <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -1737,19 +1883,22 @@
         <v>22</v>
       </c>
       <c r="R1" t="s">
+        <v>67</v>
+      </c>
+      <c r="S1" t="s">
         <v>23</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>24</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>25</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" t="str">
         <f>B2</f>
         <v>Zappo</v>
@@ -1773,7 +1922,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
         <f>B3</f>
         <v>Goblin</v>
@@ -1794,11 +1943,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:U6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="R1" sqref="R1:R1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1812,7 +1961,7 @@
     <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -1865,19 +2014,22 @@
         <v>22</v>
       </c>
       <c r="R1" t="s">
+        <v>67</v>
+      </c>
+      <c r="S1" t="s">
         <v>23</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>24</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>25</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" t="str">
         <f>B2</f>
         <v>HUME</v>
@@ -1901,7 +2053,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
         <f>B3</f>
         <v>MUTE</v>
@@ -1925,7 +2077,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4" t="str">
         <f t="shared" ref="A4:A6" si="0">B4</f>
         <v>MONS</v>
@@ -1949,7 +2101,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5" t="str">
         <f t="shared" si="0"/>
         <v>ROBO</v>
@@ -1973,7 +2125,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A6" t="str">
         <f t="shared" si="0"/>
         <v>Jerk</v>
@@ -1994,11 +2146,11 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:U5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="R1" sqref="R1:R1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2012,7 +2164,7 @@
     <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -2065,19 +2217,22 @@
         <v>22</v>
       </c>
       <c r="R1" t="s">
+        <v>67</v>
+      </c>
+      <c r="S1" t="s">
         <v>23</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>24</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>25</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" t="str">
         <f>B2</f>
         <v>Flammie</v>
@@ -2098,7 +2253,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
         <f>B3</f>
         <v>Goblin</v>
@@ -2113,7 +2268,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4" t="str">
         <f t="shared" ref="A4:A5" si="0">B4</f>
         <v>Jaguar</v>
@@ -2128,7 +2283,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5" t="str">
         <f t="shared" si="0"/>
         <v>Eagle</v>
@@ -2149,11 +2304,11 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:U3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V3"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="R1" sqref="R1:R1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2165,10 +2320,10 @@
     <col min="10" max="10" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -2221,19 +2376,22 @@
         <v>22</v>
       </c>
       <c r="R1" t="s">
+        <v>67</v>
+      </c>
+      <c r="S1" t="s">
         <v>23</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>24</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>25</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" t="str">
         <f>B2</f>
         <v>ROBO</v>
@@ -2257,7 +2415,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
         <f t="shared" ref="A3" si="0">B3</f>
         <v>Goblin</v>
@@ -2278,11 +2436,11 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:U3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="R1" sqref="R1:R1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2296,7 +2454,7 @@
     <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -2349,19 +2507,22 @@
         <v>22</v>
       </c>
       <c r="R1" t="s">
+        <v>67</v>
+      </c>
+      <c r="S1" t="s">
         <v>23</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>24</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>25</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" t="str">
         <f>B2</f>
         <v>ROBO</v>
@@ -2385,7 +2546,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
         <f>B3</f>
         <v>Goblin</v>

</xml_diff>

<commit_message>
Touch-ups on resist code
</commit_message>
<xml_diff>
--- a/Battle Log.xlsx
+++ b/Battle Log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Action IV\Documents\GitHub\pillar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28A3A275-3B4D-42C1-B37B-8EEFC153984D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DFD9898-0B4D-4783-A17D-24B63D35237D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="24915" windowHeight="12840" tabRatio="838" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="24915" windowHeight="12840" tabRatio="838" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Players" sheetId="16" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="70">
   <si>
     <t>NAME</t>
   </si>
@@ -238,18 +238,28 @@
   </si>
   <si>
     <t>O-Ice</t>
+  </si>
+  <si>
+    <t>Dragon Armor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -306,11 +316,12 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -656,8 +667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -927,6 +938,9 @@
       </c>
       <c r="N6" s="3" t="s">
         <v>67</v>
+      </c>
+      <c r="O6" s="6" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -1869,7 +1883,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:V3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="R1" sqref="R1:R1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Working status effects on Single
</commit_message>
<xml_diff>
--- a/Battle Log.xlsx
+++ b/Battle Log.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21126"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scrummel\source\repos\pillar\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Action IV\Documents\GitHub\pillar\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F104E263-C1DA-485B-A149-8A1A53A1399E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="24915" windowHeight="12840" tabRatio="838" activeTab="9"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="24915" windowHeight="12840" tabRatio="838" firstSheet="1" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Players" sheetId="16" r:id="rId1"/>
@@ -25,13 +26,14 @@
     <sheet name="PC Cure - Magic" sheetId="17" r:id="rId11"/>
     <sheet name="PC Cure - Item" sheetId="18" r:id="rId12"/>
     <sheet name="PC All Heal" sheetId="19" r:id="rId13"/>
+    <sheet name="Status Effect" sheetId="21" r:id="rId14"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="73">
   <si>
     <t>NAME</t>
   </si>
@@ -244,12 +246,18 @@
   </si>
   <si>
     <t>Skelton</t>
+  </si>
+  <si>
+    <t>Ghoul</t>
+  </si>
+  <si>
+    <t>ParaNail</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -332,7 +340,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -423,6 +431,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -458,6 +483,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -633,7 +675,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -958,11 +1000,11 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:V3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1089,7 +1131,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:V4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1247,7 +1289,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:V4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1405,7 +1447,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:V4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1560,8 +1602,145 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0E7D7FE-6694-44E8-A7B5-C26EAA80FD43}">
+  <dimension ref="A1:V3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" t="s">
+        <v>27</v>
+      </c>
+      <c r="O1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R1" t="s">
+        <v>66</v>
+      </c>
+      <c r="S1" t="s">
+        <v>23</v>
+      </c>
+      <c r="T1" t="s">
+        <v>24</v>
+      </c>
+      <c r="U1" t="s">
+        <v>25</v>
+      </c>
+      <c r="V1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A2" t="str">
+        <f>B2</f>
+        <v>Zappo</v>
+      </c>
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="L2" t="s">
+        <v>64</v>
+      </c>
+      <c r="M2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A3" t="str">
+        <f>B3</f>
+        <v>Ghoul</v>
+      </c>
+      <c r="B3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="L3" t="s">
+        <v>72</v>
+      </c>
+      <c r="M3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:V4"/>
   <sheetViews>
@@ -1718,7 +1897,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:V3"/>
   <sheetViews>
@@ -1850,7 +2029,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:V3"/>
   <sheetViews>
@@ -1980,7 +2159,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:V3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2111,7 +2290,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:V6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2314,7 +2493,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:V5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2472,7 +2651,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:V3"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
@@ -2604,7 +2783,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:V3"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Group status attacks work
Also fixed AI skill selection and end of turn cleanup.
</commit_message>
<xml_diff>
--- a/Battle Log.xlsx
+++ b/Battle Log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Action IV\Documents\GitHub\pillar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F104E263-C1DA-485B-A149-8A1A53A1399E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B8BE38C-8967-45D4-AE41-BDC01FD15962}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="24915" windowHeight="12840" tabRatio="838" firstSheet="1" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="24915" windowHeight="12840" tabRatio="838" firstSheet="2" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Players" sheetId="16" r:id="rId1"/>
@@ -27,13 +27,14 @@
     <sheet name="PC Cure - Item" sheetId="18" r:id="rId12"/>
     <sheet name="PC All Heal" sheetId="19" r:id="rId13"/>
     <sheet name="Status Effect" sheetId="21" r:id="rId14"/>
+    <sheet name="Group Status" sheetId="22" r:id="rId15"/>
   </sheets>
   <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="73">
   <si>
     <t>NAME</t>
   </si>
@@ -251,7 +252,7 @@
     <t>Ghoul</t>
   </si>
   <si>
-    <t>ParaNail</t>
+    <t>Mushroom</t>
   </si>
 </sst>
 </file>
@@ -1606,8 +1607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0E7D7FE-6694-44E8-A7B5-C26EAA80FD43}">
   <dimension ref="A1:V3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1727,11 +1728,136 @@
       <c r="D3">
         <v>1</v>
       </c>
-      <c r="L3" t="s">
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7EFE904-35AC-40B7-AEAE-FF0587D49733}">
+  <dimension ref="A1:V3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" t="s">
+        <v>27</v>
+      </c>
+      <c r="O1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R1" t="s">
+        <v>66</v>
+      </c>
+      <c r="S1" t="s">
+        <v>23</v>
+      </c>
+      <c r="T1" t="s">
+        <v>24</v>
+      </c>
+      <c r="U1" t="s">
+        <v>25</v>
+      </c>
+      <c r="V1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A2" t="str">
+        <f>B2</f>
+        <v>Zappo</v>
+      </c>
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="L2" t="s">
+        <v>64</v>
+      </c>
+      <c r="M2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A3" t="str">
+        <f>B3</f>
+        <v>Mushroom</v>
+      </c>
+      <c r="B3" t="s">
         <v>72</v>
       </c>
-      <c r="M3" t="s">
-        <v>31</v>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Status code and Group targeting fixes
STON and STUN remove other status effects, prevent targeting, and prevent further damage (need to test STON for sure).
Group and All attacks now assess whether the enemies are still there to be hit.
</commit_message>
<xml_diff>
--- a/Battle Log.xlsx
+++ b/Battle Log.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Action IV\Documents\GitHub\pillar\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scrummel\source\repos\pillar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B8BE38C-8967-45D4-AE41-BDC01FD15962}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="24915" windowHeight="12840" tabRatio="838" firstSheet="2" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="24915" windowHeight="12840" tabRatio="838" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Players" sheetId="16" r:id="rId1"/>
@@ -20,21 +19,22 @@
     <sheet name="Group MANA - PC" sheetId="9" r:id="rId5"/>
     <sheet name="Group MANA - Enemy" sheetId="11" r:id="rId6"/>
     <sheet name="All Enemies - PC" sheetId="13" r:id="rId7"/>
-    <sheet name="Static DMG" sheetId="14" r:id="rId8"/>
-    <sheet name="Group Static" sheetId="15" r:id="rId9"/>
-    <sheet name="O-Weapon" sheetId="20" r:id="rId10"/>
-    <sheet name="PC Cure - Magic" sheetId="17" r:id="rId11"/>
-    <sheet name="PC Cure - Item" sheetId="18" r:id="rId12"/>
-    <sheet name="PC All Heal" sheetId="19" r:id="rId13"/>
-    <sheet name="Status Effect" sheetId="21" r:id="rId14"/>
-    <sheet name="Group Status" sheetId="22" r:id="rId15"/>
+    <sheet name="All Enemies - Dead Test" sheetId="23" r:id="rId8"/>
+    <sheet name="Static DMG" sheetId="14" r:id="rId9"/>
+    <sheet name="Group Static" sheetId="15" r:id="rId10"/>
+    <sheet name="O-Weapon" sheetId="20" r:id="rId11"/>
+    <sheet name="PC Cure - Magic" sheetId="17" r:id="rId12"/>
+    <sheet name="PC Cure - Item" sheetId="18" r:id="rId13"/>
+    <sheet name="PC All Heal" sheetId="19" r:id="rId14"/>
+    <sheet name="Status Effect" sheetId="21" r:id="rId15"/>
+    <sheet name="Group Status" sheetId="22" r:id="rId16"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="74">
   <si>
     <t>NAME</t>
   </si>
@@ -253,12 +253,15 @@
   </si>
   <si>
     <t>Mushroom</t>
+  </si>
+  <si>
+    <t>Asigaru</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -341,7 +344,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -432,23 +435,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -484,23 +470,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -676,7 +645,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1001,7 +970,138 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R1" sqref="R1:R1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" t="s">
+        <v>27</v>
+      </c>
+      <c r="O1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R1" t="s">
+        <v>66</v>
+      </c>
+      <c r="S1" t="s">
+        <v>23</v>
+      </c>
+      <c r="T1" t="s">
+        <v>24</v>
+      </c>
+      <c r="U1" t="s">
+        <v>25</v>
+      </c>
+      <c r="V1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A2" t="str">
+        <f>B2</f>
+        <v>ROBO</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="L2" t="s">
+        <v>62</v>
+      </c>
+      <c r="M2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A3" t="str">
+        <f>B3</f>
+        <v>Goblin</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1131,8 +1231,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1289,8 +1389,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1447,8 +1547,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1603,8 +1703,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0E7D7FE-6694-44E8-A7B5-C26EAA80FD43}">
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1734,11 +1834,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7EFE904-35AC-40B7-AEAE-FF0587D49733}">
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -1866,7 +1966,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:V4"/>
   <sheetViews>
@@ -2023,7 +2123,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:V3"/>
   <sheetViews>
@@ -2155,7 +2255,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:V3"/>
   <sheetViews>
@@ -2285,7 +2385,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2416,7 +2516,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2619,7 +2719,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2777,7 +2877,165 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" t="s">
+        <v>27</v>
+      </c>
+      <c r="O1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R1" t="s">
+        <v>66</v>
+      </c>
+      <c r="S1" t="s">
+        <v>23</v>
+      </c>
+      <c r="T1" t="s">
+        <v>24</v>
+      </c>
+      <c r="U1" t="s">
+        <v>25</v>
+      </c>
+      <c r="V1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A2" t="str">
+        <f>B2</f>
+        <v>Flammie</v>
+      </c>
+      <c r="B2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="L2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A3" t="str">
+        <f>B3</f>
+        <v>Goblin</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A4" t="str">
+        <f t="shared" ref="A4:A5" si="0">B4</f>
+        <v>Jaguar</v>
+      </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A5" t="str">
+        <f t="shared" si="0"/>
+        <v>Asigaru</v>
+      </c>
+      <c r="B5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V3"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
@@ -2906,135 +3164,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:V3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R1" sqref="R1:R1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L1" t="s">
-        <v>15</v>
-      </c>
-      <c r="M1" t="s">
-        <v>16</v>
-      </c>
-      <c r="N1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O1" t="s">
-        <v>21</v>
-      </c>
-      <c r="P1" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>22</v>
-      </c>
-      <c r="R1" t="s">
-        <v>66</v>
-      </c>
-      <c r="S1" t="s">
-        <v>23</v>
-      </c>
-      <c r="T1" t="s">
-        <v>24</v>
-      </c>
-      <c r="U1" t="s">
-        <v>25</v>
-      </c>
-      <c r="V1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A2" t="str">
-        <f>B2</f>
-        <v>ROBO</v>
-      </c>
-      <c r="B2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="L2" t="s">
-        <v>62</v>
-      </c>
-      <c r="M2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A3" t="str">
-        <f>B3</f>
-        <v>Goblin</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Status fixes, print cleanup, more
</commit_message>
<xml_diff>
--- a/Battle Log.xlsx
+++ b/Battle Log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Action IV\Documents\GitHub\pillar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22FDBFD6-80AC-432C-B444-F6AE083773A7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F45A9D9-DB91-41F9-A17C-523F64FF6CA1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="838" firstSheet="8" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="838" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Players" sheetId="16" r:id="rId1"/>
@@ -30,15 +30,16 @@
     <sheet name="PC All Heal" sheetId="19" r:id="rId15"/>
     <sheet name="Status Effect" sheetId="21" r:id="rId16"/>
     <sheet name="Group Status" sheetId="22" r:id="rId17"/>
-    <sheet name="Weak - Elem Melee" sheetId="26" r:id="rId18"/>
-    <sheet name="Weak - Race Melee" sheetId="27" r:id="rId19"/>
+    <sheet name="All Enemies - Status" sheetId="28" r:id="rId18"/>
+    <sheet name="Weak - Elem Melee" sheetId="26" r:id="rId19"/>
+    <sheet name="Weak - Race Melee" sheetId="27" r:id="rId20"/>
   </sheets>
   <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="83">
   <si>
     <t>NAME</t>
   </si>
@@ -151,15 +152,9 @@
     <t>Flame</t>
   </si>
   <si>
-    <t>Mutant</t>
-  </si>
-  <si>
     <t>Robot</t>
   </si>
   <si>
-    <t>Human</t>
-  </si>
-  <si>
     <t>S7</t>
   </si>
   <si>
@@ -199,9 +194,6 @@
     <t>HP</t>
   </si>
   <si>
-    <t>TYPE</t>
-  </si>
-  <si>
     <t>CLASS</t>
   </si>
   <si>
@@ -278,18 +270,50 @@
   </si>
   <si>
     <t>Moth</t>
+  </si>
+  <si>
+    <t>SuperJerk</t>
+  </si>
+  <si>
+    <t>O-Pa/Po</t>
+  </si>
+  <si>
+    <t>Human M</t>
+  </si>
+  <si>
+    <t>Mutant F</t>
+  </si>
+  <si>
+    <t>Mutant M</t>
+  </si>
+  <si>
+    <t>Human F</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -381,11 +405,13 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -734,90 +760,87 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T8"/>
+  <dimension ref="A1:S8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="10" width="9.140625" style="1"/>
-    <col min="11" max="11" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.140625" style="1"/>
-    <col min="15" max="15" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="18" width="9.140625" style="1"/>
-    <col min="19" max="19" width="20.28515625" style="1" customWidth="1"/>
-    <col min="20" max="20" width="23.42578125" style="1" customWidth="1"/>
-    <col min="21" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="9" width="9.140625" style="1"/>
+    <col min="10" max="10" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" style="1"/>
+    <col min="14" max="14" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="17" width="9.140625" style="1"/>
+    <col min="18" max="18" width="20.28515625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="23.42578125" style="1" customWidth="1"/>
+    <col min="20" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
+      </c>
+      <c r="R1" s="9" t="s">
+        <v>73</v>
       </c>
       <c r="S1" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="T1" s="9" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="str">
         <f t="shared" ref="A2:A8" si="0">B2</f>
         <v>HUME</v>
@@ -825,39 +848,35 @@
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>39</v>
+      <c r="D2" s="12" t="s">
+        <v>79</v>
       </c>
       <c r="E2" s="1">
-        <f t="shared" ref="E2:E8" si="1">IF(D2="Human",0,IF(D2="Mutant",1,IF(D2="Robot",3,2)))</f>
-        <v>0</v>
+        <v>59</v>
       </c>
       <c r="F2" s="1">
-        <v>59</v>
+        <v>6</v>
       </c>
       <c r="G2" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H2" s="1">
+        <v>5</v>
+      </c>
+      <c r="I2" s="1">
         <v>3</v>
       </c>
-      <c r="I2" s="1">
-        <v>5</v>
-      </c>
-      <c r="J2" s="1">
-        <v>3</v>
+      <c r="J2" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="str">
         <f t="shared" si="0"/>
         <v>MUTE</v>
@@ -865,39 +884,35 @@
       <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>37</v>
+      <c r="D3" s="12" t="s">
+        <v>80</v>
       </c>
       <c r="E3" s="1">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="F3" s="1">
-        <v>45</v>
+        <v>4</v>
       </c>
       <c r="G3" s="1">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="H3" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I3" s="1">
-        <v>5</v>
-      </c>
-      <c r="J3" s="1">
         <v>6</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>36</v>
       </c>
+      <c r="N3" s="1" t="s">
+        <v>57</v>
+      </c>
       <c r="O3" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="P3" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="str">
         <f t="shared" si="0"/>
         <v>MONS</v>
@@ -906,38 +921,34 @@
         <v>2</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E4" s="1">
-        <f t="shared" si="1"/>
-        <v>2</v>
+        <v>45</v>
       </c>
       <c r="F4" s="1">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="G4" s="1">
         <v>5</v>
       </c>
       <c r="H4" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I4" s="1">
-        <v>2</v>
-      </c>
-      <c r="J4" s="1">
         <v>6</v>
       </c>
+      <c r="J4" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="K4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="L4" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="M4" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="L4" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ROBO</v>
@@ -946,36 +957,34 @@
         <v>33</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E5" s="1">
-        <f t="shared" si="1"/>
-        <v>3</v>
+        <v>60</v>
       </c>
       <c r="F5" s="1">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="G5" s="1">
+        <v>6</v>
+      </c>
+      <c r="H5" s="1">
+        <v>5</v>
+      </c>
+      <c r="I5" s="1">
         <v>0</v>
       </c>
-      <c r="H5" s="1">
-        <v>6</v>
-      </c>
-      <c r="I5" s="1">
-        <v>5</v>
-      </c>
-      <c r="J5" s="1">
-        <v>0</v>
-      </c>
-      <c r="K5" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="M5" s="3"/>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="J5" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="L5" s="11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Zappo</v>
@@ -983,45 +992,41 @@
       <c r="B6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>37</v>
+      <c r="D6" s="12" t="s">
+        <v>81</v>
       </c>
       <c r="E6" s="1">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="F6" s="1">
-        <v>200</v>
+        <v>4</v>
       </c>
       <c r="G6" s="1">
-        <v>4</v>
+        <v>99</v>
       </c>
       <c r="H6" s="1">
-        <v>99</v>
+        <v>5</v>
       </c>
       <c r="I6" s="1">
-        <v>5</v>
-      </c>
-      <c r="J6" s="1">
         <v>6</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="L6" s="2" t="s">
+      <c r="K6" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="M6" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="M6" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="N6" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="O6" s="6" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="N6" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Flammie</v>
@@ -1030,72 +1035,64 @@
         <v>35</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E7" s="1">
-        <f t="shared" si="1"/>
+        <v>999</v>
+      </c>
+      <c r="F7" s="1">
         <v>2</v>
       </c>
-      <c r="F7" s="1">
-        <v>999</v>
-      </c>
       <c r="G7" s="1">
-        <v>2</v>
+        <v>99</v>
       </c>
       <c r="H7" s="1">
-        <v>99</v>
+        <v>50</v>
       </c>
       <c r="I7" s="1">
-        <v>50</v>
-      </c>
-      <c r="J7" s="1">
         <v>10</v>
       </c>
+      <c r="J7" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="K7" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="L7" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="M7" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="L7" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Slashy</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>39</v>
+        <v>71</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>82</v>
       </c>
       <c r="E8" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>400</v>
       </c>
       <c r="F8" s="1">
-        <v>400</v>
+        <v>30</v>
       </c>
       <c r="G8" s="1">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="H8" s="1">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="I8" s="1">
-        <v>25</v>
-      </c>
-      <c r="J8" s="1">
         <v>4</v>
       </c>
-      <c r="K8" s="8" t="s">
+      <c r="J8" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="K8" s="10" t="s">
         <v>75</v>
-      </c>
-      <c r="L8" s="10" t="s">
-        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1176,7 +1173,7 @@
         <v>22</v>
       </c>
       <c r="R1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="S1" t="s">
         <v>23</v>
@@ -1209,7 +1206,7 @@
         <v>1</v>
       </c>
       <c r="L2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="M2" t="s">
         <v>4</v>
@@ -1307,7 +1304,7 @@
         <v>22</v>
       </c>
       <c r="R1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="S1" t="s">
         <v>23</v>
@@ -1340,7 +1337,7 @@
         <v>1</v>
       </c>
       <c r="L2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="M2" t="s">
         <v>4</v>
@@ -1438,7 +1435,7 @@
         <v>22</v>
       </c>
       <c r="R1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="S1" t="s">
         <v>23</v>
@@ -1471,10 +1468,10 @@
         <v>1</v>
       </c>
       <c r="L2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="M2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.2">
@@ -1483,7 +1480,7 @@
         <v>Skelton</v>
       </c>
       <c r="B3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C3" t="s">
         <v>19</v>
@@ -1569,7 +1566,7 @@
         <v>22</v>
       </c>
       <c r="R1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="S1" t="s">
         <v>23</v>
@@ -1602,7 +1599,7 @@
         <v>1</v>
       </c>
       <c r="L2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="M2" t="s">
         <v>35</v>
@@ -1727,7 +1724,7 @@
         <v>22</v>
       </c>
       <c r="R1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="S1" t="s">
         <v>23</v>
@@ -1787,7 +1784,7 @@
         <v>2</v>
       </c>
       <c r="L3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="M3" t="s">
         <v>31</v>
@@ -1886,7 +1883,7 @@
         <v>22</v>
       </c>
       <c r="R1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="S1" t="s">
         <v>23</v>
@@ -1922,7 +1919,7 @@
         <v>30</v>
       </c>
       <c r="L2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.2">
@@ -1961,7 +1958,7 @@
         <v>100</v>
       </c>
       <c r="L4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -2041,7 +2038,7 @@
         <v>22</v>
       </c>
       <c r="R1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="S1" t="s">
         <v>23</v>
@@ -2074,7 +2071,7 @@
         <v>1</v>
       </c>
       <c r="L2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="M2" t="s">
         <v>31</v>
@@ -2086,7 +2083,7 @@
         <v>Ghoul</v>
       </c>
       <c r="B3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C3" t="s">
         <v>19</v>
@@ -2172,7 +2169,7 @@
         <v>22</v>
       </c>
       <c r="R1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="S1" t="s">
         <v>23</v>
@@ -2205,7 +2202,7 @@
         <v>1</v>
       </c>
       <c r="L2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="M2" t="s">
         <v>31</v>
@@ -2217,7 +2214,7 @@
         <v>Mushroom</v>
       </c>
       <c r="B3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C3" t="s">
         <v>19</v>
@@ -2232,6 +2229,209 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE3B29AC-4EE3-4787-96AC-654F35FC0E64}">
+  <dimension ref="A1:V6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" t="s">
+        <v>27</v>
+      </c>
+      <c r="O1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R1" t="s">
+        <v>62</v>
+      </c>
+      <c r="S1" t="s">
+        <v>23</v>
+      </c>
+      <c r="T1" t="s">
+        <v>24</v>
+      </c>
+      <c r="U1" t="s">
+        <v>25</v>
+      </c>
+      <c r="V1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A2" t="str">
+        <f>B2</f>
+        <v>HUME</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="L2" t="s">
+        <v>54</v>
+      </c>
+      <c r="M2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A3" t="str">
+        <f>B3</f>
+        <v>MUTE</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="L3" t="s">
+        <v>30</v>
+      </c>
+      <c r="M3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A4" t="str">
+        <f t="shared" ref="A4:A6" si="0">B4</f>
+        <v>MONS</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="L4" t="s">
+        <v>3</v>
+      </c>
+      <c r="M4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A5" t="str">
+        <f t="shared" si="0"/>
+        <v>ROBO</v>
+      </c>
+      <c r="B5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="L5" t="s">
+        <v>59</v>
+      </c>
+      <c r="M5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A6" t="str">
+        <f t="shared" si="0"/>
+        <v>SuperJerk</v>
+      </c>
+      <c r="B6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{409A1116-4461-47A9-88CD-B9FECC587ADD}">
   <dimension ref="A1:V3"/>
   <sheetViews>
@@ -2303,7 +2503,7 @@
         <v>22</v>
       </c>
       <c r="R1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="S1" t="s">
         <v>23</v>
@@ -2324,7 +2524,7 @@
         <v>Slashy</v>
       </c>
       <c r="B2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C2" t="s">
         <v>18</v>
@@ -2336,10 +2536,10 @@
         <v>1</v>
       </c>
       <c r="L2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="M2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.2">
@@ -2348,7 +2548,7 @@
         <v>Skelton</v>
       </c>
       <c r="B3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C3" t="s">
         <v>19</v>
@@ -2362,11 +2562,168 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:V4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="5" width="11.7109375" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" t="s">
+        <v>27</v>
+      </c>
+      <c r="O1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R1" t="s">
+        <v>62</v>
+      </c>
+      <c r="S1" t="s">
+        <v>23</v>
+      </c>
+      <c r="T1" t="s">
+        <v>24</v>
+      </c>
+      <c r="U1" t="s">
+        <v>25</v>
+      </c>
+      <c r="V1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A2" t="str">
+        <f>B2</f>
+        <v>HUME</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="L2" t="s">
+        <v>54</v>
+      </c>
+      <c r="M2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A3" t="str">
+        <f t="shared" ref="A3:A4" si="0">B3</f>
+        <v>MONS</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="L3" t="s">
+        <v>3</v>
+      </c>
+      <c r="M3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A4" t="str">
+        <f t="shared" si="0"/>
+        <v>Goblin</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06BB4AEA-0818-4141-9E54-A13B42F0DE11}">
   <dimension ref="A1:V3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -2434,7 +2791,7 @@
         <v>22</v>
       </c>
       <c r="R1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="S1" t="s">
         <v>23</v>
@@ -2455,7 +2812,7 @@
         <v>Slashy</v>
       </c>
       <c r="B2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C2" t="s">
         <v>18</v>
@@ -2467,10 +2824,10 @@
         <v>1</v>
       </c>
       <c r="L2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="M2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.2">
@@ -2479,170 +2836,13 @@
         <v>Moth</v>
       </c>
       <c r="B3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C3" t="s">
         <v>19</v>
       </c>
       <c r="D3">
         <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:V4"/>
-  <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="R1" sqref="R1:R1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="4" max="5" width="11.7109375" customWidth="1"/>
-    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="15.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L1" t="s">
-        <v>15</v>
-      </c>
-      <c r="M1" t="s">
-        <v>16</v>
-      </c>
-      <c r="N1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O1" t="s">
-        <v>21</v>
-      </c>
-      <c r="P1" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>22</v>
-      </c>
-      <c r="R1" t="s">
-        <v>65</v>
-      </c>
-      <c r="S1" t="s">
-        <v>23</v>
-      </c>
-      <c r="T1" t="s">
-        <v>24</v>
-      </c>
-      <c r="U1" t="s">
-        <v>25</v>
-      </c>
-      <c r="V1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A2" t="str">
-        <f>B2</f>
-        <v>HUME</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>2</v>
-      </c>
-      <c r="L2" t="s">
-        <v>57</v>
-      </c>
-      <c r="M2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A3" t="str">
-        <f t="shared" ref="A3:A4" si="0">B3</f>
-        <v>MONS</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="L3" t="s">
-        <v>3</v>
-      </c>
-      <c r="M3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A4" t="str">
-        <f t="shared" si="0"/>
-        <v>Goblin</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4">
-        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -2723,7 +2923,7 @@
         <v>22</v>
       </c>
       <c r="R1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="S1" t="s">
         <v>23</v>
@@ -2856,7 +3056,7 @@
         <v>22</v>
       </c>
       <c r="R1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="S1" t="s">
         <v>23</v>
@@ -2889,7 +3089,7 @@
         <v>1</v>
       </c>
       <c r="L2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.2">
@@ -2984,7 +3184,7 @@
         <v>22</v>
       </c>
       <c r="R1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="S1" t="s">
         <v>23</v>
@@ -3115,7 +3315,7 @@
         <v>22</v>
       </c>
       <c r="R1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="S1" t="s">
         <v>23</v>
@@ -3148,7 +3348,7 @@
         <v>1</v>
       </c>
       <c r="L2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="M2" t="s">
         <v>34</v>
@@ -3220,7 +3420,7 @@
         <v>4</v>
       </c>
       <c r="L5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="M5" t="s">
         <v>34</v>
@@ -3318,7 +3518,7 @@
         <v>22</v>
       </c>
       <c r="R1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="S1" t="s">
         <v>23</v>
@@ -3351,7 +3551,7 @@
         <v>1</v>
       </c>
       <c r="L2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.2">
@@ -3420,7 +3620,7 @@
         <v>4</v>
       </c>
       <c r="L5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="M5" t="s">
         <v>34</v>
@@ -3518,7 +3718,7 @@
         <v>22</v>
       </c>
       <c r="R1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="S1" t="s">
         <v>23</v>
@@ -3676,7 +3876,7 @@
         <v>22</v>
       </c>
       <c r="R1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="S1" t="s">
         <v>23</v>
@@ -3748,7 +3948,7 @@
         <v>Asigaru</v>
       </c>
       <c r="B5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C5" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
Confusion works. Major overhauls
</commit_message>
<xml_diff>
--- a/Battle Log.xlsx
+++ b/Battle Log.xlsx
@@ -8,38 +8,39 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Action IV\Documents\GitHub\pillar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F45A9D9-DB91-41F9-A17C-523F64FF6CA1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3158C319-5CF4-4A0C-8CD3-886B6B86A22E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="838" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="838" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Players" sheetId="16" r:id="rId1"/>
     <sheet name="Single STR" sheetId="1" r:id="rId2"/>
-    <sheet name="Single AGL" sheetId="3" r:id="rId3"/>
-    <sheet name="Shield" sheetId="7" r:id="rId4"/>
-    <sheet name="Group MANA - PC" sheetId="9" r:id="rId5"/>
-    <sheet name="Group MANA - Enemy" sheetId="11" r:id="rId6"/>
-    <sheet name="Barrier" sheetId="24" r:id="rId7"/>
-    <sheet name="All Enemies - PC" sheetId="13" r:id="rId8"/>
-    <sheet name="All Enemies - Dead Test" sheetId="23" r:id="rId9"/>
-    <sheet name="Static DMG" sheetId="14" r:id="rId10"/>
-    <sheet name="Group Static" sheetId="15" r:id="rId11"/>
-    <sheet name="O-Weapon" sheetId="20" r:id="rId12"/>
-    <sheet name="PC Cure - Magic" sheetId="17" r:id="rId13"/>
-    <sheet name="PC Cure - Item" sheetId="18" r:id="rId14"/>
-    <sheet name="PC All Heal" sheetId="19" r:id="rId15"/>
-    <sheet name="Status Effect" sheetId="21" r:id="rId16"/>
-    <sheet name="Group Status" sheetId="22" r:id="rId17"/>
-    <sheet name="All Enemies - Status" sheetId="28" r:id="rId18"/>
-    <sheet name="Weak - Elem Melee" sheetId="26" r:id="rId19"/>
-    <sheet name="Weak - Race Melee" sheetId="27" r:id="rId20"/>
+    <sheet name="Ineffective" sheetId="29" r:id="rId3"/>
+    <sheet name="Single AGL" sheetId="3" r:id="rId4"/>
+    <sheet name="Shield" sheetId="7" r:id="rId5"/>
+    <sheet name="Group MANA - PC" sheetId="9" r:id="rId6"/>
+    <sheet name="Group MANA - Enemy" sheetId="11" r:id="rId7"/>
+    <sheet name="Barrier" sheetId="24" r:id="rId8"/>
+    <sheet name="All Enemies - PC" sheetId="13" r:id="rId9"/>
+    <sheet name="All Enemies - Dead Test" sheetId="23" r:id="rId10"/>
+    <sheet name="Static DMG" sheetId="14" r:id="rId11"/>
+    <sheet name="Group Static" sheetId="15" r:id="rId12"/>
+    <sheet name="O-Weapon" sheetId="20" r:id="rId13"/>
+    <sheet name="PC Cure - Magic" sheetId="17" r:id="rId14"/>
+    <sheet name="PC Cure - Item" sheetId="18" r:id="rId15"/>
+    <sheet name="PC All Heal" sheetId="19" r:id="rId16"/>
+    <sheet name="Status Effect" sheetId="21" r:id="rId17"/>
+    <sheet name="Group Status" sheetId="22" r:id="rId18"/>
+    <sheet name="All Enemies - Status" sheetId="28" r:id="rId19"/>
+    <sheet name="Weak - Elem Melee" sheetId="26" r:id="rId20"/>
+    <sheet name="Weak - Race Melee" sheetId="27" r:id="rId21"/>
   </sheets>
   <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="83">
   <si>
     <t>NAME</t>
   </si>
@@ -251,9 +252,6 @@
     <t>Asigaru</t>
   </si>
   <si>
-    <t>Baby-D</t>
-  </si>
-  <si>
     <t>Slashy</t>
   </si>
   <si>
@@ -288,6 +286,9 @@
   </si>
   <si>
     <t>Human F</t>
+  </si>
+  <si>
+    <t>Hatchling</t>
   </si>
 </sst>
 </file>
@@ -762,8 +763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -833,11 +834,11 @@
       <c r="Q1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="R1" s="9" t="s">
+      <c r="R1" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="S1" s="8" t="s">
         <v>73</v>
-      </c>
-      <c r="S1" s="9" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -848,8 +849,8 @@
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="12" t="s">
-        <v>79</v>
+      <c r="D2" s="11" t="s">
+        <v>78</v>
       </c>
       <c r="E2" s="1">
         <v>59</v>
@@ -884,8 +885,8 @@
       <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="12" t="s">
-        <v>80</v>
+      <c r="D3" s="11" t="s">
+        <v>79</v>
       </c>
       <c r="E3" s="1">
         <v>45</v>
@@ -920,8 +921,8 @@
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>70</v>
+      <c r="D4" s="12" t="s">
+        <v>82</v>
       </c>
       <c r="E4" s="1">
         <v>45</v>
@@ -980,8 +981,8 @@
       <c r="K5" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="L5" s="11" t="s">
-        <v>78</v>
+      <c r="L5" s="10" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
@@ -992,8 +993,8 @@
       <c r="B6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="12" t="s">
-        <v>81</v>
+      <c r="D6" s="11" t="s">
+        <v>80</v>
       </c>
       <c r="E6" s="1">
         <v>200</v>
@@ -1034,8 +1035,8 @@
       <c r="B7" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="7" t="s">
-        <v>70</v>
+      <c r="D7" s="12" t="s">
+        <v>82</v>
       </c>
       <c r="E7" s="1">
         <v>999</v>
@@ -1067,11 +1068,11 @@
         <f t="shared" si="0"/>
         <v>Slashy</v>
       </c>
-      <c r="B8" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>82</v>
+      <c r="B8" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>81</v>
       </c>
       <c r="E8" s="1">
         <v>400</v>
@@ -1088,11 +1089,11 @@
       <c r="I8" s="1">
         <v>4</v>
       </c>
-      <c r="J8" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="K8" s="10" t="s">
-        <v>75</v>
+      <c r="J8" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="K8" s="9" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1101,6 +1102,164 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:V5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" t="s">
+        <v>27</v>
+      </c>
+      <c r="O1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R1" t="s">
+        <v>62</v>
+      </c>
+      <c r="S1" t="s">
+        <v>23</v>
+      </c>
+      <c r="T1" t="s">
+        <v>24</v>
+      </c>
+      <c r="U1" t="s">
+        <v>25</v>
+      </c>
+      <c r="V1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A2" t="str">
+        <f>B2</f>
+        <v>Flammie</v>
+      </c>
+      <c r="B2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="L2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A3" t="str">
+        <f>B3</f>
+        <v>Goblin</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A4" t="str">
+        <f t="shared" ref="A4:A5" si="0">B4</f>
+        <v>Jaguar</v>
+      </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A5" t="str">
+        <f t="shared" si="0"/>
+        <v>Asigaru</v>
+      </c>
+      <c r="B5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:V3"/>
   <sheetViews>
@@ -1232,7 +1391,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:V3"/>
   <sheetViews>
@@ -1363,7 +1522,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:V3"/>
   <sheetViews>
@@ -1494,7 +1653,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:V4"/>
   <sheetViews>
@@ -1652,7 +1811,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:V4"/>
   <sheetViews>
@@ -1810,12 +1969,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:V4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1966,7 +2125,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:V3"/>
   <sheetViews>
@@ -2097,7 +2256,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:V3"/>
   <sheetViews>
@@ -2228,7 +2387,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE3B29AC-4EE3-4787-96AC-654F35FC0E64}">
   <dimension ref="A1:V6"/>
   <sheetViews>
@@ -2336,7 +2495,7 @@
         <v>54</v>
       </c>
       <c r="M2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.2">
@@ -2360,7 +2519,7 @@
         <v>30</v>
       </c>
       <c r="M3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.2">
@@ -2384,7 +2543,7 @@
         <v>3</v>
       </c>
       <c r="M4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.2">
@@ -2408,7 +2567,7 @@
         <v>59</v>
       </c>
       <c r="M5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.2">
@@ -2417,144 +2576,13 @@
         <v>SuperJerk</v>
       </c>
       <c r="B6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C6" t="s">
         <v>19</v>
       </c>
       <c r="D6">
         <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{409A1116-4461-47A9-88CD-B9FECC587ADD}">
-  <dimension ref="A1:V3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L1" t="s">
-        <v>15</v>
-      </c>
-      <c r="M1" t="s">
-        <v>16</v>
-      </c>
-      <c r="N1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O1" t="s">
-        <v>21</v>
-      </c>
-      <c r="P1" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>22</v>
-      </c>
-      <c r="R1" t="s">
-        <v>62</v>
-      </c>
-      <c r="S1" t="s">
-        <v>23</v>
-      </c>
-      <c r="T1" t="s">
-        <v>24</v>
-      </c>
-      <c r="U1" t="s">
-        <v>25</v>
-      </c>
-      <c r="V1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A2" t="str">
-        <f>B2</f>
-        <v>Slashy</v>
-      </c>
-      <c r="B2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="L2" t="s">
-        <v>72</v>
-      </c>
-      <c r="M2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A3" t="str">
-        <f>B3</f>
-        <v>Skelton</v>
-      </c>
-      <c r="B3" t="s">
-        <v>66</v>
-      </c>
-      <c r="C3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3">
-        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -2720,6 +2748,137 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{409A1116-4461-47A9-88CD-B9FECC587ADD}">
+  <dimension ref="A1:V3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" t="s">
+        <v>27</v>
+      </c>
+      <c r="O1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R1" t="s">
+        <v>62</v>
+      </c>
+      <c r="S1" t="s">
+        <v>23</v>
+      </c>
+      <c r="T1" t="s">
+        <v>24</v>
+      </c>
+      <c r="U1" t="s">
+        <v>25</v>
+      </c>
+      <c r="V1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A2" t="str">
+        <f>B2</f>
+        <v>Slashy</v>
+      </c>
+      <c r="B2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="L2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A3" t="str">
+        <f>B3</f>
+        <v>Skelton</v>
+      </c>
+      <c r="B3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06BB4AEA-0818-4141-9E54-A13B42F0DE11}">
   <dimension ref="A1:V3"/>
   <sheetViews>
@@ -2812,7 +2971,7 @@
         <v>Slashy</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C2" t="s">
         <v>18</v>
@@ -2824,10 +2983,10 @@
         <v>1</v>
       </c>
       <c r="L2" t="s">
+        <v>74</v>
+      </c>
+      <c r="M2" t="s">
         <v>75</v>
-      </c>
-      <c r="M2" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.2">
@@ -2836,7 +2995,7 @@
         <v>Moth</v>
       </c>
       <c r="B3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C3" t="s">
         <v>19</v>
@@ -2851,6 +3010,177 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CE52F63-C62E-442E-94CC-CFA305D8A1FC}">
+  <dimension ref="A1:V5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="5" width="11.7109375" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" t="s">
+        <v>27</v>
+      </c>
+      <c r="O1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R1" t="s">
+        <v>62</v>
+      </c>
+      <c r="S1" t="s">
+        <v>23</v>
+      </c>
+      <c r="T1" t="s">
+        <v>24</v>
+      </c>
+      <c r="U1" t="s">
+        <v>25</v>
+      </c>
+      <c r="V1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A2" t="str">
+        <f>B2</f>
+        <v>Slashy</v>
+      </c>
+      <c r="B2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="L2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A3" t="str">
+        <f t="shared" ref="A3:A5" si="0">B3</f>
+        <v>MONS</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="L3" t="s">
+        <v>3</v>
+      </c>
+      <c r="M3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A4" t="str">
+        <f t="shared" si="0"/>
+        <v>Goblin</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A5" t="str">
+        <f t="shared" si="0"/>
+        <v>Jaguar</v>
+      </c>
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:V3"/>
@@ -2982,7 +3312,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:V3"/>
@@ -3112,7 +3442,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:V3"/>
   <sheetViews>
@@ -3243,7 +3573,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:V6"/>
   <sheetViews>
@@ -3446,7 +3776,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:V6"/>
   <sheetViews>
@@ -3646,7 +3976,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:V5"/>
   <sheetViews>
@@ -3802,162 +4132,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:V5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L1" t="s">
-        <v>15</v>
-      </c>
-      <c r="M1" t="s">
-        <v>16</v>
-      </c>
-      <c r="N1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O1" t="s">
-        <v>21</v>
-      </c>
-      <c r="P1" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>22</v>
-      </c>
-      <c r="R1" t="s">
-        <v>62</v>
-      </c>
-      <c r="S1" t="s">
-        <v>23</v>
-      </c>
-      <c r="T1" t="s">
-        <v>24</v>
-      </c>
-      <c r="U1" t="s">
-        <v>25</v>
-      </c>
-      <c r="V1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A2" t="str">
-        <f>B2</f>
-        <v>Flammie</v>
-      </c>
-      <c r="B2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="L2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A3" t="str">
-        <f>B3</f>
-        <v>Goblin</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A4" t="str">
-        <f t="shared" ref="A4:A5" si="0">B4</f>
-        <v>Jaguar</v>
-      </c>
-      <c r="B4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A5" t="str">
-        <f t="shared" si="0"/>
-        <v>Asigaru</v>
-      </c>
-      <c r="B5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5">
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Status cleanup, Reflect, bug fixes
</commit_message>
<xml_diff>
--- a/Battle Log.xlsx
+++ b/Battle Log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Action IV\Documents\GitHub\pillar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3158C319-5CF4-4A0C-8CD3-886B6B86A22E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE3A3B12-D480-47BB-AB5B-9103836D36E7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="838" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="838" firstSheet="10" activeTab="21" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Players" sheetId="16" r:id="rId1"/>
@@ -34,13 +34,14 @@
     <sheet name="All Enemies - Status" sheetId="28" r:id="rId19"/>
     <sheet name="Weak - Elem Melee" sheetId="26" r:id="rId20"/>
     <sheet name="Weak - Race Melee" sheetId="27" r:id="rId21"/>
+    <sheet name="Reflect" sheetId="31" r:id="rId22"/>
   </sheets>
   <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="84">
   <si>
     <t>NAME</t>
   </si>
@@ -289,18 +290,28 @@
   </si>
   <si>
     <t>Hatchling</t>
+  </si>
+  <si>
+    <t>Mirror</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -406,11 +417,12 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -764,7 +776,7 @@
   <dimension ref="A1:S8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -905,6 +917,9 @@
       </c>
       <c r="J3" s="1" t="s">
         <v>36</v>
+      </c>
+      <c r="K3" s="13" t="s">
+        <v>83</v>
       </c>
       <c r="N3" s="1" t="s">
         <v>57</v>
@@ -3009,11 +3024,139 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{789776D0-B53E-467F-9655-A7AE3A317022}">
+  <dimension ref="A1:V3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" t="s">
+        <v>27</v>
+      </c>
+      <c r="O1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R1" t="s">
+        <v>62</v>
+      </c>
+      <c r="S1" t="s">
+        <v>23</v>
+      </c>
+      <c r="T1" t="s">
+        <v>24</v>
+      </c>
+      <c r="U1" t="s">
+        <v>25</v>
+      </c>
+      <c r="V1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A2" t="str">
+        <f>B2</f>
+        <v>MUTE</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="L2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A3" t="str">
+        <f>B3</f>
+        <v>Jerk</v>
+      </c>
+      <c r="B3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CE52F63-C62E-442E-94CC-CFA305D8A1FC}">
   <dimension ref="A1:V5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Group Status effects now iterate. Cleaned up all target types
</commit_message>
<xml_diff>
--- a/Battle Log.xlsx
+++ b/Battle Log.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21231"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Action IV\Documents\GitHub\pillar\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scrummel\source\repos\pillar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE3A3B12-D480-47BB-AB5B-9103836D36E7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="838" firstSheet="10" activeTab="21" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="838" firstSheet="9" activeTab="17"/>
   </bookViews>
   <sheets>
     <sheet name="Players" sheetId="16" r:id="rId1"/>
@@ -36,12 +35,12 @@
     <sheet name="Weak - Race Melee" sheetId="27" r:id="rId21"/>
     <sheet name="Reflect" sheetId="31" r:id="rId22"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="84">
   <si>
     <t>NAME</t>
   </si>
@@ -247,9 +246,6 @@
     <t>Ghoul</t>
   </si>
   <si>
-    <t>Mushroom</t>
-  </si>
-  <si>
     <t>Asigaru</t>
   </si>
   <si>
@@ -293,12 +289,15 @@
   </si>
   <si>
     <t>Mirror</t>
+  </si>
+  <si>
+    <t>Stone Book</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -437,7 +436,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -528,23 +527,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -580,23 +562,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -772,11 +737,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -847,10 +812,10 @@
         <v>38</v>
       </c>
       <c r="R1" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="S1" s="8" t="s">
         <v>72</v>
-      </c>
-      <c r="S1" s="8" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -862,7 +827,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E2" s="1">
         <v>59</v>
@@ -898,7 +863,7 @@
         <v>6</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E3" s="1">
         <v>45</v>
@@ -919,7 +884,7 @@
         <v>36</v>
       </c>
       <c r="K3" s="13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="N3" s="1" t="s">
         <v>57</v>
@@ -937,7 +902,7 @@
         <v>2</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E4" s="1">
         <v>45</v>
@@ -997,7 +962,7 @@
         <v>58</v>
       </c>
       <c r="L5" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
@@ -1009,7 +974,7 @@
         <v>31</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E6" s="1">
         <v>200</v>
@@ -1040,6 +1005,9 @@
       </c>
       <c r="N6" s="6" t="s">
         <v>65</v>
+      </c>
+      <c r="O6" s="13" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
@@ -1051,7 +1019,7 @@
         <v>35</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E7" s="1">
         <v>999</v>
@@ -1084,10 +1052,10 @@
         <v>Slashy</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E8" s="1">
         <v>400</v>
@@ -1105,10 +1073,10 @@
         <v>4</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K8" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1117,7 +1085,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1260,7 +1228,7 @@
         <v>Asigaru</v>
       </c>
       <c r="B5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C5" t="s">
         <v>19</v>
@@ -1275,7 +1243,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V3"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
@@ -1407,7 +1375,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1538,7 +1506,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1669,7 +1637,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1827,7 +1795,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1985,7 +1953,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2141,7 +2109,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2272,11 +2240,11 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2376,25 +2344,25 @@
         <v>1</v>
       </c>
       <c r="L2" t="s">
-        <v>60</v>
+        <v>83</v>
       </c>
       <c r="M2" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
         <f>B3</f>
-        <v>Mushroom</v>
+        <v>Goblin</v>
       </c>
       <c r="B3" t="s">
-        <v>68</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
         <v>19</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -2403,7 +2371,7 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE3B29AC-4EE3-4787-96AC-654F35FC0E64}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2510,7 +2478,7 @@
         <v>54</v>
       </c>
       <c r="M2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.2">
@@ -2534,7 +2502,7 @@
         <v>30</v>
       </c>
       <c r="M3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.2">
@@ -2558,7 +2526,7 @@
         <v>3</v>
       </c>
       <c r="M4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.2">
@@ -2582,7 +2550,7 @@
         <v>59</v>
       </c>
       <c r="M5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.2">
@@ -2591,7 +2559,7 @@
         <v>SuperJerk</v>
       </c>
       <c r="B6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C6" t="s">
         <v>19</v>
@@ -2606,7 +2574,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:V4"/>
   <sheetViews>
@@ -2763,7 +2731,7 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{409A1116-4461-47A9-88CD-B9FECC587ADD}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2855,7 +2823,7 @@
         <v>Slashy</v>
       </c>
       <c r="B2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C2" t="s">
         <v>18</v>
@@ -2867,7 +2835,7 @@
         <v>1</v>
       </c>
       <c r="L2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="M2" t="s">
         <v>66</v>
@@ -2894,7 +2862,7 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06BB4AEA-0818-4141-9E54-A13B42F0DE11}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2986,7 +2954,7 @@
         <v>Slashy</v>
       </c>
       <c r="B2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C2" t="s">
         <v>18</v>
@@ -2998,10 +2966,10 @@
         <v>1</v>
       </c>
       <c r="L2" t="s">
+        <v>73</v>
+      </c>
+      <c r="M2" t="s">
         <v>74</v>
-      </c>
-      <c r="M2" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.2">
@@ -3010,7 +2978,7 @@
         <v>Moth</v>
       </c>
       <c r="B3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C3" t="s">
         <v>19</v>
@@ -3025,10 +2993,10 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{789776D0-B53E-467F-9655-A7AE3A317022}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
@@ -3129,7 +3097,7 @@
         <v>1</v>
       </c>
       <c r="L2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.2">
@@ -3153,7 +3121,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CE52F63-C62E-442E-94CC-CFA305D8A1FC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3246,7 +3214,7 @@
         <v>Slashy</v>
       </c>
       <c r="B2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C2" t="s">
         <v>18</v>
@@ -3258,7 +3226,7 @@
         <v>2</v>
       </c>
       <c r="L2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="M2" t="s">
         <v>4</v>
@@ -3324,7 +3292,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:V3"/>
   <sheetViews>
@@ -3456,7 +3424,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:V3"/>
   <sheetViews>
@@ -3586,7 +3554,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3717,7 +3685,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3920,7 +3888,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4120,7 +4088,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V5"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Change to save Actions Taken
</commit_message>
<xml_diff>
--- a/Battle Log.xlsx
+++ b/Battle Log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Action IV\Documents\GitHub\pillar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCD65F7D-0871-41D3-8478-350961C96950}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD8AE56C-1D84-416A-BB74-B9977FFBC584}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="838" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="838" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Players" sheetId="16" r:id="rId1"/>
@@ -9279,7 +9279,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F9CF8B5-E403-487C-8FDB-E1A3B4A0FA54}">
   <dimension ref="A1:U14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:U14"/>
     </sheetView>
   </sheetViews>
@@ -10996,8 +10996,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:U4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -11099,33 +11099,33 @@
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="K3" t="s">
+        <v>3</v>
+      </c>
+      <c r="L3" t="s">
         <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4">
         <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="K4" t="s">
-        <v>3</v>
-      </c>
-      <c r="L4" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -12202,7 +12202,7 @@
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -12307,7 +12307,7 @@
         <v>19</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed Stunned column. Fixed Position bug
</commit_message>
<xml_diff>
--- a/Battle Log.xlsx
+++ b/Battle Log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Action IV\Documents\GitHub\pillar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD8AE56C-1D84-416A-BB74-B9977FFBC584}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE3B93DE-0127-40F6-82D0-645A59CEF658}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="838" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="838" firstSheet="13" activeTab="24" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Players" sheetId="16" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="859" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="835" uniqueCount="95">
   <si>
     <t>NAME</t>
   </si>
@@ -113,9 +113,6 @@
   </si>
   <si>
     <t>Cursed</t>
-  </si>
-  <si>
-    <t>Stunned</t>
   </si>
   <si>
     <t>Paralyzed</t>
@@ -8547,70 +8544,70 @@
         <v>20</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F1" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="G1" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="H1" s="16" t="s">
+      <c r="I1" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="J1" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="I1" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="J1" s="16" t="s">
+      <c r="K1" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="L1" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="K1" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="L1" s="16" t="s">
-        <v>93</v>
-      </c>
       <c r="M1" s="18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="N1" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O1" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="P1" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Q1" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="R1" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="S1" s="15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="T1" s="15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="U1" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="V1" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="W1" s="17" t="s">
         <v>71</v>
-      </c>
-      <c r="W1" s="17" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
@@ -8622,7 +8619,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E2" s="1">
         <v>59</v>
@@ -8656,13 +8653,13 @@
         <v>3</v>
       </c>
       <c r="N2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="O2" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="Q2" s="13"/>
     </row>
@@ -8675,7 +8672,7 @@
         <v>6</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E3" s="1">
         <v>45</v>
@@ -8709,16 +8706,16 @@
         <v>6</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="O3" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
@@ -8730,7 +8727,7 @@
         <v>2</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E4" s="1">
         <v>45</v>
@@ -8767,10 +8764,10 @@
         <v>3</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P4" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
@@ -8779,10 +8776,10 @@
         <v>ROBO</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E5" s="1">
         <v>60</v>
@@ -8816,13 +8813,13 @@
         <v>0</v>
       </c>
       <c r="N5" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="P5" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
@@ -8831,10 +8828,10 @@
         <v>Zappo</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E6" s="1">
         <v>200</v>
@@ -8868,22 +8865,22 @@
         <v>6</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="P6" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="Q6" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="R6" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="S6" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
@@ -8892,10 +8889,10 @@
         <v>Flammie</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E7" s="1">
         <v>999</v>
@@ -8932,10 +8929,10 @@
         <v>3</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P7" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
@@ -8944,10 +8941,10 @@
         <v>Slashy</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E8" s="1">
         <v>400</v>
@@ -8981,10 +8978,10 @@
         <v>4</v>
       </c>
       <c r="N8" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="O8" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
@@ -8993,10 +8990,10 @@
         <v>Revenge</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E9" s="1">
         <v>100</v>
@@ -9030,7 +9027,7 @@
         <v>3</v>
       </c>
       <c r="N9" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
@@ -9039,10 +9036,10 @@
         <v>Turtle1</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E10" s="1">
         <v>100</v>
@@ -9076,7 +9073,7 @@
         <v>10</v>
       </c>
       <c r="N10" s="14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
@@ -9085,10 +9082,10 @@
         <v>Turtle2</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E11" s="1">
         <v>100</v>
@@ -9122,7 +9119,7 @@
         <v>10</v>
       </c>
       <c r="N11" s="14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -9138,10 +9135,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:U5"/>
+  <dimension ref="A1:T5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="P1" sqref="P1:P1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9155,7 +9152,7 @@
     <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -9193,19 +9190,19 @@
         <v>16</v>
       </c>
       <c r="M1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N1" t="s">
         <v>21</v>
       </c>
       <c r="O1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q1" t="s">
         <v>22</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>62</v>
       </c>
       <c r="R1" t="s">
         <v>23</v>
@@ -9214,15 +9211,12 @@
         <v>24</v>
       </c>
       <c r="T1" t="s">
-        <v>25</v>
-      </c>
-      <c r="U1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
@@ -9234,10 +9228,10 @@
         <v>1</v>
       </c>
       <c r="K2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -9248,9 +9242,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4" t="s">
         <v>19</v>
@@ -9259,9 +9253,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B5" t="s">
         <v>19</v>
@@ -9277,10 +9271,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F9CF8B5-E403-487C-8FDB-E1A3B4A0FA54}">
-  <dimension ref="A1:U14"/>
+  <dimension ref="A1:T14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:U14"/>
+      <selection activeCell="P1" sqref="P1:P1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9294,7 +9288,7 @@
     <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -9332,19 +9326,19 @@
         <v>16</v>
       </c>
       <c r="M1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N1" t="s">
         <v>21</v>
       </c>
       <c r="O1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q1" t="s">
         <v>22</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>62</v>
       </c>
       <c r="R1" t="s">
         <v>23</v>
@@ -9353,15 +9347,12 @@
         <v>24</v>
       </c>
       <c r="T1" t="s">
-        <v>25</v>
-      </c>
-      <c r="U1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
@@ -9391,12 +9382,12 @@
         <v>99</v>
       </c>
       <c r="K2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
         <v>19</v>
@@ -9426,30 +9417,30 @@
         <v>5</v>
       </c>
       <c r="K3" t="s">
+        <v>93</v>
+      </c>
+      <c r="N3" t="s">
         <v>94</v>
       </c>
-      <c r="N3" t="s">
-        <v>95</v>
-      </c>
       <c r="O3" t="s">
-        <v>95</v>
+        <v>94</v>
+      </c>
+      <c r="P3" t="s">
+        <v>94</v>
       </c>
       <c r="Q3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="R3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="S3" t="s">
-        <v>95</v>
-      </c>
-      <c r="T3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B4" t="s">
         <v>19</v>
@@ -9479,12 +9470,12 @@
         <v>6</v>
       </c>
       <c r="K4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5" t="s">
         <v>19</v>
@@ -9514,30 +9505,30 @@
         <v>5</v>
       </c>
       <c r="K5" t="s">
+        <v>93</v>
+      </c>
+      <c r="N5" t="s">
         <v>94</v>
       </c>
-      <c r="N5" t="s">
-        <v>95</v>
-      </c>
       <c r="O5" t="s">
-        <v>95</v>
+        <v>94</v>
+      </c>
+      <c r="P5" t="s">
+        <v>94</v>
       </c>
       <c r="Q5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="R5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="S5" t="s">
-        <v>95</v>
-      </c>
-      <c r="T5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B6" t="s">
         <v>19</v>
@@ -9567,12 +9558,12 @@
         <v>6</v>
       </c>
       <c r="K6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B7" t="s">
         <v>19</v>
@@ -9602,12 +9593,12 @@
         <v>6</v>
       </c>
       <c r="K7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B8" t="s">
         <v>19</v>
@@ -9637,12 +9628,12 @@
         <v>6</v>
       </c>
       <c r="K8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B9" t="s">
         <v>19</v>
@@ -9672,30 +9663,30 @@
         <v>5</v>
       </c>
       <c r="K9" t="s">
+        <v>93</v>
+      </c>
+      <c r="N9" t="s">
         <v>94</v>
       </c>
-      <c r="N9" t="s">
-        <v>95</v>
-      </c>
       <c r="O9" t="s">
-        <v>95</v>
+        <v>94</v>
+      </c>
+      <c r="P9" t="s">
+        <v>94</v>
       </c>
       <c r="Q9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="R9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="S9" t="s">
-        <v>95</v>
-      </c>
-      <c r="T9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10" t="s">
         <v>19</v>
@@ -9725,28 +9716,28 @@
         <v>5</v>
       </c>
       <c r="K10" t="s">
+        <v>93</v>
+      </c>
+      <c r="N10" t="s">
         <v>94</v>
       </c>
-      <c r="N10" t="s">
-        <v>95</v>
-      </c>
       <c r="O10" t="s">
-        <v>95</v>
+        <v>94</v>
+      </c>
+      <c r="P10" t="s">
+        <v>94</v>
       </c>
       <c r="Q10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="R10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="S10" t="s">
-        <v>95</v>
-      </c>
-      <c r="T10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -9778,28 +9769,28 @@
         <v>5</v>
       </c>
       <c r="K11" t="s">
+        <v>93</v>
+      </c>
+      <c r="N11" t="s">
         <v>94</v>
       </c>
-      <c r="N11" t="s">
-        <v>95</v>
-      </c>
       <c r="O11" t="s">
-        <v>95</v>
+        <v>94</v>
+      </c>
+      <c r="P11" t="s">
+        <v>94</v>
       </c>
       <c r="Q11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="R11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="S11" t="s">
-        <v>95</v>
-      </c>
-      <c r="T11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -9831,28 +9822,28 @@
         <v>5</v>
       </c>
       <c r="K12" t="s">
+        <v>93</v>
+      </c>
+      <c r="N12" t="s">
         <v>94</v>
       </c>
-      <c r="N12" t="s">
-        <v>95</v>
-      </c>
       <c r="O12" t="s">
-        <v>95</v>
+        <v>94</v>
+      </c>
+      <c r="P12" t="s">
+        <v>94</v>
       </c>
       <c r="Q12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="R12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="S12" t="s">
-        <v>95</v>
-      </c>
-      <c r="T12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -9884,28 +9875,28 @@
         <v>5</v>
       </c>
       <c r="K13" t="s">
+        <v>93</v>
+      </c>
+      <c r="N13" t="s">
         <v>94</v>
       </c>
-      <c r="N13" t="s">
-        <v>95</v>
-      </c>
       <c r="O13" t="s">
-        <v>95</v>
+        <v>94</v>
+      </c>
+      <c r="P13" t="s">
+        <v>94</v>
       </c>
       <c r="Q13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="R13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="S13" t="s">
-        <v>95</v>
-      </c>
-      <c r="T13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -9937,25 +9928,25 @@
         <v>5</v>
       </c>
       <c r="K14" t="s">
+        <v>93</v>
+      </c>
+      <c r="N14" t="s">
         <v>94</v>
       </c>
-      <c r="N14" t="s">
-        <v>95</v>
-      </c>
       <c r="O14" t="s">
-        <v>95</v>
+        <v>94</v>
+      </c>
+      <c r="P14" t="s">
+        <v>94</v>
       </c>
       <c r="Q14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="R14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="S14" t="s">
-        <v>95</v>
-      </c>
-      <c r="T14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -9965,10 +9956,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:U3"/>
+  <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="P1" sqref="P1:P1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9980,10 +9971,10 @@
     <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -10021,19 +10012,19 @@
         <v>16</v>
       </c>
       <c r="M1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N1" t="s">
         <v>21</v>
       </c>
       <c r="O1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q1" t="s">
         <v>22</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>62</v>
       </c>
       <c r="R1" t="s">
         <v>23</v>
@@ -10042,15 +10033,12 @@
         <v>24</v>
       </c>
       <c r="T1" t="s">
-        <v>25</v>
-      </c>
-      <c r="U1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
@@ -10062,13 +10050,13 @@
         <v>1</v>
       </c>
       <c r="K2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -10086,10 +10074,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <dimension ref="A1:U3"/>
+  <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="P1" sqref="P1:P1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -10103,7 +10091,7 @@
     <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -10141,19 +10129,19 @@
         <v>16</v>
       </c>
       <c r="M1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N1" t="s">
         <v>21</v>
       </c>
       <c r="O1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q1" t="s">
         <v>22</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>62</v>
       </c>
       <c r="R1" t="s">
         <v>23</v>
@@ -10162,15 +10150,12 @@
         <v>24</v>
       </c>
       <c r="T1" t="s">
-        <v>25</v>
-      </c>
-      <c r="U1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
@@ -10182,13 +10167,13 @@
         <v>1</v>
       </c>
       <c r="K2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -10206,10 +10191,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <dimension ref="A1:U3"/>
+  <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="P1" sqref="P1:P1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -10223,7 +10208,7 @@
     <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -10261,19 +10246,19 @@
         <v>16</v>
       </c>
       <c r="M1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N1" t="s">
         <v>21</v>
       </c>
       <c r="O1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q1" t="s">
         <v>22</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>62</v>
       </c>
       <c r="R1" t="s">
         <v>23</v>
@@ -10282,15 +10267,12 @@
         <v>24</v>
       </c>
       <c r="T1" t="s">
-        <v>25</v>
-      </c>
-      <c r="U1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
@@ -10302,15 +10284,15 @@
         <v>1</v>
       </c>
       <c r="K2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B3" t="s">
         <v>19</v>
@@ -10326,10 +10308,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
-  <dimension ref="A1:U4"/>
+  <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="P1" sqref="P1:P1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -10343,7 +10325,7 @@
     <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -10381,19 +10363,19 @@
         <v>16</v>
       </c>
       <c r="M1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N1" t="s">
         <v>21</v>
       </c>
       <c r="O1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q1" t="s">
         <v>22</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>62</v>
       </c>
       <c r="R1" t="s">
         <v>23</v>
@@ -10402,15 +10384,12 @@
         <v>24</v>
       </c>
       <c r="T1" t="s">
-        <v>25</v>
-      </c>
-      <c r="U1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
@@ -10422,15 +10401,15 @@
         <v>1</v>
       </c>
       <c r="K2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B3" t="s">
         <v>18</v>
@@ -10451,7 +10430,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -10469,10 +10448,10 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
-  <dimension ref="A1:U4"/>
+  <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="P1" sqref="P1:P1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -10486,7 +10465,7 @@
     <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -10524,19 +10503,19 @@
         <v>16</v>
       </c>
       <c r="M1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N1" t="s">
         <v>21</v>
       </c>
       <c r="O1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q1" t="s">
         <v>22</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>62</v>
       </c>
       <c r="R1" t="s">
         <v>23</v>
@@ -10545,15 +10524,12 @@
         <v>24</v>
       </c>
       <c r="T1" t="s">
-        <v>25</v>
-      </c>
-      <c r="U1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
@@ -10568,15 +10544,15 @@
         <v>150</v>
       </c>
       <c r="K2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B3" t="s">
         <v>18</v>
@@ -10588,13 +10564,13 @@
         <v>2</v>
       </c>
       <c r="K3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -10612,10 +10588,10 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <dimension ref="A1:U4"/>
+  <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="P1" sqref="P1:P1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -10627,10 +10603,10 @@
     <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -10668,19 +10644,19 @@
         <v>16</v>
       </c>
       <c r="M1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N1" t="s">
         <v>21</v>
       </c>
       <c r="O1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q1" t="s">
         <v>22</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>62</v>
       </c>
       <c r="R1" t="s">
         <v>23</v>
@@ -10689,13 +10665,10 @@
         <v>24</v>
       </c>
       <c r="T1" t="s">
-        <v>25</v>
-      </c>
-      <c r="U1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -10712,12 +10685,12 @@
         <v>30</v>
       </c>
       <c r="K2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
         <v>19</v>
@@ -10726,9 +10699,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
@@ -10743,7 +10716,7 @@
         <v>100</v>
       </c>
       <c r="K4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -10753,10 +10726,10 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
-  <dimension ref="A1:U3"/>
+  <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="P1" sqref="P1:P1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -10770,7 +10743,7 @@
     <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -10808,19 +10781,19 @@
         <v>16</v>
       </c>
       <c r="M1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N1" t="s">
         <v>21</v>
       </c>
       <c r="O1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q1" t="s">
         <v>22</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>62</v>
       </c>
       <c r="R1" t="s">
         <v>23</v>
@@ -10829,15 +10802,12 @@
         <v>24</v>
       </c>
       <c r="T1" t="s">
-        <v>25</v>
-      </c>
-      <c r="U1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
@@ -10849,15 +10819,15 @@
         <v>1</v>
       </c>
       <c r="K2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B3" t="s">
         <v>19</v>
@@ -10873,10 +10843,10 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
-  <dimension ref="A1:U3"/>
+  <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="P1" sqref="P1:P1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -10890,7 +10860,7 @@
     <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -10928,19 +10898,19 @@
         <v>16</v>
       </c>
       <c r="M1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N1" t="s">
         <v>21</v>
       </c>
       <c r="O1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q1" t="s">
         <v>22</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>62</v>
       </c>
       <c r="R1" t="s">
         <v>23</v>
@@ -10949,15 +10919,12 @@
         <v>24</v>
       </c>
       <c r="T1" t="s">
-        <v>25</v>
-      </c>
-      <c r="U1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
@@ -10969,13 +10936,13 @@
         <v>1</v>
       </c>
       <c r="K2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -10994,10 +10961,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:U4"/>
+  <dimension ref="A1:T4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P1" sqref="P1:P1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -11009,10 +10976,10 @@
     <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -11050,19 +11017,19 @@
         <v>16</v>
       </c>
       <c r="M1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N1" t="s">
         <v>21</v>
       </c>
       <c r="O1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q1" t="s">
         <v>22</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>62</v>
       </c>
       <c r="R1" t="s">
         <v>23</v>
@@ -11071,13 +11038,10 @@
         <v>24</v>
       </c>
       <c r="T1" t="s">
-        <v>25</v>
-      </c>
-      <c r="U1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -11091,13 +11055,13 @@
         <v>2</v>
       </c>
       <c r="K2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -11117,7 +11081,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -11135,10 +11099,10 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
-  <dimension ref="A1:U6"/>
+  <dimension ref="A1:T6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="P1" sqref="P1:P1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -11152,7 +11116,7 @@
     <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -11190,19 +11154,19 @@
         <v>16</v>
       </c>
       <c r="M1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N1" t="s">
         <v>21</v>
       </c>
       <c r="O1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q1" t="s">
         <v>22</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>62</v>
       </c>
       <c r="R1" t="s">
         <v>23</v>
@@ -11211,13 +11175,10 @@
         <v>24</v>
       </c>
       <c r="T1" t="s">
-        <v>25</v>
-      </c>
-      <c r="U1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -11231,13 +11192,13 @@
         <v>1</v>
       </c>
       <c r="K2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -11251,13 +11212,13 @@
         <v>2</v>
       </c>
       <c r="K3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -11274,12 +11235,12 @@
         <v>3</v>
       </c>
       <c r="L4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B5" t="s">
         <v>18</v>
@@ -11291,15 +11252,15 @@
         <v>4</v>
       </c>
       <c r="K5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B6" t="s">
         <v>19</v>
@@ -11315,10 +11276,10 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
-  <dimension ref="A1:U3"/>
+  <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="P1" sqref="P1:P1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -11332,7 +11293,7 @@
     <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -11370,19 +11331,19 @@
         <v>16</v>
       </c>
       <c r="M1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N1" t="s">
         <v>21</v>
       </c>
       <c r="O1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q1" t="s">
         <v>22</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>62</v>
       </c>
       <c r="R1" t="s">
         <v>23</v>
@@ -11391,15 +11352,12 @@
         <v>24</v>
       </c>
       <c r="T1" t="s">
-        <v>25</v>
-      </c>
-      <c r="U1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
@@ -11411,15 +11369,15 @@
         <v>1</v>
       </c>
       <c r="K2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B3" t="s">
         <v>19</v>
@@ -11435,10 +11393,10 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
-  <dimension ref="A1:U3"/>
+  <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="P1" sqref="P1:P1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -11452,7 +11410,7 @@
     <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -11490,19 +11448,19 @@
         <v>16</v>
       </c>
       <c r="M1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N1" t="s">
         <v>21</v>
       </c>
       <c r="O1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q1" t="s">
         <v>22</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>62</v>
       </c>
       <c r="R1" t="s">
         <v>23</v>
@@ -11511,15 +11469,12 @@
         <v>24</v>
       </c>
       <c r="T1" t="s">
-        <v>25</v>
-      </c>
-      <c r="U1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
@@ -11531,15 +11486,15 @@
         <v>1</v>
       </c>
       <c r="K2" t="s">
+        <v>72</v>
+      </c>
+      <c r="L2" t="s">
         <v>73</v>
       </c>
-      <c r="L2" t="s">
-        <v>74</v>
-      </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B3" t="s">
         <v>19</v>
@@ -11555,10 +11510,10 @@
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
-  <dimension ref="A1:U3"/>
+  <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="P1" sqref="P1:P1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -11572,7 +11527,7 @@
     <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -11610,19 +11565,19 @@
         <v>16</v>
       </c>
       <c r="M1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N1" t="s">
         <v>21</v>
       </c>
       <c r="O1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q1" t="s">
         <v>22</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>62</v>
       </c>
       <c r="R1" t="s">
         <v>23</v>
@@ -11631,13 +11586,10 @@
         <v>24</v>
       </c>
       <c r="T1" t="s">
-        <v>25</v>
-      </c>
-      <c r="U1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -11651,12 +11603,12 @@
         <v>1</v>
       </c>
       <c r="K2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
         <v>19</v>
@@ -11672,10 +11624,10 @@
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40C62C4B-A558-47BB-B36D-F4A067E322AA}">
-  <dimension ref="A1:U3"/>
+  <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="P1" sqref="P1:P1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -11687,10 +11639,10 @@
     <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -11728,19 +11680,19 @@
         <v>16</v>
       </c>
       <c r="M1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N1" t="s">
         <v>21</v>
       </c>
       <c r="O1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q1" t="s">
         <v>22</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>62</v>
       </c>
       <c r="R1" t="s">
         <v>23</v>
@@ -11749,15 +11701,12 @@
         <v>24</v>
       </c>
       <c r="T1" t="s">
-        <v>25</v>
-      </c>
-      <c r="U1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
@@ -11769,10 +11718,10 @@
         <v>1</v>
       </c>
       <c r="K2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -11790,10 +11739,10 @@
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4822E79-A2B0-4184-B515-4C5C1DD56F74}">
-  <dimension ref="A1:U4"/>
+  <dimension ref="A1:T4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -11805,10 +11754,10 @@
     <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -11846,19 +11795,19 @@
         <v>16</v>
       </c>
       <c r="M1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N1" t="s">
         <v>21</v>
       </c>
       <c r="O1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q1" t="s">
         <v>22</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>62</v>
       </c>
       <c r="R1" t="s">
         <v>23</v>
@@ -11867,15 +11816,12 @@
         <v>24</v>
       </c>
       <c r="T1" t="s">
-        <v>25</v>
-      </c>
-      <c r="U1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
@@ -11887,10 +11833,10 @@
         <v>1</v>
       </c>
       <c r="K2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -11901,9 +11847,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
@@ -11915,7 +11861,7 @@
         <v>2</v>
       </c>
       <c r="K4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -11925,10 +11871,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:U5"/>
+  <dimension ref="A1:T5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="P1" sqref="P1:P1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -11940,10 +11886,10 @@
     <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -11981,19 +11927,19 @@
         <v>16</v>
       </c>
       <c r="M1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N1" t="s">
         <v>21</v>
       </c>
       <c r="O1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q1" t="s">
         <v>22</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>62</v>
       </c>
       <c r="R1" t="s">
         <v>23</v>
@@ -12002,15 +11948,12 @@
         <v>24</v>
       </c>
       <c r="T1" t="s">
-        <v>25</v>
-      </c>
-      <c r="U1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
@@ -12022,13 +11965,13 @@
         <v>2</v>
       </c>
       <c r="K2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -12048,7 +11991,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -12059,9 +12002,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5" t="s">
         <v>19</v>
@@ -12078,10 +12021,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:U3"/>
+  <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="P1" sqref="P1:P1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -12095,7 +12038,7 @@
     <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -12133,19 +12076,19 @@
         <v>16</v>
       </c>
       <c r="M1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N1" t="s">
         <v>21</v>
       </c>
       <c r="O1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q1" t="s">
         <v>22</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>62</v>
       </c>
       <c r="R1" t="s">
         <v>23</v>
@@ -12154,13 +12097,10 @@
         <v>24</v>
       </c>
       <c r="T1" t="s">
-        <v>25</v>
-      </c>
-      <c r="U1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -12174,15 +12114,15 @@
         <v>1</v>
       </c>
       <c r="K2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
         <v>19</v>
@@ -12199,10 +12139,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:U3"/>
+  <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="P1" sqref="P1:P1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -12214,10 +12154,10 @@
     <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -12255,19 +12195,19 @@
         <v>16</v>
       </c>
       <c r="M1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N1" t="s">
         <v>21</v>
       </c>
       <c r="O1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q1" t="s">
         <v>22</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>62</v>
       </c>
       <c r="R1" t="s">
         <v>23</v>
@@ -12276,13 +12216,10 @@
         <v>24</v>
       </c>
       <c r="T1" t="s">
-        <v>25</v>
-      </c>
-      <c r="U1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -12296,12 +12233,12 @@
         <v>1</v>
       </c>
       <c r="K2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
         <v>19</v>
@@ -12317,10 +12254,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:U3"/>
+  <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="P1" sqref="P1:P1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -12334,7 +12271,7 @@
     <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -12372,19 +12309,19 @@
         <v>16</v>
       </c>
       <c r="M1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N1" t="s">
         <v>21</v>
       </c>
       <c r="O1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q1" t="s">
         <v>22</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>62</v>
       </c>
       <c r="R1" t="s">
         <v>23</v>
@@ -12393,15 +12330,12 @@
         <v>24</v>
       </c>
       <c r="T1" t="s">
-        <v>25</v>
-      </c>
-      <c r="U1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
@@ -12413,13 +12347,13 @@
         <v>1</v>
       </c>
       <c r="K2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -12437,10 +12371,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:U6"/>
+  <dimension ref="A1:T6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="P1" sqref="P1:P1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -12454,7 +12388,7 @@
     <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -12492,19 +12426,19 @@
         <v>16</v>
       </c>
       <c r="M1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N1" t="s">
         <v>21</v>
       </c>
       <c r="O1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q1" t="s">
         <v>22</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>62</v>
       </c>
       <c r="R1" t="s">
         <v>23</v>
@@ -12513,13 +12447,10 @@
         <v>24</v>
       </c>
       <c r="T1" t="s">
-        <v>25</v>
-      </c>
-      <c r="U1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -12533,13 +12464,13 @@
         <v>1</v>
       </c>
       <c r="K2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -12553,13 +12484,13 @@
         <v>2</v>
       </c>
       <c r="K3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -12576,12 +12507,12 @@
         <v>3</v>
       </c>
       <c r="L4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B5" t="s">
         <v>18</v>
@@ -12593,15 +12524,15 @@
         <v>4</v>
       </c>
       <c r="K5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B6" t="s">
         <v>19</v>
@@ -12617,10 +12548,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:U6"/>
+  <dimension ref="A1:T6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="P1" sqref="P1:P1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -12634,7 +12565,7 @@
     <col min="11" max="11" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -12672,19 +12603,19 @@
         <v>16</v>
       </c>
       <c r="M1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N1" t="s">
         <v>21</v>
       </c>
       <c r="O1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q1" t="s">
         <v>22</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>62</v>
       </c>
       <c r="R1" t="s">
         <v>23</v>
@@ -12693,13 +12624,10 @@
         <v>24</v>
       </c>
       <c r="T1" t="s">
-        <v>25</v>
-      </c>
-      <c r="U1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -12713,10 +12641,10 @@
         <v>1</v>
       </c>
       <c r="K2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -12730,13 +12658,13 @@
         <v>2</v>
       </c>
       <c r="K3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -12753,12 +12681,12 @@
         <v>3</v>
       </c>
       <c r="L4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B5" t="s">
         <v>18</v>
@@ -12770,15 +12698,15 @@
         <v>4</v>
       </c>
       <c r="K5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B6" t="s">
         <v>19</v>
@@ -12794,10 +12722,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:U5"/>
+  <dimension ref="A1:T5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="P1" sqref="P1:P1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -12811,7 +12739,7 @@
     <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -12849,19 +12777,19 @@
         <v>16</v>
       </c>
       <c r="M1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N1" t="s">
         <v>21</v>
       </c>
       <c r="O1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q1" t="s">
         <v>22</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>62</v>
       </c>
       <c r="R1" t="s">
         <v>23</v>
@@ -12870,15 +12798,12 @@
         <v>24</v>
       </c>
       <c r="T1" t="s">
-        <v>25</v>
-      </c>
-      <c r="U1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
@@ -12890,10 +12815,10 @@
         <v>1</v>
       </c>
       <c r="K2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -12904,9 +12829,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4" t="s">
         <v>19</v>
@@ -12915,9 +12840,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B5" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
Surprise and Warning. "None" Command bug fix
</commit_message>
<xml_diff>
--- a/Battle Log.xlsx
+++ b/Battle Log.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21231"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Action IV\Documents\GitHub\pillar\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scrummel\source\repos\pillar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE3B93DE-0127-40F6-82D0-645A59CEF658}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="838" firstSheet="13" activeTab="24" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="-120" windowWidth="20490" windowHeight="7785" tabRatio="838" firstSheet="19" activeTab="27"/>
   </bookViews>
   <sheets>
     <sheet name="Players" sheetId="16" r:id="rId1"/>
@@ -38,16 +37,19 @@
     <sheet name="Reflect" sheetId="31" r:id="rId23"/>
     <sheet name="STR Counter" sheetId="32" r:id="rId24"/>
     <sheet name="Other Counters" sheetId="33" r:id="rId25"/>
+    <sheet name="Enemy Surprise" sheetId="36" r:id="rId26"/>
+    <sheet name="Player Surprise" sheetId="37" r:id="rId27"/>
+    <sheet name="Both Surprise" sheetId="38" r:id="rId28"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId26"/>
+    <externalReference r:id="rId29"/>
   </externalReferences>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="835" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="918" uniqueCount="100">
   <si>
     <t>NAME</t>
   </si>
@@ -333,11 +335,26 @@
   <si>
     <t>n</t>
   </si>
+  <si>
+    <t>WereWolf</t>
+  </si>
+  <si>
+    <t>Leonardo</t>
+  </si>
+  <si>
+    <t>Warning</t>
+  </si>
+  <si>
+    <t>Surprise</t>
+  </si>
+  <si>
+    <t>Katana</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -485,7 +502,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -515,10 +532,11 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -8271,23 +8289,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -8323,23 +8324,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -8515,11 +8499,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:W12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8612,7 +8596,7 @@
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="str">
-        <f t="shared" ref="A2:A11" si="0">B2</f>
+        <f t="shared" ref="A2:A12" si="0">B2</f>
         <v>HUME</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -8681,7 +8665,7 @@
         <v>4</v>
       </c>
       <c r="G3" s="19">
-        <f t="shared" ref="G3:G11" si="1">F3</f>
+        <f t="shared" ref="G3:G12" si="1">F3</f>
         <v>4</v>
       </c>
       <c r="H3" s="1">
@@ -8695,14 +8679,14 @@
         <v>5</v>
       </c>
       <c r="K3" s="19">
-        <f t="shared" ref="K3:K11" si="2">J3</f>
+        <f t="shared" ref="K3:K12" si="2">J3</f>
         <v>5</v>
       </c>
       <c r="L3" s="1">
         <v>6</v>
       </c>
       <c r="M3" s="19">
-        <f t="shared" ref="M3:M11" si="3">L3</f>
+        <f t="shared" ref="M3:M12" si="3">L3</f>
         <v>6</v>
       </c>
       <c r="N3" s="1" t="s">
@@ -9120,6 +9104,57 @@
       </c>
       <c r="N11" s="14" t="s">
         <v>88</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Leonardo</v>
+      </c>
+      <c r="B12" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="D12" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="E12" s="1">
+        <v>250</v>
+      </c>
+      <c r="F12" s="1">
+        <v>30</v>
+      </c>
+      <c r="G12" s="1">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="H12" s="1">
+        <v>15</v>
+      </c>
+      <c r="I12" s="19">
+        <v>30</v>
+      </c>
+      <c r="J12" s="1">
+        <v>50</v>
+      </c>
+      <c r="K12" s="1">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+      <c r="L12" s="1">
+        <v>11</v>
+      </c>
+      <c r="M12" s="1">
+        <f t="shared" si="3"/>
+        <v>11</v>
+      </c>
+      <c r="N12" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="O12" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="P12" s="21" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -9134,7 +9169,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9270,7 +9305,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F9CF8B5-E403-487C-8FDB-E1A3B4A0FA54}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9955,7 +9990,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10073,7 +10108,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10190,7 +10225,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10307,7 +10342,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10447,7 +10482,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10587,7 +10622,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10725,7 +10760,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10842,7 +10877,7 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10959,7 +10994,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:T4"/>
   <sheetViews>
@@ -11098,7 +11133,7 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11275,7 +11310,7 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11392,7 +11427,7 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11509,7 +11544,7 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11623,7 +11658,7 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40C62C4B-A558-47BB-B36D-F4A067E322AA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11738,10 +11773,10 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4822E79-A2B0-4184-B515-4C5C1DD56F74}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
@@ -11869,8 +11904,362 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="4" width="11.7109375" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" t="s">
+        <v>25</v>
+      </c>
+      <c r="P1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R1" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1" t="s">
+        <v>24</v>
+      </c>
+      <c r="T1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="K2" t="s">
+        <v>3</v>
+      </c>
+      <c r="L2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="4" width="11.7109375" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" t="s">
+        <v>25</v>
+      </c>
+      <c r="P1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R1" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1" t="s">
+        <v>24</v>
+      </c>
+      <c r="T1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="K2" t="s">
+        <v>99</v>
+      </c>
+      <c r="L2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="4" width="11.7109375" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" t="s">
+        <v>25</v>
+      </c>
+      <c r="P1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R1" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1" t="s">
+        <v>24</v>
+      </c>
+      <c r="T1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="K2" t="s">
+        <v>99</v>
+      </c>
+      <c r="L2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12019,7 +12408,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:T3"/>
   <sheetViews>
@@ -12137,7 +12526,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:T3"/>
   <sheetViews>
@@ -12253,7 +12642,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12370,7 +12759,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12547,7 +12936,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12721,7 +13110,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T5"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Included more weapon types, fixed bugs
</commit_message>
<xml_diff>
--- a/Battle Log.xlsx
+++ b/Battle Log.xlsx
@@ -9,21 +9,21 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-120" windowWidth="20490" windowHeight="7785" tabRatio="838" firstSheet="19" activeTab="27"/>
+    <workbookView xWindow="0" yWindow="-120" windowWidth="20490" windowHeight="7785" tabRatio="838" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Players" sheetId="16" r:id="rId1"/>
     <sheet name="Single STR" sheetId="1" r:id="rId2"/>
     <sheet name="Ineffective" sheetId="29" r:id="rId3"/>
     <sheet name="Single AGL" sheetId="3" r:id="rId4"/>
-    <sheet name="Shield" sheetId="7" r:id="rId5"/>
-    <sheet name="Group MANA - PC" sheetId="9" r:id="rId6"/>
-    <sheet name="Group MANA - Enemy" sheetId="11" r:id="rId7"/>
-    <sheet name="Barrier" sheetId="24" r:id="rId8"/>
-    <sheet name="All Enemies - PC" sheetId="13" r:id="rId9"/>
-    <sheet name="All Enemies - Dead Test" sheetId="23" r:id="rId10"/>
-    <sheet name="All Enemies - Dead Test (2)" sheetId="34" r:id="rId11"/>
-    <sheet name="Static DMG" sheetId="14" r:id="rId12"/>
+    <sheet name="Bow" sheetId="40" r:id="rId5"/>
+    <sheet name="Shield" sheetId="7" r:id="rId6"/>
+    <sheet name="Group MANA - PC" sheetId="9" r:id="rId7"/>
+    <sheet name="Group MANA - Enemy" sheetId="11" r:id="rId8"/>
+    <sheet name="Barrier" sheetId="24" r:id="rId9"/>
+    <sheet name="All Enemies - PC" sheetId="13" r:id="rId10"/>
+    <sheet name="All Enemies - Dead Test" sheetId="23" r:id="rId11"/>
+    <sheet name="Single Gun" sheetId="14" r:id="rId12"/>
     <sheet name="Group Static" sheetId="15" r:id="rId13"/>
     <sheet name="O-Weapon" sheetId="20" r:id="rId14"/>
     <sheet name="PC Cure - Magic" sheetId="17" r:id="rId15"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="918" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="839" uniqueCount="100">
   <si>
     <t>NAME</t>
   </si>
@@ -261,9 +261,6 @@
     <t>Flame Sword</t>
   </si>
   <si>
-    <t>MAGI</t>
-  </si>
-  <si>
     <t>INVENTORY</t>
   </si>
   <si>
@@ -330,12 +327,6 @@
     <t>Natural MANA</t>
   </si>
   <si>
-    <t>nan</t>
-  </si>
-  <si>
-    <t>n</t>
-  </si>
-  <si>
     <t>WereWolf</t>
   </si>
   <si>
@@ -349,6 +340,15 @@
   </si>
   <si>
     <t>Katana</t>
+  </si>
+  <si>
+    <t>Bow</t>
+  </si>
+  <si>
+    <t>EQUIPPED MAGI</t>
+  </si>
+  <si>
+    <t>OTHER MAGI</t>
   </si>
 </sst>
 </file>
@@ -8500,10 +8500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W12"/>
+  <dimension ref="A1:X12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="V7" sqref="V7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8518,12 +8518,12 @@
     <col min="17" max="17" width="9.140625" style="1"/>
     <col min="18" max="18" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="19" max="21" width="9.140625" style="1"/>
-    <col min="22" max="22" width="20.28515625" style="1" customWidth="1"/>
-    <col min="23" max="23" width="23.42578125" style="1" customWidth="1"/>
-    <col min="24" max="16384" width="9.140625" style="1"/>
+    <col min="22" max="23" width="20.28515625" style="1" customWidth="1"/>
+    <col min="24" max="24" width="23.42578125" style="1" customWidth="1"/>
+    <col min="25" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>20</v>
       </c>
@@ -8540,25 +8540,25 @@
         <v>49</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G1" s="18" t="s">
         <v>48</v>
       </c>
       <c r="H1" s="16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I1" s="18" t="s">
         <v>47</v>
       </c>
       <c r="J1" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K1" s="18" t="s">
         <v>46</v>
       </c>
       <c r="L1" s="16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="M1" s="18" t="s">
         <v>45</v>
@@ -8587,14 +8587,17 @@
       <c r="U1" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="V1" s="17" t="s">
+      <c r="V1" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="W1" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="X1" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="W1" s="17" t="s">
-        <v>71</v>
-      </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="str">
         <f t="shared" ref="A2:A12" si="0">B2</f>
         <v>HUME</v>
@@ -8603,7 +8606,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E2" s="1">
         <v>59</v>
@@ -8647,7 +8650,7 @@
       </c>
       <c r="Q2" s="13"/>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="str">
         <f t="shared" si="0"/>
         <v>MUTE</v>
@@ -8656,7 +8659,7 @@
         <v>6</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E3" s="1">
         <v>45</v>
@@ -8693,7 +8696,7 @@
         <v>35</v>
       </c>
       <c r="O3" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="R3" s="1" t="s">
         <v>56</v>
@@ -8701,8 +8704,11 @@
       <c r="S3" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="T3" s="21" t="s">
+        <v>97</v>
+      </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="str">
         <f t="shared" si="0"/>
         <v>MONS</v>
@@ -8711,7 +8717,7 @@
         <v>2</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E4" s="1">
         <v>45</v>
@@ -8754,7 +8760,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ROBO</v>
@@ -8803,10 +8809,10 @@
         <v>57</v>
       </c>
       <c r="P5" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Zappo</v>
@@ -8815,7 +8821,7 @@
         <v>30</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E6" s="1">
         <v>200</v>
@@ -8864,10 +8870,10 @@
         <v>64</v>
       </c>
       <c r="S6" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Flammie</v>
@@ -8876,7 +8882,7 @@
         <v>34</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E7" s="1">
         <v>999</v>
@@ -8919,7 +8925,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Slashy</v>
@@ -8928,7 +8934,7 @@
         <v>68</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E8" s="1">
         <v>400</v>
@@ -8965,19 +8971,19 @@
         <v>69</v>
       </c>
       <c r="O8" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Revenge</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E9" s="1">
         <v>100</v>
@@ -9011,19 +9017,19 @@
         <v>3</v>
       </c>
       <c r="N9" s="13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Turtle1</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E10" s="1">
         <v>100</v>
@@ -9057,19 +9063,19 @@
         <v>10</v>
       </c>
       <c r="N10" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Turtle2</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E11" s="1">
         <v>100</v>
@@ -9103,19 +9109,19 @@
         <v>10</v>
       </c>
       <c r="N11" s="14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Leonardo</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D12" s="21" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E12" s="1">
         <v>250</v>
@@ -9148,13 +9154,13 @@
         <v>11</v>
       </c>
       <c r="N12" s="21" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="O12" s="21" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="P12" s="21" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -9290,7 +9296,7 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>67</v>
+        <v>27</v>
       </c>
       <c r="B5" t="s">
         <v>19</v>
@@ -9306,7 +9312,7 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T14"/>
+  <dimension ref="A1:T5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="P1" sqref="P1:P1048576"/>
@@ -9398,590 +9404,41 @@
       <c r="D2">
         <v>1</v>
       </c>
-      <c r="E2">
-        <v>54</v>
-      </c>
-      <c r="F2">
-        <v>999</v>
-      </c>
-      <c r="G2">
-        <v>2</v>
-      </c>
-      <c r="H2">
-        <v>50</v>
-      </c>
-      <c r="I2">
-        <v>10</v>
-      </c>
-      <c r="J2">
-        <v>99</v>
-      </c>
       <c r="K2" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>19</v>
       </c>
       <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
         <v>4</v>
-      </c>
-      <c r="E3">
-        <v>6.25</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>6</v>
-      </c>
-      <c r="H3">
-        <v>5</v>
-      </c>
-      <c r="I3">
-        <v>3</v>
-      </c>
-      <c r="J3">
-        <v>5</v>
-      </c>
-      <c r="K3" t="s">
-        <v>93</v>
-      </c>
-      <c r="N3" t="s">
-        <v>94</v>
-      </c>
-      <c r="O3" t="s">
-        <v>94</v>
-      </c>
-      <c r="P3" t="s">
-        <v>94</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>94</v>
-      </c>
-      <c r="R3" t="s">
-        <v>94</v>
-      </c>
-      <c r="S3" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>67</v>
+        <v>28</v>
       </c>
       <c r="B4" t="s">
         <v>19</v>
       </c>
       <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-      <c r="E4">
-        <v>6.05</v>
-      </c>
-      <c r="F4">
-        <v>68.52000000000001</v>
-      </c>
-      <c r="G4">
-        <v>5</v>
-      </c>
-      <c r="H4">
-        <v>5</v>
-      </c>
-      <c r="I4">
-        <v>2</v>
-      </c>
-      <c r="J4">
-        <v>6</v>
-      </c>
-      <c r="K4" t="s">
-        <v>93</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>67</v>
       </c>
       <c r="B5" t="s">
         <v>19</v>
       </c>
       <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>2</v>
-      </c>
-      <c r="E5">
-        <v>6</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>6</v>
-      </c>
-      <c r="H5">
-        <v>5</v>
-      </c>
-      <c r="I5">
-        <v>3</v>
-      </c>
-      <c r="J5">
-        <v>5</v>
-      </c>
-      <c r="K5" t="s">
-        <v>93</v>
-      </c>
-      <c r="N5" t="s">
-        <v>94</v>
-      </c>
-      <c r="O5" t="s">
-        <v>94</v>
-      </c>
-      <c r="P5" t="s">
-        <v>94</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>94</v>
-      </c>
-      <c r="R5" t="s">
-        <v>94</v>
-      </c>
-      <c r="S5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>67</v>
-      </c>
-      <c r="B6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6">
-        <v>3</v>
-      </c>
-      <c r="E6">
-        <v>5.6499999999999986</v>
-      </c>
-      <c r="F6">
-        <v>68.52000000000001</v>
-      </c>
-      <c r="G6">
-        <v>5</v>
-      </c>
-      <c r="H6">
-        <v>5</v>
-      </c>
-      <c r="I6">
-        <v>2</v>
-      </c>
-      <c r="J6">
-        <v>6</v>
-      </c>
-      <c r="K6" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>67</v>
-      </c>
-      <c r="B7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7">
         <v>4</v>
-      </c>
-      <c r="E7">
-        <v>5.5500000000000007</v>
-      </c>
-      <c r="F7">
-        <v>68.52000000000001</v>
-      </c>
-      <c r="G7">
-        <v>5</v>
-      </c>
-      <c r="H7">
-        <v>5</v>
-      </c>
-      <c r="I7">
-        <v>2</v>
-      </c>
-      <c r="J7">
-        <v>6</v>
-      </c>
-      <c r="K7" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>67</v>
-      </c>
-      <c r="B8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8">
-        <v>5.4</v>
-      </c>
-      <c r="F8">
-        <v>68.52000000000001</v>
-      </c>
-      <c r="G8">
-        <v>5</v>
-      </c>
-      <c r="H8">
-        <v>5</v>
-      </c>
-      <c r="I8">
-        <v>2</v>
-      </c>
-      <c r="J8">
-        <v>6</v>
-      </c>
-      <c r="K8" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9">
-        <v>5.3000000000000007</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>6</v>
-      </c>
-      <c r="H9">
-        <v>5</v>
-      </c>
-      <c r="I9">
-        <v>3</v>
-      </c>
-      <c r="J9">
-        <v>5</v>
-      </c>
-      <c r="K9" t="s">
-        <v>93</v>
-      </c>
-      <c r="N9" t="s">
-        <v>94</v>
-      </c>
-      <c r="O9" t="s">
-        <v>94</v>
-      </c>
-      <c r="P9" t="s">
-        <v>94</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>94</v>
-      </c>
-      <c r="R9" t="s">
-        <v>94</v>
-      </c>
-      <c r="S9" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>3</v>
-      </c>
-      <c r="E10">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>6</v>
-      </c>
-      <c r="H10">
-        <v>5</v>
-      </c>
-      <c r="I10">
-        <v>3</v>
-      </c>
-      <c r="J10">
-        <v>5</v>
-      </c>
-      <c r="K10" t="s">
-        <v>93</v>
-      </c>
-      <c r="N10" t="s">
-        <v>94</v>
-      </c>
-      <c r="O10" t="s">
-        <v>94</v>
-      </c>
-      <c r="P10" t="s">
-        <v>94</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>94</v>
-      </c>
-      <c r="R10" t="s">
-        <v>94</v>
-      </c>
-      <c r="S10" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11">
-        <v>4.68</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <v>7</v>
-      </c>
-      <c r="H11">
-        <v>4</v>
-      </c>
-      <c r="I11">
-        <v>5</v>
-      </c>
-      <c r="J11">
-        <v>5</v>
-      </c>
-      <c r="K11" t="s">
-        <v>93</v>
-      </c>
-      <c r="N11" t="s">
-        <v>94</v>
-      </c>
-      <c r="O11" t="s">
-        <v>94</v>
-      </c>
-      <c r="P11" t="s">
-        <v>94</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>94</v>
-      </c>
-      <c r="R11" t="s">
-        <v>94</v>
-      </c>
-      <c r="S11" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>4</v>
-      </c>
-      <c r="E12">
-        <v>4.4800000000000004</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-      <c r="G12">
-        <v>7</v>
-      </c>
-      <c r="H12">
-        <v>4</v>
-      </c>
-      <c r="I12">
-        <v>5</v>
-      </c>
-      <c r="J12">
-        <v>5</v>
-      </c>
-      <c r="K12" t="s">
-        <v>93</v>
-      </c>
-      <c r="N12" t="s">
-        <v>94</v>
-      </c>
-      <c r="O12" t="s">
-        <v>94</v>
-      </c>
-      <c r="P12" t="s">
-        <v>94</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>94</v>
-      </c>
-      <c r="R12" t="s">
-        <v>94</v>
-      </c>
-      <c r="S12" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>2</v>
-      </c>
-      <c r="E13">
-        <v>4.12</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="G13">
-        <v>7</v>
-      </c>
-      <c r="H13">
-        <v>4</v>
-      </c>
-      <c r="I13">
-        <v>5</v>
-      </c>
-      <c r="J13">
-        <v>5</v>
-      </c>
-      <c r="K13" t="s">
-        <v>93</v>
-      </c>
-      <c r="N13" t="s">
-        <v>94</v>
-      </c>
-      <c r="O13" t="s">
-        <v>94</v>
-      </c>
-      <c r="P13" t="s">
-        <v>94</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>94</v>
-      </c>
-      <c r="R13" t="s">
-        <v>94</v>
-      </c>
-      <c r="S13" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-      <c r="D14">
-        <v>3</v>
-      </c>
-      <c r="E14">
-        <v>4.04</v>
-      </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-      <c r="G14">
-        <v>7</v>
-      </c>
-      <c r="H14">
-        <v>4</v>
-      </c>
-      <c r="I14">
-        <v>5</v>
-      </c>
-      <c r="J14">
-        <v>5</v>
-      </c>
-      <c r="K14" t="s">
-        <v>93</v>
-      </c>
-      <c r="N14" t="s">
-        <v>94</v>
-      </c>
-      <c r="O14" t="s">
-        <v>94</v>
-      </c>
-      <c r="P14" t="s">
-        <v>94</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>94</v>
-      </c>
-      <c r="R14" t="s">
-        <v>94</v>
-      </c>
-      <c r="S14" t="s">
-        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -10971,7 +10428,7 @@
         <v>1</v>
       </c>
       <c r="K2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L2" t="s">
         <v>4</v>
@@ -11230,7 +10687,7 @@
         <v>53</v>
       </c>
       <c r="L2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
@@ -11250,7 +10707,7 @@
         <v>29</v>
       </c>
       <c r="L3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
@@ -11270,7 +10727,7 @@
         <v>3</v>
       </c>
       <c r="L4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
@@ -11290,12 +10747,12 @@
         <v>58</v>
       </c>
       <c r="L5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B6" t="s">
         <v>19</v>
@@ -11521,15 +10978,15 @@
         <v>1</v>
       </c>
       <c r="K2" t="s">
+        <v>71</v>
+      </c>
+      <c r="L2" t="s">
         <v>72</v>
-      </c>
-      <c r="L2" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B3" t="s">
         <v>19</v>
@@ -11638,7 +11095,7 @@
         <v>1</v>
       </c>
       <c r="K2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
@@ -11741,7 +11198,7 @@
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
@@ -11753,7 +11210,7 @@
         <v>1</v>
       </c>
       <c r="K2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
@@ -11856,7 +11313,7 @@
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
@@ -11868,7 +11325,7 @@
         <v>1</v>
       </c>
       <c r="K2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
@@ -11884,7 +11341,7 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
@@ -11896,7 +11353,7 @@
         <v>2</v>
       </c>
       <c r="K4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -12003,12 +11460,12 @@
         <v>3</v>
       </c>
       <c r="L2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B3" t="s">
         <v>19</v>
@@ -12106,7 +11563,7 @@
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
@@ -12118,7 +11575,7 @@
         <v>1</v>
       </c>
       <c r="K2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="L2" t="s">
         <v>4</v>
@@ -12144,7 +11601,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
@@ -12224,7 +11681,7 @@
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
@@ -12236,15 +11693,15 @@
         <v>1</v>
       </c>
       <c r="K2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="L2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B3" t="s">
         <v>19</v>
@@ -12527,6 +11984,123 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" t="s">
+        <v>25</v>
+      </c>
+      <c r="P1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R1" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1" t="s">
+        <v>24</v>
+      </c>
+      <c r="T1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="K2" t="s">
+        <v>97</v>
+      </c>
+      <c r="L2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:T3"/>
   <sheetViews>
@@ -12641,7 +12215,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T3"/>
   <sheetViews>
@@ -12758,12 +12332,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P1" sqref="P1:P1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -12935,7 +12509,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T6"/>
   <sheetViews>
@@ -13107,140 +12681,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P1" sqref="P1:P1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L1" t="s">
-        <v>16</v>
-      </c>
-      <c r="M1" t="s">
-        <v>26</v>
-      </c>
-      <c r="N1" t="s">
-        <v>21</v>
-      </c>
-      <c r="O1" t="s">
-        <v>25</v>
-      </c>
-      <c r="P1" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>22</v>
-      </c>
-      <c r="R1" t="s">
-        <v>23</v>
-      </c>
-      <c r="S1" t="s">
-        <v>24</v>
-      </c>
-      <c r="T1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="K2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5">
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Refactoring to support MAGI inclusion
Append MAGI to skills list for PCs
Built new functions for each Actor subclass: getAgility, getStrength, getDefense, getMana
Refactored everything to use the new functions
Added MAGI calculations for stats and elements
</commit_message>
<xml_diff>
--- a/Battle Log.xlsx
+++ b/Battle Log.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-120" windowWidth="20490" windowHeight="7785" tabRatio="838" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="-120" windowWidth="20490" windowHeight="7785" tabRatio="838"/>
   </bookViews>
   <sheets>
     <sheet name="Players" sheetId="16" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="839" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="105">
   <si>
     <t>NAME</t>
   </si>
@@ -350,6 +350,21 @@
   <si>
     <t>OTHER MAGI</t>
   </si>
+  <si>
+    <t>Power-2, Fire-1</t>
+  </si>
+  <si>
+    <t>Cure Potion-3, Elixier</t>
+  </si>
+  <si>
+    <t>Mana Magi-2</t>
+  </si>
+  <si>
+    <t>Ice Magi-1</t>
+  </si>
+  <si>
+    <t>Fire Magi-1</t>
+  </si>
 </sst>
 </file>
 
@@ -580,9 +595,9 @@
       <sheetName val="Move Prob - %"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
       <sheetData sheetId="3">
         <row r="1">
           <cell r="A1" t="str">
@@ -8202,12 +8217,12 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -8502,7 +8517,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X12"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="V7" sqref="V7"/>
     </sheetView>
   </sheetViews>
@@ -8649,6 +8664,12 @@
         <v>55</v>
       </c>
       <c r="Q2" s="13"/>
+      <c r="W2" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="X2" s="21" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="str">
@@ -8707,6 +8728,10 @@
       <c r="T3" s="21" t="s">
         <v>97</v>
       </c>
+      <c r="V3" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="W3" s="21"/>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="str">
@@ -8872,6 +8897,10 @@
       <c r="S6" s="12" t="s">
         <v>81</v>
       </c>
+      <c r="V6" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="W6" s="21"/>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="str">
@@ -8923,6 +8952,9 @@
       </c>
       <c r="P7" s="3" t="s">
         <v>60</v>
+      </c>
+      <c r="V7" s="21" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
@@ -12336,7 +12368,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Absorb and Multi-hit Effects
</commit_message>
<xml_diff>
--- a/Battle Log.xlsx
+++ b/Battle Log.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Action IV\Documents\GitHub\pillar\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scrummel\source\repos\pillar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDD943F3-80E3-4420-ABEF-001E00D7E153}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="838" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="838" firstSheet="22" activeTab="27"/>
   </bookViews>
   <sheets>
     <sheet name="Players" sheetId="16" r:id="rId1"/>
@@ -38,22 +37,25 @@
     <sheet name="All Enemies - Status" sheetId="28" r:id="rId23"/>
     <sheet name="Weak - Elem Melee" sheetId="26" r:id="rId24"/>
     <sheet name="Weak - Race Melee" sheetId="27" r:id="rId25"/>
-    <sheet name="Reflect" sheetId="31" r:id="rId26"/>
-    <sheet name="STR Counter" sheetId="32" r:id="rId27"/>
-    <sheet name="Other Counters" sheetId="33" r:id="rId28"/>
-    <sheet name="Enemy Surprise" sheetId="36" r:id="rId29"/>
-    <sheet name="Player Surprise" sheetId="37" r:id="rId30"/>
-    <sheet name="Both Surprise" sheetId="38" r:id="rId31"/>
+    <sheet name="Drain Reversal" sheetId="44" r:id="rId26"/>
+    <sheet name="Drain Success" sheetId="45" r:id="rId27"/>
+    <sheet name="Multi-hit" sheetId="46" r:id="rId28"/>
+    <sheet name="Reflect" sheetId="31" r:id="rId29"/>
+    <sheet name="STR Counter" sheetId="32" r:id="rId30"/>
+    <sheet name="Other Counters" sheetId="33" r:id="rId31"/>
+    <sheet name="Enemy Surprise" sheetId="36" r:id="rId32"/>
+    <sheet name="Player Surprise" sheetId="37" r:id="rId33"/>
+    <sheet name="Both Surprise" sheetId="38" r:id="rId34"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId32"/>
+    <externalReference r:id="rId35"/>
   </externalReferences>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="938" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1018" uniqueCount="124">
   <si>
     <t>NAME</t>
   </si>
@@ -417,11 +419,20 @@
   <si>
     <t>Recover</t>
   </si>
+  <si>
+    <t>Vampic Sword</t>
+  </si>
+  <si>
+    <t>Seven Sword</t>
+  </si>
+  <si>
+    <t>Crab</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -618,7 +629,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -662,9 +673,9 @@
       <sheetName val="Move Prob - %"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
       <sheetData sheetId="3">
         <row r="1">
           <cell r="A1" t="str">
@@ -8284,12 +8295,12 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -8371,23 +8382,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -8423,23 +8417,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -8615,11 +8592,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9097,17 +9074,23 @@
         <v>25</v>
       </c>
       <c r="L8" s="1">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="M8" s="19">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="N8" s="7" t="s">
         <v>69</v>
       </c>
       <c r="O8" s="8" t="s">
         <v>71</v>
+      </c>
+      <c r="P8" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q8" s="22" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
@@ -9434,7 +9417,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9551,7 +9534,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9728,7 +9711,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9902,7 +9885,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10038,7 +10021,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10174,7 +10157,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10292,7 +10275,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10409,7 +10392,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10526,7 +10509,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10666,7 +10649,7 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10806,7 +10789,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:T4"/>
   <sheetViews>
@@ -10945,7 +10928,7 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11083,7 +11066,7 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11200,7 +11183,7 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11317,7 +11300,7 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11494,7 +11477,7 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11611,7 +11594,7 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11728,7 +11711,358 @@
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" t="s">
+        <v>25</v>
+      </c>
+      <c r="P1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R1" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1" t="s">
+        <v>24</v>
+      </c>
+      <c r="T1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="K2" t="s">
+        <v>121</v>
+      </c>
+      <c r="L2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" t="s">
+        <v>25</v>
+      </c>
+      <c r="P1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R1" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1" t="s">
+        <v>24</v>
+      </c>
+      <c r="T1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="K2" t="s">
+        <v>121</v>
+      </c>
+      <c r="L2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" t="s">
+        <v>25</v>
+      </c>
+      <c r="P1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R1" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1" t="s">
+        <v>24</v>
+      </c>
+      <c r="T1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="K2" t="s">
+        <v>122</v>
+      </c>
+      <c r="L2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11841,8 +12175,157 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P1" sqref="P1:P1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="4" width="11.7109375" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" t="s">
+        <v>25</v>
+      </c>
+      <c r="P1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R1" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1" t="s">
+        <v>24</v>
+      </c>
+      <c r="T1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="K2" t="s">
+        <v>69</v>
+      </c>
+      <c r="L2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="K3" t="s">
+        <v>3</v>
+      </c>
+      <c r="L3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11956,8 +12439,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12088,8 +12571,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12206,157 +12689,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:T5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P1" sqref="P1:P1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="3" max="4" width="11.7109375" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L1" t="s">
-        <v>16</v>
-      </c>
-      <c r="M1" t="s">
-        <v>26</v>
-      </c>
-      <c r="N1" t="s">
-        <v>21</v>
-      </c>
-      <c r="O1" t="s">
-        <v>25</v>
-      </c>
-      <c r="P1" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>22</v>
-      </c>
-      <c r="R1" t="s">
-        <v>23</v>
-      </c>
-      <c r="S1" t="s">
-        <v>24</v>
-      </c>
-      <c r="T1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>2</v>
-      </c>
-      <c r="K2" t="s">
-        <v>69</v>
-      </c>
-      <c r="L2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="K3" t="s">
-        <v>3</v>
-      </c>
-      <c r="L3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12473,8 +12807,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12592,7 +12926,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2167536-BCD6-4485-BB27-1A881AF06677}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12710,7 +13044,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F613FB1-311D-44AF-A16D-7121D97D052A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12825,7 +13159,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:T3"/>
   <sheetViews>
@@ -12943,7 +13277,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A425FDE-C9EC-4D06-BAAE-85C83CB3C979}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13060,7 +13394,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13177,7 +13511,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:T3"/>
   <sheetViews>

</xml_diff>

<commit_message>
Buff, Debuff, Cut effects working
new bug with ally / allies targeting around ignoring the dead
</commit_message>
<xml_diff>
--- a/Battle Log.xlsx
+++ b/Battle Log.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="838" firstSheet="22" activeTab="27"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="838" firstSheet="27" activeTab="37"/>
   </bookViews>
   <sheets>
     <sheet name="Players" sheetId="16" r:id="rId1"/>
@@ -40,22 +40,26 @@
     <sheet name="Drain Reversal" sheetId="44" r:id="rId26"/>
     <sheet name="Drain Success" sheetId="45" r:id="rId27"/>
     <sheet name="Multi-hit" sheetId="46" r:id="rId28"/>
-    <sheet name="Reflect" sheetId="31" r:id="rId29"/>
-    <sheet name="STR Counter" sheetId="32" r:id="rId30"/>
-    <sheet name="Other Counters" sheetId="33" r:id="rId31"/>
-    <sheet name="Enemy Surprise" sheetId="36" r:id="rId32"/>
-    <sheet name="Player Surprise" sheetId="37" r:id="rId33"/>
-    <sheet name="Both Surprise" sheetId="38" r:id="rId34"/>
+    <sheet name="Buff and Debuff" sheetId="47" r:id="rId29"/>
+    <sheet name="Reflect" sheetId="31" r:id="rId30"/>
+    <sheet name="STR Counter" sheetId="32" r:id="rId31"/>
+    <sheet name="Other Counters" sheetId="33" r:id="rId32"/>
+    <sheet name="ChainSaw" sheetId="48" r:id="rId33"/>
+    <sheet name="Enemy Surprise" sheetId="36" r:id="rId34"/>
+    <sheet name="Player Surprise" sheetId="37" r:id="rId35"/>
+    <sheet name="Both Surprise" sheetId="38" r:id="rId36"/>
+    <sheet name="Run" sheetId="49" r:id="rId37"/>
+    <sheet name="Heart" sheetId="50" r:id="rId38"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId35"/>
+    <externalReference r:id="rId39"/>
   </externalReferences>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1018" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1140" uniqueCount="130">
   <si>
     <t>NAME</t>
   </si>
@@ -428,6 +432,24 @@
   <si>
     <t>Crab</t>
   </si>
+  <si>
+    <t>Haste</t>
+  </si>
+  <si>
+    <t>Cobble</t>
+  </si>
+  <si>
+    <t>ChainSaw</t>
+  </si>
+  <si>
+    <t>Run</t>
+  </si>
+  <si>
+    <t>NPC</t>
+  </si>
+  <si>
+    <t>Heart Magi</t>
+  </si>
 </sst>
 </file>
 
@@ -673,9 +695,9 @@
       <sheetName val="Move Prob - %"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
       <sheetData sheetId="3">
         <row r="1">
           <cell r="A1" t="str">
@@ -5730,10 +5752,10 @@
         </row>
         <row r="164">
           <cell r="A164" t="str">
-            <v>MegaCure</v>
+            <v>Life</v>
           </cell>
           <cell r="B164" t="str">
-            <v>MegaCure</v>
+            <v>Life</v>
           </cell>
           <cell r="C164" t="str">
             <v>Life</v>
@@ -8295,12 +8317,12 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -8596,7 +8618,7 @@
   <dimension ref="A1:X14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q9" sqref="Q9"/>
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8741,7 +8763,7 @@
       <c r="P2" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="Q2" s="13"/>
+      <c r="Q2" s="22"/>
       <c r="W2" s="20" t="s">
         <v>100</v>
       </c>
@@ -9138,6 +9160,9 @@
       <c r="N9" s="13" t="s">
         <v>82</v>
       </c>
+      <c r="O9" s="22" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="str">
@@ -9281,6 +9306,9 @@
       </c>
       <c r="P12" s="20" t="s">
         <v>95</v>
+      </c>
+      <c r="Q12" s="22" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
@@ -11948,7 +11976,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
@@ -12066,7 +12094,7 @@
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P1" sqref="P1:P1048576"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -12144,7 +12172,7 @@
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>93</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
@@ -12156,18 +12184,18 @@
         <v>1</v>
       </c>
       <c r="K2" t="s">
-        <v>80</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>125</v>
       </c>
       <c r="B3" t="s">
         <v>19</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -12334,6 +12362,120 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" t="s">
+        <v>25</v>
+      </c>
+      <c r="P1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R1" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1" t="s">
+        <v>24</v>
+      </c>
+      <c r="T1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="K2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P1" sqref="P1:P1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
     <col min="3" max="4" width="11.7109375" customWidth="1"/>
     <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
@@ -12439,7 +12581,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T4"/>
   <sheetViews>
@@ -12564,124 +12706,6 @@
       </c>
       <c r="K4" t="s">
         <v>87</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="3" max="4" width="11.7109375" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L1" t="s">
-        <v>16</v>
-      </c>
-      <c r="M1" t="s">
-        <v>26</v>
-      </c>
-      <c r="N1" t="s">
-        <v>21</v>
-      </c>
-      <c r="O1" t="s">
-        <v>25</v>
-      </c>
-      <c r="P1" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>22</v>
-      </c>
-      <c r="R1" t="s">
-        <v>23</v>
-      </c>
-      <c r="S1" t="s">
-        <v>24</v>
-      </c>
-      <c r="T1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="K2" t="s">
-        <v>3</v>
-      </c>
-      <c r="L2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>92</v>
-      </c>
-      <c r="B3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -12773,7 +12797,7 @@
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
@@ -12785,7 +12809,7 @@
         <v>1</v>
       </c>
       <c r="K2" t="s">
-        <v>96</v>
+        <v>126</v>
       </c>
       <c r="L2" t="s">
         <v>4</v>
@@ -12799,7 +12823,7 @@
         <v>19</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -12891,7 +12915,7 @@
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>93</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
@@ -12903,7 +12927,7 @@
         <v>1</v>
       </c>
       <c r="K2" t="s">
-        <v>96</v>
+        <v>3</v>
       </c>
       <c r="L2" t="s">
         <v>92</v>
@@ -12918,6 +12942,568 @@
       </c>
       <c r="C3">
         <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="4" width="11.7109375" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" t="s">
+        <v>25</v>
+      </c>
+      <c r="P1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R1" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1" t="s">
+        <v>24</v>
+      </c>
+      <c r="T1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="K2" t="s">
+        <v>96</v>
+      </c>
+      <c r="L2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="4" width="11.7109375" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" t="s">
+        <v>25</v>
+      </c>
+      <c r="P1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R1" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1" t="s">
+        <v>24</v>
+      </c>
+      <c r="T1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="K2" t="s">
+        <v>96</v>
+      </c>
+      <c r="L2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="4" width="11.7109375" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" t="s">
+        <v>25</v>
+      </c>
+      <c r="P1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R1" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1" t="s">
+        <v>24</v>
+      </c>
+      <c r="T1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="K2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="K3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" t="s">
+        <v>25</v>
+      </c>
+      <c r="P1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R1" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1" t="s">
+        <v>24</v>
+      </c>
+      <c r="T1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="K2" t="s">
+        <v>53</v>
+      </c>
+      <c r="L2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="K3" t="s">
+        <v>29</v>
+      </c>
+      <c r="L3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="K4" t="s">
+        <v>3</v>
+      </c>
+      <c r="L4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="K5" t="s">
+        <v>58</v>
+      </c>
+      <c r="L5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>105</v>
+      </c>
+      <c r="B6" t="s">
+        <v>128</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="K6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Began postBattle and finished MAGI
Fixed Actions Taken by making it a string
Started post battle calculations
Changed ally targeting to look for the dead or petrified when appropriate
Fixed ordering bug (again)
</commit_message>
<xml_diff>
--- a/Battle Log.xlsx
+++ b/Battle Log.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scrummel\source\repos\pillar\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Action IV\Documents\GitHub\pillar\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A4FA8AC-6485-4962-8C3B-338EB00625AA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="838" firstSheet="27" activeTab="37"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="838" firstSheet="12" activeTab="23" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Players" sheetId="16" r:id="rId1"/>
@@ -35,31 +36,32 @@
     <sheet name="Status Effect" sheetId="21" r:id="rId21"/>
     <sheet name="Group Status" sheetId="22" r:id="rId22"/>
     <sheet name="All Enemies - Status" sheetId="28" r:id="rId23"/>
-    <sheet name="Weak - Elem Melee" sheetId="26" r:id="rId24"/>
-    <sheet name="Weak - Race Melee" sheetId="27" r:id="rId25"/>
-    <sheet name="Drain Reversal" sheetId="44" r:id="rId26"/>
-    <sheet name="Drain Success" sheetId="45" r:id="rId27"/>
-    <sheet name="Multi-hit" sheetId="46" r:id="rId28"/>
-    <sheet name="Buff and Debuff" sheetId="47" r:id="rId29"/>
-    <sheet name="Reflect" sheetId="31" r:id="rId30"/>
-    <sheet name="STR Counter" sheetId="32" r:id="rId31"/>
-    <sheet name="Other Counters" sheetId="33" r:id="rId32"/>
-    <sheet name="ChainSaw" sheetId="48" r:id="rId33"/>
-    <sheet name="Enemy Surprise" sheetId="36" r:id="rId34"/>
-    <sheet name="Player Surprise" sheetId="37" r:id="rId35"/>
-    <sheet name="Both Surprise" sheetId="38" r:id="rId36"/>
-    <sheet name="Run" sheetId="49" r:id="rId37"/>
-    <sheet name="Heart" sheetId="50" r:id="rId38"/>
+    <sheet name="Confuse Enemies" sheetId="51" r:id="rId24"/>
+    <sheet name="Weak - Elem Melee" sheetId="26" r:id="rId25"/>
+    <sheet name="Weak - Race Melee" sheetId="27" r:id="rId26"/>
+    <sheet name="Drain Reversal" sheetId="44" r:id="rId27"/>
+    <sheet name="Drain Success" sheetId="45" r:id="rId28"/>
+    <sheet name="Multi-hit" sheetId="46" r:id="rId29"/>
+    <sheet name="Buff and Debuff" sheetId="47" r:id="rId30"/>
+    <sheet name="Reflect" sheetId="31" r:id="rId31"/>
+    <sheet name="STR Counter" sheetId="32" r:id="rId32"/>
+    <sheet name="Other Counters" sheetId="33" r:id="rId33"/>
+    <sheet name="ChainSaw" sheetId="48" r:id="rId34"/>
+    <sheet name="Enemy Surprise" sheetId="36" r:id="rId35"/>
+    <sheet name="Player Surprise" sheetId="37" r:id="rId36"/>
+    <sheet name="Both Surprise" sheetId="38" r:id="rId37"/>
+    <sheet name="Run" sheetId="49" r:id="rId38"/>
+    <sheet name="Heart" sheetId="50" r:id="rId39"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId39"/>
+    <externalReference r:id="rId40"/>
   </externalReferences>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1140" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1190" uniqueCount="149">
   <si>
     <t>NAME</t>
   </si>
@@ -449,18 +451,82 @@
   </si>
   <si>
     <t>Heart Magi</t>
+  </si>
+  <si>
+    <t>S0 Uses Left</t>
+  </si>
+  <si>
+    <t>MAGI Uses Left</t>
+  </si>
+  <si>
+    <t>S1 Uses Left</t>
+  </si>
+  <si>
+    <t>S2 Uses Left</t>
+  </si>
+  <si>
+    <t>S3 Uses Left</t>
+  </si>
+  <si>
+    <t>S4 Uses Left</t>
+  </si>
+  <si>
+    <t>S5 Uses Left</t>
+  </si>
+  <si>
+    <t>S6 Uses Left</t>
+  </si>
+  <si>
+    <t>S7 Uses Left</t>
+  </si>
+  <si>
+    <t>HypnoToad</t>
+  </si>
+  <si>
+    <t>Tongue</t>
+  </si>
+  <si>
+    <t>Kick</t>
+  </si>
+  <si>
+    <t>Tie Up</t>
+  </si>
+  <si>
+    <t>Gas</t>
+  </si>
+  <si>
+    <t>MadSong</t>
+  </si>
+  <si>
+    <t>CursSong</t>
+  </si>
+  <si>
+    <t>O-Poison</t>
+  </si>
+  <si>
+    <t>Thunder</t>
+  </si>
+  <si>
+    <t>Haste, Haste</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="19" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -603,7 +669,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -611,47 +677,104 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -695,9 +818,9 @@
       <sheetName val="Move Prob - %"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
       <sheetData sheetId="3">
         <row r="1">
           <cell r="A1" t="str">
@@ -8316,13 +8439,21 @@
             <v>O</v>
           </cell>
         </row>
+        <row r="259">
+          <cell r="A259" t="str">
+            <v>Tremor</v>
+          </cell>
+          <cell r="B259" t="str">
+            <v>Tremor</v>
+          </cell>
+        </row>
       </sheetData>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -8404,6 +8535,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -8439,6 +8587,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -8614,11 +8779,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AG15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8628,93 +8793,133 @@
     <col min="3" max="3" width="9.140625" style="1"/>
     <col min="4" max="4" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="13" width="9.140625" style="1"/>
-    <col min="14" max="14" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.140625" style="1"/>
-    <col min="18" max="18" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="21" width="9.140625" style="1"/>
-    <col min="22" max="23" width="20.28515625" style="1" customWidth="1"/>
-    <col min="24" max="24" width="23.42578125" style="1" customWidth="1"/>
-    <col min="25" max="16384" width="9.140625" style="1"/>
+    <col min="14" max="14" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.7109375" style="1" customWidth="1"/>
+    <col min="16" max="16" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.7109375" style="1" customWidth="1"/>
+    <col min="18" max="18" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.7109375" style="1" customWidth="1"/>
+    <col min="20" max="20" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.7109375" style="1" customWidth="1"/>
+    <col min="22" max="22" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.7109375" style="1" customWidth="1"/>
+    <col min="24" max="24" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="7.7109375" style="1" customWidth="1"/>
+    <col min="26" max="26" width="9.140625" style="1"/>
+    <col min="27" max="27" width="7.7109375" style="1" customWidth="1"/>
+    <col min="28" max="28" width="9.140625" style="1"/>
+    <col min="29" max="29" width="7.7109375" style="1" customWidth="1"/>
+    <col min="30" max="30" width="20.28515625" style="1" customWidth="1"/>
+    <col min="31" max="31" width="7.7109375" style="1" customWidth="1"/>
+    <col min="32" max="32" width="20.28515625" style="1" customWidth="1"/>
+    <col min="33" max="33" width="23.42578125" style="1" customWidth="1"/>
+    <col min="34" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" s="15" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="41" t="s">
         <v>88</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="41" t="s">
         <v>89</v>
       </c>
-      <c r="I1" s="18" t="s">
+      <c r="I1" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="J1" s="16" t="s">
+      <c r="J1" s="41" t="s">
         <v>90</v>
       </c>
-      <c r="K1" s="18" t="s">
+      <c r="K1" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="L1" s="16" t="s">
+      <c r="L1" s="41" t="s">
         <v>91</v>
       </c>
-      <c r="M1" s="18" t="s">
+      <c r="M1" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="N1" s="15" t="s">
+      <c r="N1" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="O1" s="15" t="s">
+      <c r="O1" s="39" t="s">
+        <v>130</v>
+      </c>
+      <c r="P1" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="P1" s="15" t="s">
+      <c r="Q1" s="39" t="s">
+        <v>132</v>
+      </c>
+      <c r="R1" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="Q1" s="15" t="s">
+      <c r="S1" s="39" t="s">
+        <v>133</v>
+      </c>
+      <c r="T1" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="R1" s="15" t="s">
+      <c r="U1" s="39" t="s">
+        <v>134</v>
+      </c>
+      <c r="V1" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="S1" s="15" t="s">
+      <c r="W1" s="39" t="s">
+        <v>135</v>
+      </c>
+      <c r="X1" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="T1" s="15" t="s">
+      <c r="Y1" s="39" t="s">
+        <v>136</v>
+      </c>
+      <c r="Z1" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="U1" s="15" t="s">
+      <c r="AA1" s="39" t="s">
+        <v>137</v>
+      </c>
+      <c r="AB1" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="V1" s="16" t="s">
+      <c r="AC1" s="39" t="s">
+        <v>138</v>
+      </c>
+      <c r="AD1" s="36" t="s">
         <v>98</v>
       </c>
-      <c r="W1" s="16" t="s">
+      <c r="AE1" s="39" t="s">
+        <v>131</v>
+      </c>
+      <c r="AF1" s="36" t="s">
         <v>99</v>
       </c>
-      <c r="X1" s="17" t="s">
+      <c r="AG1" s="40" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="str">
-        <f t="shared" ref="A2:A14" si="0">B2</f>
+        <f t="shared" ref="A2:A15" si="0">B2</f>
         <v>HUME</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -8726,52 +8931,57 @@
       <c r="E2" s="1">
         <v>59</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2" s="20">
         <v>6</v>
       </c>
-      <c r="G2" s="19">
+      <c r="G2" s="16">
         <f>F2</f>
         <v>6</v>
       </c>
-      <c r="H2" s="1">
+      <c r="H2" s="20">
         <v>0</v>
       </c>
-      <c r="I2" s="19">
-        <f>H2+_xlfn.IFNA(VLOOKUP(N2,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(O2,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(P2,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(Q2,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(R2,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(S2,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(T2,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(U2,[1]Weapon!$A$1:$M$259,9,FALSE),0)</f>
+      <c r="I2" s="16">
+        <f>H2+_xlfn.IFNA(VLOOKUP(N2,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(P2,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(R2,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(T2,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(V2,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(X2,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(Z2,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(AB2,[1]Weapon!$A$1:$M$259,9,FALSE),0)</f>
         <v>3</v>
       </c>
-      <c r="J2" s="1">
+      <c r="J2" s="20">
         <v>5</v>
       </c>
-      <c r="K2" s="19">
+      <c r="K2" s="16">
         <f>J2</f>
         <v>5</v>
       </c>
-      <c r="L2" s="1">
+      <c r="L2" s="20">
         <v>3</v>
       </c>
-      <c r="M2" s="19">
+      <c r="M2" s="16">
         <f>L2</f>
         <v>3</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="N2" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="P2" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="R2" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="Q2" s="22"/>
-      <c r="W2" s="20" t="s">
+      <c r="T2" s="30"/>
+      <c r="U2" s="19"/>
+      <c r="V2" s="20"/>
+      <c r="X2" s="20"/>
+      <c r="Z2" s="20"/>
+      <c r="AB2" s="20"/>
+      <c r="AF2" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="X2" s="20" t="s">
+      <c r="AG2" s="17" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="str">
         <f t="shared" si="0"/>
         <v>MUTE</v>
@@ -8785,58 +8995,64 @@
       <c r="E3" s="1">
         <v>45</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3" s="20">
         <v>4</v>
       </c>
-      <c r="G3" s="19">
-        <f t="shared" ref="G3:G14" si="1">F3</f>
+      <c r="G3" s="16">
+        <f t="shared" ref="G3:G15" si="1">F3</f>
         <v>4</v>
       </c>
-      <c r="H3" s="1">
+      <c r="H3" s="20">
         <v>0</v>
       </c>
-      <c r="I3" s="19">
-        <f>H3+_xlfn.IFNA(VLOOKUP(N3,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(O3,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(P3,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(Q3,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(R3,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(S3,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(T3,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(U3,[1]Weapon!$A$1:$M$259,9,FALSE),0)</f>
+      <c r="I3" s="16">
+        <f>H3+_xlfn.IFNA(VLOOKUP(N3,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(P3,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(R3,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(T3,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(V3,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(X3,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(Z3,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(AB3,[1]Weapon!$A$1:$M$259,9,FALSE),0)</f>
         <v>13</v>
       </c>
-      <c r="J3" s="1">
+      <c r="J3" s="20">
         <v>5</v>
       </c>
-      <c r="K3" s="19">
-        <f t="shared" ref="K3:K14" si="2">J3</f>
+      <c r="K3" s="16">
+        <f t="shared" ref="K3:K15" si="2">J3</f>
         <v>5</v>
       </c>
-      <c r="L3" s="1">
+      <c r="L3" s="20">
         <v>6</v>
       </c>
-      <c r="M3" s="19">
-        <f t="shared" ref="M3:M14" si="3">L3</f>
+      <c r="M3" s="16">
+        <f t="shared" ref="M3:M15" si="3">L3</f>
         <v>6</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="N3" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="O3" s="12" t="s">
+      <c r="P3" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="R3" s="1" t="s">
+      <c r="Q3" s="12"/>
+      <c r="R3" s="20"/>
+      <c r="T3" s="20"/>
+      <c r="V3" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="S3" s="1" t="s">
+      <c r="X3" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="T3" s="20" t="s">
+      <c r="Z3" s="25" t="s">
         <v>97</v>
       </c>
-      <c r="U3" s="22" t="s">
+      <c r="AA3" s="17"/>
+      <c r="AB3" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="V3" s="20" t="s">
+      <c r="AC3" s="19"/>
+      <c r="AD3" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="W3" s="20"/>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="AE3" s="17"/>
+      <c r="AF3" s="17"/>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="str">
         <f t="shared" si="0"/>
         <v>MONS</v>
@@ -8850,45 +9066,51 @@
       <c r="E4" s="1">
         <v>45</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4" s="20">
         <v>5</v>
       </c>
-      <c r="G4" s="19">
+      <c r="G4" s="16">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="H4" s="1">
+      <c r="H4" s="20">
         <v>5</v>
       </c>
-      <c r="I4" s="19">
-        <f>H4+_xlfn.IFNA(VLOOKUP(N4,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(O4,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(P4,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(Q4,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(R4,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(S4,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(T4,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(U4,[1]Weapon!$A$1:$M$259,9,FALSE),0)</f>
+      <c r="I4" s="16">
+        <f>H4+_xlfn.IFNA(VLOOKUP(N4,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(P4,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(R4,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(T4,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(V4,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(X4,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(Z4,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(AB4,[1]Weapon!$A$1:$M$259,9,FALSE),0)</f>
         <v>5</v>
       </c>
-      <c r="J4" s="1">
+      <c r="J4" s="20">
         <v>2</v>
       </c>
-      <c r="K4" s="19">
+      <c r="K4" s="16">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="L4" s="1">
+      <c r="L4" s="20">
         <v>6</v>
       </c>
-      <c r="M4" s="19">
+      <c r="M4" s="16">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="N4" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="O4" s="1" t="s">
+      <c r="P4" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="P4" s="4" t="s">
+      <c r="R4" s="31" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="S4" s="4"/>
+      <c r="T4" s="20"/>
+      <c r="V4" s="20"/>
+      <c r="X4" s="20"/>
+      <c r="Z4" s="20"/>
+      <c r="AB4" s="20"/>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ROBO</v>
@@ -8902,45 +9124,52 @@
       <c r="E5" s="1">
         <v>60</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5" s="20">
         <v>0</v>
       </c>
-      <c r="G5" s="19">
+      <c r="G5" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H5" s="1">
+      <c r="H5" s="20">
         <v>6</v>
       </c>
-      <c r="I5" s="19">
-        <f>H5+_xlfn.IFNA(VLOOKUP(N5,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(O5,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(P5,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(Q5,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(R5,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(S5,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(T5,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(U5,[1]Weapon!$A$1:$M$259,9,FALSE),0)</f>
+      <c r="I5" s="16">
+        <f>H5+_xlfn.IFNA(VLOOKUP(N5,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(P5,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(R5,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(T5,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(V5,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(X5,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(Z5,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(AB5,[1]Weapon!$A$1:$M$259,9,FALSE),0)</f>
         <v>6</v>
       </c>
-      <c r="J5" s="1">
+      <c r="J5" s="20">
         <v>5</v>
       </c>
-      <c r="K5" s="19">
+      <c r="K5" s="16">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="L5" s="1">
+      <c r="L5" s="20">
         <v>0</v>
       </c>
-      <c r="M5" s="19">
+      <c r="M5" s="16">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N5" s="5" t="s">
+      <c r="N5" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="O5" s="1" t="s">
+      <c r="O5" s="5"/>
+      <c r="P5" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="P5" s="9" t="s">
+      <c r="R5" s="32" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="S5" s="9"/>
+      <c r="T5" s="20"/>
+      <c r="V5" s="20"/>
+      <c r="X5" s="20"/>
+      <c r="Z5" s="20"/>
+      <c r="AB5" s="20"/>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Zappo</v>
@@ -8954,58 +9183,66 @@
       <c r="E6" s="1">
         <v>200</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="20">
         <v>4</v>
       </c>
-      <c r="G6" s="19">
+      <c r="G6" s="16">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="H6" s="1">
+      <c r="H6" s="20">
         <v>0</v>
       </c>
-      <c r="I6" s="19">
-        <f>H6+_xlfn.IFNA(VLOOKUP(N6,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(O6,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(P6,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(Q6,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(R6,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(S6,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(T6,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(U6,[1]Weapon!$A$1:$M$259,9,FALSE),0)</f>
+      <c r="I6" s="16">
+        <f>H6+_xlfn.IFNA(VLOOKUP(N6,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(P6,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(R6,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(T6,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(V6,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(X6,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(Z6,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(AB6,[1]Weapon!$A$1:$M$259,9,FALSE),0)</f>
         <v>21</v>
       </c>
-      <c r="J6" s="1">
+      <c r="J6" s="20">
         <v>5</v>
       </c>
-      <c r="K6" s="19">
+      <c r="K6" s="16">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="L6" s="1">
+      <c r="L6" s="20">
         <v>6</v>
       </c>
-      <c r="M6" s="19">
+      <c r="M6" s="16">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="N6" s="1" t="s">
+      <c r="N6" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="O6" s="2" t="s">
+      <c r="P6" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="P6" s="3" t="s">
+      <c r="Q6" s="2"/>
+      <c r="R6" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="Q6" s="3" t="s">
+      <c r="S6" s="3"/>
+      <c r="T6" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="R6" s="6" t="s">
+      <c r="U6" s="3"/>
+      <c r="V6" s="34" t="s">
         <v>64</v>
       </c>
-      <c r="S6" s="12" t="s">
+      <c r="W6" s="6"/>
+      <c r="X6" s="27" t="s">
         <v>81</v>
       </c>
-      <c r="V6" s="20" t="s">
+      <c r="Y6" s="12"/>
+      <c r="Z6" s="20"/>
+      <c r="AB6" s="20"/>
+      <c r="AD6" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="W6" s="20"/>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="AE6" s="17"/>
+      <c r="AF6" s="17"/>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Flammie</v>
@@ -9019,48 +9256,55 @@
       <c r="E7" s="1">
         <v>999</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="20">
         <v>2</v>
       </c>
-      <c r="G7" s="19">
+      <c r="G7" s="16">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="H7" s="1">
+      <c r="H7" s="20">
         <v>99</v>
       </c>
-      <c r="I7" s="19">
-        <f>H7+_xlfn.IFNA(VLOOKUP(N7,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(O7,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(P7,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(Q7,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(R7,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(S7,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(T7,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(U7,[1]Weapon!$A$1:$M$259,9,FALSE),0)</f>
+      <c r="I7" s="16">
+        <f>H7+_xlfn.IFNA(VLOOKUP(N7,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(P7,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(R7,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(T7,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(V7,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(X7,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(Z7,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(AB7,[1]Weapon!$A$1:$M$259,9,FALSE),0)</f>
         <v>99</v>
       </c>
-      <c r="J7" s="1">
+      <c r="J7" s="20">
         <v>50</v>
       </c>
-      <c r="K7" s="19">
+      <c r="K7" s="16">
         <f t="shared" si="2"/>
         <v>50</v>
       </c>
-      <c r="L7" s="1">
+      <c r="L7" s="20">
         <v>10</v>
       </c>
-      <c r="M7" s="19">
+      <c r="M7" s="16">
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
-      <c r="N7" s="1" t="s">
+      <c r="N7" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="O7" s="1" t="s">
+      <c r="P7" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="P7" s="3" t="s">
+      <c r="R7" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="V7" s="20" t="s">
+      <c r="S7" s="3"/>
+      <c r="T7" s="20"/>
+      <c r="V7" s="20"/>
+      <c r="X7" s="20"/>
+      <c r="Z7" s="20"/>
+      <c r="AB7" s="20"/>
+      <c r="AD7" s="17" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="AE7" s="17"/>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Slashy</v>
@@ -9074,48 +9318,56 @@
       <c r="E8" s="1">
         <v>400</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8" s="20">
         <v>30</v>
       </c>
-      <c r="G8" s="19">
+      <c r="G8" s="16">
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="H8" s="1">
+      <c r="H8" s="20">
         <v>50</v>
       </c>
-      <c r="I8" s="19">
-        <f>H8+_xlfn.IFNA(VLOOKUP(N8,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(O8,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(P8,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(Q8,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(R8,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(S8,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(T8,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(U8,[1]Weapon!$A$1:$M$259,9,FALSE),0)</f>
+      <c r="I8" s="16">
+        <f>H8+_xlfn.IFNA(VLOOKUP(N8,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(P8,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(R8,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(T8,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(V8,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(X8,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(Z8,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(AB8,[1]Weapon!$A$1:$M$259,9,FALSE),0)</f>
         <v>50</v>
       </c>
-      <c r="J8" s="1">
+      <c r="J8" s="20">
         <v>25</v>
       </c>
-      <c r="K8" s="19">
+      <c r="K8" s="16">
         <f t="shared" si="2"/>
         <v>25</v>
       </c>
-      <c r="L8" s="1">
+      <c r="L8" s="20">
         <v>30</v>
       </c>
-      <c r="M8" s="19">
+      <c r="M8" s="16">
         <f t="shared" si="3"/>
         <v>30</v>
       </c>
-      <c r="N8" s="7" t="s">
+      <c r="N8" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="O8" s="8" t="s">
+      <c r="O8" s="7"/>
+      <c r="P8" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="P8" s="22" t="s">
+      <c r="Q8" s="8"/>
+      <c r="R8" s="30" t="s">
         <v>121</v>
       </c>
-      <c r="Q8" s="22" t="s">
+      <c r="S8" s="19"/>
+      <c r="T8" s="30" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="U8" s="19"/>
+      <c r="V8" s="20"/>
+      <c r="X8" s="20"/>
+      <c r="Z8" s="20"/>
+      <c r="AB8" s="20"/>
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Revenge</v>
@@ -9129,42 +9381,50 @@
       <c r="E9" s="1">
         <v>100</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9" s="20">
         <v>15</v>
       </c>
-      <c r="G9" s="19">
+      <c r="G9" s="16">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="H9" s="1">
+      <c r="H9" s="20">
         <v>9</v>
       </c>
-      <c r="I9" s="19">
-        <f>H9+_xlfn.IFNA(VLOOKUP(N9,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(O9,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(P9,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(Q9,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(R9,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(S9,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(T9,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(U9,[1]Weapon!$A$1:$M$259,9,FALSE),0)</f>
+      <c r="I9" s="16">
+        <f>H9+_xlfn.IFNA(VLOOKUP(N9,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(P9,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(R9,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(T9,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(V9,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(X9,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(Z9,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(AB9,[1]Weapon!$A$1:$M$259,9,FALSE),0)</f>
         <v>9</v>
       </c>
-      <c r="J9" s="1">
+      <c r="J9" s="20">
         <v>8</v>
       </c>
-      <c r="K9" s="19">
+      <c r="K9" s="16">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="L9" s="1">
+      <c r="L9" s="20">
         <v>3</v>
       </c>
-      <c r="M9" s="19">
+      <c r="M9" s="16">
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="N9" s="13" t="s">
+      <c r="N9" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="O9" s="22" t="s">
+      <c r="O9" s="13"/>
+      <c r="P9" s="30" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Q9" s="19"/>
+      <c r="R9" s="20"/>
+      <c r="T9" s="20"/>
+      <c r="V9" s="20"/>
+      <c r="X9" s="20"/>
+      <c r="Z9" s="20"/>
+      <c r="AB9" s="20"/>
+    </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Turtle1</v>
@@ -9178,39 +9438,47 @@
       <c r="E10" s="1">
         <v>100</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F10" s="20">
         <v>2</v>
       </c>
-      <c r="G10" s="19">
+      <c r="G10" s="16">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="H10" s="1">
+      <c r="H10" s="20">
         <v>9</v>
       </c>
-      <c r="I10" s="19">
-        <f>H10+_xlfn.IFNA(VLOOKUP(N10,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(O10,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(P10,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(Q10,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(R10,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(S10,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(T10,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(U10,[1]Weapon!$A$1:$M$259,9,FALSE),0)</f>
+      <c r="I10" s="16">
+        <f>H10+_xlfn.IFNA(VLOOKUP(N10,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(P10,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(R10,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(T10,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(V10,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(X10,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(Z10,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(AB10,[1]Weapon!$A$1:$M$259,9,FALSE),0)</f>
         <v>9</v>
       </c>
-      <c r="J10" s="1">
+      <c r="J10" s="20">
         <v>10</v>
       </c>
-      <c r="K10" s="19">
+      <c r="K10" s="16">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="L10" s="1">
+      <c r="L10" s="20">
         <v>10</v>
       </c>
-      <c r="M10" s="19">
+      <c r="M10" s="16">
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
-      <c r="N10" s="14" t="s">
+      <c r="N10" s="24" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="O10" s="14"/>
+      <c r="P10" s="20"/>
+      <c r="R10" s="20"/>
+      <c r="T10" s="20"/>
+      <c r="V10" s="20"/>
+      <c r="X10" s="20"/>
+      <c r="Z10" s="20"/>
+      <c r="AB10" s="20"/>
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Turtle2</v>
@@ -9224,213 +9492,304 @@
       <c r="E11" s="1">
         <v>100</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F11" s="20">
         <v>2</v>
       </c>
-      <c r="G11" s="19">
+      <c r="G11" s="16">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="H11" s="1">
+      <c r="H11" s="20">
         <v>9</v>
       </c>
-      <c r="I11" s="19">
-        <f>H11+_xlfn.IFNA(VLOOKUP(N11,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(O11,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(P11,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(Q11,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(R11,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(S11,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(T11,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(U11,[1]Weapon!$A$1:$M$259,9,FALSE),0)</f>
+      <c r="I11" s="16">
+        <f>H11+_xlfn.IFNA(VLOOKUP(N11,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(P11,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(R11,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(T11,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(V11,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(X11,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(Z11,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(AB11,[1]Weapon!$A$1:$M$259,9,FALSE),0)</f>
         <v>9</v>
       </c>
-      <c r="J11" s="1">
+      <c r="J11" s="20">
         <v>10</v>
       </c>
-      <c r="K11" s="19">
+      <c r="K11" s="16">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="L11" s="1">
+      <c r="L11" s="20">
         <v>10</v>
       </c>
-      <c r="M11" s="19">
+      <c r="M11" s="16">
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
-      <c r="N11" s="14" t="s">
+      <c r="N11" s="24" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="O11" s="14"/>
+      <c r="P11" s="20"/>
+      <c r="R11" s="20"/>
+      <c r="T11" s="20"/>
+      <c r="V11" s="20"/>
+      <c r="X11" s="20"/>
+      <c r="Z11" s="20"/>
+      <c r="AB11" s="20"/>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Leonardo</v>
       </c>
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="D12" s="20" t="s">
+      <c r="D12" s="17" t="s">
         <v>77</v>
       </c>
       <c r="E12" s="1">
         <v>250</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F12" s="20">
         <v>30</v>
       </c>
-      <c r="G12" s="19">
+      <c r="G12" s="16">
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="H12" s="1">
+      <c r="H12" s="20">
         <v>15</v>
       </c>
-      <c r="I12" s="19">
-        <f>H12+_xlfn.IFNA(VLOOKUP(N12,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(O12,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(P12,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(Q12,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(R12,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(S12,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(T12,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(U12,[1]Weapon!$A$1:$M$259,9,FALSE),0)</f>
+      <c r="I12" s="16">
+        <f>H12+_xlfn.IFNA(VLOOKUP(N12,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(P12,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(R12,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(T12,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(V12,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(X12,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(Z12,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(AB12,[1]Weapon!$A$1:$M$259,9,FALSE),0)</f>
         <v>15</v>
       </c>
-      <c r="J12" s="1">
+      <c r="J12" s="20">
         <v>50</v>
       </c>
-      <c r="K12" s="19">
+      <c r="K12" s="16">
         <f t="shared" si="2"/>
         <v>50</v>
       </c>
-      <c r="L12" s="1">
+      <c r="L12" s="20">
         <v>11</v>
       </c>
-      <c r="M12" s="19">
+      <c r="M12" s="16">
         <f t="shared" si="3"/>
         <v>11</v>
       </c>
-      <c r="N12" s="20" t="s">
+      <c r="N12" s="25" t="s">
         <v>96</v>
       </c>
-      <c r="O12" s="20" t="s">
+      <c r="O12" s="17"/>
+      <c r="P12" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="P12" s="20" t="s">
+      <c r="Q12" s="17"/>
+      <c r="R12" s="25" t="s">
         <v>95</v>
       </c>
-      <c r="Q12" s="22" t="s">
+      <c r="S12" s="17"/>
+      <c r="T12" s="30" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="U12" s="19"/>
+      <c r="V12" s="20"/>
+      <c r="X12" s="20"/>
+      <c r="Z12" s="20"/>
+      <c r="AB12" s="20"/>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Isis</v>
       </c>
-      <c r="B13" s="21" t="s">
+      <c r="B13" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="D13" s="21" t="s">
+      <c r="D13" s="18" t="s">
         <v>78</v>
       </c>
       <c r="E13" s="1">
         <v>999</v>
       </c>
-      <c r="F13" s="1">
+      <c r="F13" s="20">
         <v>99</v>
       </c>
-      <c r="G13" s="19">
+      <c r="G13" s="16">
         <f t="shared" si="1"/>
         <v>99</v>
       </c>
-      <c r="H13" s="1">
+      <c r="H13" s="20">
         <v>99</v>
       </c>
-      <c r="I13" s="19">
-        <f>H13+_xlfn.IFNA(VLOOKUP(N13,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(O13,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(P13,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(Q13,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(R13,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(S13,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(T13,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(U13,[1]Weapon!$A$1:$M$259,9,FALSE),0)</f>
+      <c r="I13" s="16">
+        <f>H13+_xlfn.IFNA(VLOOKUP(N13,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(P13,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(R13,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(T13,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(V13,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(X13,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(Z13,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(AB13,[1]Weapon!$A$1:$M$259,9,FALSE),0)</f>
         <v>99</v>
       </c>
-      <c r="J13" s="1">
+      <c r="J13" s="20">
         <v>99</v>
       </c>
-      <c r="K13" s="19">
+      <c r="K13" s="16">
         <f t="shared" si="2"/>
         <v>99</v>
       </c>
-      <c r="L13" s="1">
+      <c r="L13" s="20">
         <v>99</v>
       </c>
-      <c r="M13" s="19">
+      <c r="M13" s="16">
         <f t="shared" si="3"/>
         <v>99</v>
       </c>
-      <c r="N13" s="21" t="s">
+      <c r="N13" s="26" t="s">
         <v>106</v>
       </c>
-      <c r="O13" s="21" t="s">
+      <c r="O13" s="18"/>
+      <c r="P13" s="26" t="s">
         <v>107</v>
       </c>
-      <c r="P13" s="22" t="s">
+      <c r="Q13" s="18"/>
+      <c r="R13" s="30" t="s">
         <v>111</v>
       </c>
-      <c r="Q13" s="22" t="s">
+      <c r="S13" s="19"/>
+      <c r="T13" s="30" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="U13" s="19"/>
+      <c r="V13" s="20"/>
+      <c r="X13" s="20"/>
+      <c r="Z13" s="20"/>
+      <c r="AB13" s="20"/>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="str">
         <f t="shared" si="0"/>
         <v>EyeUponU</v>
       </c>
-      <c r="B14" s="22" t="s">
+      <c r="B14" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="D14" s="22" t="s">
+      <c r="D14" s="19" t="s">
         <v>110</v>
       </c>
       <c r="E14" s="1">
         <v>858</v>
       </c>
-      <c r="F14" s="1">
+      <c r="F14" s="20">
         <v>83</v>
       </c>
-      <c r="G14" s="19">
+      <c r="G14" s="16">
         <f t="shared" si="1"/>
         <v>83</v>
       </c>
-      <c r="H14" s="1">
+      <c r="H14" s="20">
         <v>78</v>
       </c>
-      <c r="I14" s="19">
-        <f>H14+_xlfn.IFNA(VLOOKUP(N14,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(O14,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(P14,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(Q14,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(R14,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(S14,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(T14,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(U14,[1]Weapon!$A$1:$M$259,9,FALSE),0)</f>
+      <c r="I14" s="16">
+        <f>H14+_xlfn.IFNA(VLOOKUP(N14,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(P14,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(R14,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(T14,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(V14,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(X14,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(Z14,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(AB14,[1]Weapon!$A$1:$M$259,9,FALSE),0)</f>
         <v>78</v>
       </c>
-      <c r="J14" s="1">
+      <c r="J14" s="20">
         <v>97</v>
       </c>
-      <c r="K14" s="19">
+      <c r="K14" s="16">
         <f t="shared" si="2"/>
         <v>97</v>
       </c>
-      <c r="L14" s="1">
+      <c r="L14" s="20">
         <v>86</v>
       </c>
-      <c r="M14" s="19">
+      <c r="M14" s="16">
         <f t="shared" si="3"/>
         <v>86</v>
       </c>
-      <c r="N14" s="1" t="s">
+      <c r="N14" s="20" t="s">
         <v>113</v>
       </c>
-      <c r="O14" s="1" t="s">
+      <c r="P14" s="20" t="s">
         <v>114</v>
       </c>
-      <c r="P14" s="1" t="s">
+      <c r="R14" s="20" t="s">
         <v>115</v>
       </c>
-      <c r="Q14" s="1" t="s">
+      <c r="T14" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="R14" s="1" t="s">
+      <c r="V14" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="S14" s="1" t="s">
+      <c r="X14" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="T14" s="1" t="s">
+      <c r="Z14" s="20" t="s">
         <v>118</v>
       </c>
-      <c r="U14" s="1" t="s">
+      <c r="AB14" s="20" t="s">
         <v>119</v>
+      </c>
+    </row>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>HypnoToad</v>
+      </c>
+      <c r="B15" s="42" t="s">
+        <v>139</v>
+      </c>
+      <c r="D15" s="42" t="s">
+        <v>108</v>
+      </c>
+      <c r="E15" s="1">
+        <v>885</v>
+      </c>
+      <c r="F15" s="20">
+        <v>86</v>
+      </c>
+      <c r="G15" s="16">
+        <f t="shared" si="1"/>
+        <v>86</v>
+      </c>
+      <c r="H15" s="20">
+        <v>83</v>
+      </c>
+      <c r="I15" s="16">
+        <f>H15+_xlfn.IFNA(VLOOKUP(N15,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(P15,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(R15,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(T15,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(V15,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(X15,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(Z15,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(AB15,[1]Weapon!$A$1:$M$259,9,FALSE),0)</f>
+        <v>83</v>
+      </c>
+      <c r="J15" s="20">
+        <v>91</v>
+      </c>
+      <c r="K15" s="16">
+        <f t="shared" si="2"/>
+        <v>91</v>
+      </c>
+      <c r="L15" s="20">
+        <v>80</v>
+      </c>
+      <c r="M15" s="16">
+        <f t="shared" si="3"/>
+        <v>80</v>
+      </c>
+      <c r="N15" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="P15" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="R15" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="T15" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="V15" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="X15" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="Z15" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="AB15" s="20" t="s">
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -9445,7 +9804,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9562,7 +9921,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:T6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9739,7 +10098,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:T6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9913,7 +10272,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:T5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10049,7 +10408,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:T5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10185,7 +10544,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10303,7 +10662,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10420,7 +10779,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10537,7 +10896,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10677,7 +11036,7 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10817,8 +11176,149 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:T4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="4" width="11.7109375" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" t="s">
+        <v>25</v>
+      </c>
+      <c r="P1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R1" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1" t="s">
+        <v>24</v>
+      </c>
+      <c r="T1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="K2" t="s">
+        <v>53</v>
+      </c>
+      <c r="L2" t="s">
+        <v>4</v>
+      </c>
+      <c r="T2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="K3" t="s">
+        <v>3</v>
+      </c>
+      <c r="L3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10910,144 +11410,6 @@
         <v>1</v>
       </c>
       <c r="D2">
-        <v>2</v>
-      </c>
-      <c r="K2" t="s">
-        <v>53</v>
-      </c>
-      <c r="L2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="K3" t="s">
-        <v>3</v>
-      </c>
-      <c r="L3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P1" sqref="P1:P1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="3" max="4" width="11.7109375" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L1" t="s">
-        <v>16</v>
-      </c>
-      <c r="M1" t="s">
-        <v>26</v>
-      </c>
-      <c r="N1" t="s">
-        <v>21</v>
-      </c>
-      <c r="O1" t="s">
-        <v>25</v>
-      </c>
-      <c r="P1" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>22</v>
-      </c>
-      <c r="R1" t="s">
-        <v>23</v>
-      </c>
-      <c r="S1" t="s">
-        <v>24</v>
-      </c>
-      <c r="T1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
         <v>1</v>
       </c>
       <c r="F2">
@@ -11094,7 +11456,7 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11211,7 +11573,7 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11328,7 +11690,7 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:T6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11505,7 +11867,143 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6CE5A13-43F3-4D09-BA0A-70545C4F6BB2}">
+  <dimension ref="A1:T5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" t="s">
+        <v>25</v>
+      </c>
+      <c r="P1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R1" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1" t="s">
+        <v>24</v>
+      </c>
+      <c r="T1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="K2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11621,8 +12119,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11738,8 +12236,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11855,8 +12353,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11972,8 +12470,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12089,122 +12587,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L1" t="s">
-        <v>16</v>
-      </c>
-      <c r="M1" t="s">
-        <v>26</v>
-      </c>
-      <c r="N1" t="s">
-        <v>21</v>
-      </c>
-      <c r="O1" t="s">
-        <v>25</v>
-      </c>
-      <c r="P1" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>22</v>
-      </c>
-      <c r="R1" t="s">
-        <v>23</v>
-      </c>
-      <c r="S1" t="s">
-        <v>24</v>
-      </c>
-      <c r="T1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="K2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>125</v>
-      </c>
-      <c r="B3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:T5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12353,7 +12737,121 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
+  <dimension ref="A1:T3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" t="s">
+        <v>25</v>
+      </c>
+      <c r="P1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R1" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1" t="s">
+        <v>24</v>
+      </c>
+      <c r="T1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="K2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12466,8 +12964,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12581,8 +13079,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
   <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12713,8 +13211,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2000-000000000000}">
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12831,8 +13329,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2100-000000000000}">
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12949,8 +13447,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2200-000000000000}">
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13067,8 +13565,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2300-000000000000}">
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13185,8 +13683,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2400-000000000000}">
   <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13317,11 +13815,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2500-000000000000}">
   <dimension ref="A1:T7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
@@ -13512,7 +14010,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13630,7 +14128,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13745,7 +14243,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:T3"/>
   <sheetViews>
@@ -13863,7 +14361,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13980,7 +14478,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -14097,12 +14595,12 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P1" sqref="P1:P1048576"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -14195,10 +14693,13 @@
       <c r="K2" t="s">
         <v>55</v>
       </c>
+      <c r="L2" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>147</v>
       </c>
       <c r="B3" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
Added HP gain for humans and mutants
</commit_message>
<xml_diff>
--- a/Battle Log.xlsx
+++ b/Battle Log.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Action IV\Documents\GitHub\pillar\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scrummel\source\repos\pillar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A4FA8AC-6485-4962-8C3B-338EB00625AA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="838" firstSheet="12" activeTab="23" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="838" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Players" sheetId="16" r:id="rId1"/>
@@ -56,7 +55,7 @@
   <externalReferences>
     <externalReference r:id="rId40"/>
   </externalReferences>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -513,7 +512,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -774,7 +773,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -807,10 +806,11 @@
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Monster"/>
-      <sheetName val="Magic"/>
+      <sheetName val="Growth Rates"/>
+      <sheetName val="Mutant Skills"/>
+      <sheetName val="Encounters"/>
       <sheetName val="Evolve"/>
       <sheetName val="Weapon"/>
-      <sheetName val="Items"/>
       <sheetName val="Treasure"/>
       <sheetName val="Shops"/>
       <sheetName val="Item Hex"/>
@@ -821,7 +821,9 @@
       <sheetData sheetId="0"/>
       <sheetData sheetId="1"/>
       <sheetData sheetId="2"/>
-      <sheetData sheetId="3">
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5">
         <row r="1">
           <cell r="A1" t="str">
             <v>Index</v>
@@ -8448,12 +8450,11 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
       <sheetData sheetId="6"/>
       <sheetData sheetId="7"/>
       <sheetData sheetId="8"/>
       <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -8535,23 +8536,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -8587,23 +8571,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -8779,11 +8746,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9804,7 +9771,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9921,7 +9888,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10098,7 +10065,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10272,7 +10239,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10408,7 +10375,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10544,7 +10511,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10662,7 +10629,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10779,7 +10746,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10896,7 +10863,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11036,7 +11003,7 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11176,7 +11143,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:T4"/>
   <sheetViews>
@@ -11318,7 +11285,7 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11456,7 +11423,7 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11573,7 +11540,7 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11690,7 +11657,7 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11867,10 +11834,10 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6CE5A13-43F3-4D09-BA0A-70545C4F6BB2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
@@ -12003,7 +11970,7 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12120,7 +12087,7 @@
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12237,7 +12204,7 @@
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12354,7 +12321,7 @@
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12471,7 +12438,7 @@
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12588,7 +12555,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12737,7 +12704,7 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12851,7 +12818,7 @@
 </file>
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12965,7 +12932,7 @@
 </file>
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13080,7 +13047,7 @@
 </file>
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13212,7 +13179,7 @@
 </file>
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13330,7 +13297,7 @@
 </file>
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13448,7 +13415,7 @@
 </file>
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13566,7 +13533,7 @@
 </file>
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13684,7 +13651,7 @@
 </file>
 
 <file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13816,7 +13783,7 @@
 </file>
 
 <file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -14010,7 +13977,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -14128,7 +14095,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -14243,12 +14210,12 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P1" sqref="P1:P1048576"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -14361,7 +14328,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -14478,11 +14445,11 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -14575,12 +14542,12 @@
         <v>97</v>
       </c>
       <c r="L2" t="s">
-        <v>27</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>19</v>
@@ -14595,7 +14562,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:T3"/>
   <sheetViews>

</xml_diff>

<commit_message>
Added Item Drops, hit
</commit_message>
<xml_diff>
--- a/Battle Log.xlsx
+++ b/Battle Log.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Action IV\Documents\GitHub\pillar\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scrummel\source\repos\pillar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3DAC3A1-589E-4868-83D1-4C25714FF854}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="838" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="838"/>
   </bookViews>
   <sheets>
     <sheet name="Players" sheetId="16" r:id="rId1"/>
@@ -23,45 +22,46 @@
     <sheet name="Bow" sheetId="40" r:id="rId8"/>
     <sheet name="Shield" sheetId="7" r:id="rId9"/>
     <sheet name="Group MANA - PC" sheetId="9" r:id="rId10"/>
-    <sheet name="Group MANA - Enemy" sheetId="11" r:id="rId11"/>
-    <sheet name="Barrier" sheetId="24" r:id="rId12"/>
-    <sheet name="All Enemies - PC" sheetId="13" r:id="rId13"/>
-    <sheet name="All Enemies - Dead Test" sheetId="23" r:id="rId14"/>
-    <sheet name="Single Gun" sheetId="14" r:id="rId15"/>
-    <sheet name="Group Static" sheetId="15" r:id="rId16"/>
-    <sheet name="O-Weapon" sheetId="20" r:id="rId17"/>
-    <sheet name="PC Cure - Magic" sheetId="17" r:id="rId18"/>
-    <sheet name="PC Cure - Item" sheetId="18" r:id="rId19"/>
-    <sheet name="PC All Heal" sheetId="19" r:id="rId20"/>
-    <sheet name="Status Effect" sheetId="21" r:id="rId21"/>
-    <sheet name="Group Status" sheetId="22" r:id="rId22"/>
-    <sheet name="All Enemies - Status" sheetId="28" r:id="rId23"/>
-    <sheet name="Confuse Enemies" sheetId="51" r:id="rId24"/>
-    <sheet name="Weak - Elem Melee" sheetId="26" r:id="rId25"/>
-    <sheet name="Weak - Race Melee" sheetId="27" r:id="rId26"/>
-    <sheet name="Drain Reversal" sheetId="44" r:id="rId27"/>
-    <sheet name="Drain Success" sheetId="45" r:id="rId28"/>
-    <sheet name="Multi-hit" sheetId="46" r:id="rId29"/>
-    <sheet name="Buff and Debuff" sheetId="47" r:id="rId30"/>
-    <sheet name="Reflect" sheetId="31" r:id="rId31"/>
-    <sheet name="STR Counter" sheetId="32" r:id="rId32"/>
-    <sheet name="Other Counters" sheetId="33" r:id="rId33"/>
-    <sheet name="ChainSaw" sheetId="48" r:id="rId34"/>
-    <sheet name="Enemy Surprise" sheetId="36" r:id="rId35"/>
-    <sheet name="Player Surprise" sheetId="37" r:id="rId36"/>
-    <sheet name="Both Surprise" sheetId="38" r:id="rId37"/>
-    <sheet name="Run" sheetId="49" r:id="rId38"/>
-    <sheet name="Heart" sheetId="50" r:id="rId39"/>
+    <sheet name="Group Reflect" sheetId="52" r:id="rId11"/>
+    <sheet name="Group MANA - Enemy" sheetId="11" r:id="rId12"/>
+    <sheet name="Barrier" sheetId="24" r:id="rId13"/>
+    <sheet name="All Enemies - PC" sheetId="13" r:id="rId14"/>
+    <sheet name="All Enemies - Dead Test" sheetId="23" r:id="rId15"/>
+    <sheet name="Single Gun" sheetId="14" r:id="rId16"/>
+    <sheet name="Group Static" sheetId="15" r:id="rId17"/>
+    <sheet name="O-Weapon" sheetId="20" r:id="rId18"/>
+    <sheet name="PC Cure - Magic" sheetId="17" r:id="rId19"/>
+    <sheet name="PC Cure - Item" sheetId="18" r:id="rId20"/>
+    <sheet name="PC All Heal" sheetId="19" r:id="rId21"/>
+    <sheet name="Status Effect" sheetId="21" r:id="rId22"/>
+    <sheet name="Group Status" sheetId="22" r:id="rId23"/>
+    <sheet name="All Enemies - Status" sheetId="28" r:id="rId24"/>
+    <sheet name="Confuse Enemies" sheetId="51" r:id="rId25"/>
+    <sheet name="Weak - Elem Melee" sheetId="26" r:id="rId26"/>
+    <sheet name="Weak - Race Melee" sheetId="27" r:id="rId27"/>
+    <sheet name="Drain Reversal" sheetId="44" r:id="rId28"/>
+    <sheet name="Drain Success" sheetId="45" r:id="rId29"/>
+    <sheet name="Multi-hit" sheetId="46" r:id="rId30"/>
+    <sheet name="Buff and Debuff" sheetId="47" r:id="rId31"/>
+    <sheet name="Reflect" sheetId="31" r:id="rId32"/>
+    <sheet name="STR Counter" sheetId="32" r:id="rId33"/>
+    <sheet name="Other Counters" sheetId="33" r:id="rId34"/>
+    <sheet name="ChainSaw" sheetId="48" r:id="rId35"/>
+    <sheet name="Enemy Surprise" sheetId="36" r:id="rId36"/>
+    <sheet name="Player Surprise" sheetId="37" r:id="rId37"/>
+    <sheet name="Both Surprise" sheetId="38" r:id="rId38"/>
+    <sheet name="Run" sheetId="49" r:id="rId39"/>
+    <sheet name="Heart" sheetId="50" r:id="rId40"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId40"/>
+    <externalReference r:id="rId41"/>
   </externalReferences>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1228" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1259" uniqueCount="153">
   <si>
     <t>NAME</t>
   </si>
@@ -511,12 +511,21 @@
   </si>
   <si>
     <t>STATS USED</t>
+  </si>
+  <si>
+    <t>SpellGod</t>
+  </si>
+  <si>
+    <t>Thunder Book</t>
+  </si>
+  <si>
+    <t>Rakshasa</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -777,7 +786,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -3255,13 +3264,13 @@
         </row>
         <row r="75">
           <cell r="A75" t="str">
-            <v>Chop Art</v>
+            <v>Strike</v>
           </cell>
           <cell r="B75" t="str">
-            <v>Chop Art</v>
+            <v>Strike</v>
           </cell>
           <cell r="C75" t="str">
-            <v>Chop</v>
+            <v>Strike</v>
           </cell>
           <cell r="D75" t="str">
             <v>Art</v>
@@ -3287,13 +3296,13 @@
         </row>
         <row r="76">
           <cell r="A76" t="str">
-            <v>Kick Art</v>
+            <v>Elbow</v>
           </cell>
           <cell r="B76" t="str">
-            <v>Kick Art</v>
+            <v>Elbow</v>
           </cell>
           <cell r="C76" t="str">
-            <v>Kick</v>
+            <v>Elbow</v>
           </cell>
           <cell r="D76" t="str">
             <v>Art</v>
@@ -3319,13 +3328,13 @@
         </row>
         <row r="77">
           <cell r="A77" t="str">
-            <v>HeadBut Art</v>
+            <v>HeadButt</v>
           </cell>
           <cell r="B77" t="str">
-            <v>HeadBut Art</v>
+            <v>HeadButt</v>
           </cell>
           <cell r="C77" t="str">
-            <v>HeadBut</v>
+            <v>HeadButt</v>
           </cell>
           <cell r="D77" t="str">
             <v>Art</v>
@@ -3351,10 +3360,10 @@
         </row>
         <row r="78">
           <cell r="A78" t="str">
-            <v>Roundhouse Art</v>
+            <v>Roundhouse</v>
           </cell>
           <cell r="B78" t="str">
-            <v>Roundhouse Art</v>
+            <v>Roundhouse</v>
           </cell>
           <cell r="C78" t="str">
             <v>Roundhouse</v>
@@ -3383,10 +3392,10 @@
         </row>
         <row r="79">
           <cell r="A79" t="str">
-            <v>Jyudo Art</v>
+            <v>Jyudo</v>
           </cell>
           <cell r="B79" t="str">
-            <v>Jyudo Art</v>
+            <v>Jyudo</v>
           </cell>
           <cell r="C79" t="str">
             <v>Jyudo</v>
@@ -3415,10 +3424,10 @@
         </row>
         <row r="80">
           <cell r="A80" t="str">
-            <v>Karate Art</v>
+            <v>Karate</v>
           </cell>
           <cell r="B80" t="str">
-            <v>Karate Art</v>
+            <v>Karate</v>
           </cell>
           <cell r="C80" t="str">
             <v>Karate</v>
@@ -3525,9 +3534,6 @@
           <cell r="G83">
             <v>30</v>
           </cell>
-          <cell r="H83">
-            <v>0</v>
-          </cell>
           <cell r="L83">
             <v>9</v>
           </cell>
@@ -3554,9 +3560,6 @@
           <cell r="G84">
             <v>30</v>
           </cell>
-          <cell r="H84">
-            <v>0</v>
-          </cell>
           <cell r="L84">
             <v>9</v>
           </cell>
@@ -3583,9 +3586,6 @@
           <cell r="G85">
             <v>30</v>
           </cell>
-          <cell r="H85">
-            <v>0</v>
-          </cell>
           <cell r="L85">
             <v>9</v>
           </cell>
@@ -3656,10 +3656,10 @@
         </row>
         <row r="88">
           <cell r="A88" t="str">
-            <v>Bazooka Cannon</v>
+            <v>Bazooka</v>
           </cell>
           <cell r="B88" t="str">
-            <v>Bazooka Cannon</v>
+            <v>Bazooka</v>
           </cell>
           <cell r="C88" t="str">
             <v>Bazooka</v>
@@ -3688,10 +3688,10 @@
         </row>
         <row r="89">
           <cell r="A89" t="str">
-            <v>Vulcan Cannon</v>
+            <v>Vulcan</v>
           </cell>
           <cell r="B89" t="str">
-            <v>Vulcan Cannon</v>
+            <v>Vulcan</v>
           </cell>
           <cell r="C89" t="str">
             <v>Vulcan</v>
@@ -3720,10 +3720,10 @@
         </row>
         <row r="90">
           <cell r="A90" t="str">
-            <v>Tank Cannon</v>
+            <v>Tank</v>
           </cell>
           <cell r="B90" t="str">
-            <v>Tank Cannon</v>
+            <v>Tank</v>
           </cell>
           <cell r="C90" t="str">
             <v>Tank</v>
@@ -3784,10 +3784,10 @@
         </row>
         <row r="92">
           <cell r="A92" t="str">
-            <v>Missile Cannon</v>
+            <v>Missile</v>
           </cell>
           <cell r="B92" t="str">
-            <v>Missile Cannon</v>
+            <v>Missile</v>
           </cell>
           <cell r="C92" t="str">
             <v>Missile</v>
@@ -4055,10 +4055,10 @@
         </row>
         <row r="100">
           <cell r="A100" t="str">
-            <v>Kimono Armor</v>
+            <v>Kimono</v>
           </cell>
           <cell r="B100" t="str">
-            <v>Kimono Armor</v>
+            <v>Kimono</v>
           </cell>
           <cell r="C100" t="str">
             <v>Kimono</v>
@@ -4160,10 +4160,10 @@
         </row>
         <row r="103">
           <cell r="A103" t="str">
-            <v>Gungnir Spear</v>
+            <v>Gungnir</v>
           </cell>
           <cell r="B103" t="str">
-            <v>Gungnir Spear</v>
+            <v>Gungnir</v>
           </cell>
           <cell r="C103" t="str">
             <v>Gungnir</v>
@@ -8540,23 +8540,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -8592,23 +8575,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -8784,11 +8750,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AG15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AG16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8924,7 +8890,7 @@
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="str">
-        <f t="shared" ref="A2:A15" si="0">B2</f>
+        <f t="shared" ref="A2:A16" si="0">B2</f>
         <v>HUME</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -9004,7 +8970,7 @@
         <v>4</v>
       </c>
       <c r="G3" s="16">
-        <f t="shared" ref="G3:G15" si="1">F3</f>
+        <f t="shared" ref="G3:G16" si="1">F3</f>
         <v>4</v>
       </c>
       <c r="H3" s="20">
@@ -9018,14 +8984,14 @@
         <v>5</v>
       </c>
       <c r="K3" s="16">
-        <f t="shared" ref="K3:K15" si="2">J3</f>
+        <f t="shared" ref="K3:K16" si="2">J3</f>
         <v>5</v>
       </c>
       <c r="L3" s="20">
         <v>6</v>
       </c>
       <c r="M3" s="16">
-        <f t="shared" ref="M3:M15" si="3">L3</f>
+        <f t="shared" ref="M3:M16" si="3">L3</f>
         <v>6</v>
       </c>
       <c r="N3" s="20" t="s">
@@ -9795,6 +9761,55 @@
       </c>
       <c r="AB15" s="20" t="s">
         <v>146</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>SpellGod</v>
+      </c>
+      <c r="B16" s="42" t="s">
+        <v>150</v>
+      </c>
+      <c r="D16" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="E16" s="1">
+        <v>1500</v>
+      </c>
+      <c r="F16" s="1">
+        <v>99</v>
+      </c>
+      <c r="G16" s="1">
+        <f t="shared" si="1"/>
+        <v>99</v>
+      </c>
+      <c r="H16" s="1">
+        <v>120</v>
+      </c>
+      <c r="I16" s="16">
+        <f>H16+_xlfn.IFNA(VLOOKUP(N16,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(P16,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(R16,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(T16,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(V16,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(X16,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(Z16,[1]Weapon!$A$1:$M$259,9,FALSE),0)+_xlfn.IFNA(VLOOKUP(AB16,[1]Weapon!$A$1:$M$259,9,FALSE),0)</f>
+        <v>120</v>
+      </c>
+      <c r="J16" s="1">
+        <v>120</v>
+      </c>
+      <c r="K16" s="1">
+        <f t="shared" si="2"/>
+        <v>120</v>
+      </c>
+      <c r="L16" s="1">
+        <v>99</v>
+      </c>
+      <c r="M16" s="1">
+        <f t="shared" si="3"/>
+        <v>99</v>
+      </c>
+      <c r="N16" s="42" t="s">
+        <v>151</v>
+      </c>
+      <c r="P16" s="42" t="s">
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -9809,7 +9824,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9929,7 +9944,127 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" t="s">
+        <v>25</v>
+      </c>
+      <c r="P1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R1" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1" t="s">
+        <v>24</v>
+      </c>
+      <c r="T1" t="s">
+        <v>17</v>
+      </c>
+      <c r="U1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="K2" t="s">
+        <v>151</v>
+      </c>
+      <c r="L2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10108,8 +10243,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10285,8 +10420,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10424,8 +10559,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10563,8 +10698,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10684,8 +10819,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10804,8 +10939,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10924,8 +11059,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11067,151 +11202,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
-  <dimension ref="A1:U4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="U1" sqref="U1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L1" t="s">
-        <v>16</v>
-      </c>
-      <c r="M1" t="s">
-        <v>26</v>
-      </c>
-      <c r="N1" t="s">
-        <v>21</v>
-      </c>
-      <c r="O1" t="s">
-        <v>25</v>
-      </c>
-      <c r="P1" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>22</v>
-      </c>
-      <c r="R1" t="s">
-        <v>23</v>
-      </c>
-      <c r="S1" t="s">
-        <v>24</v>
-      </c>
-      <c r="T1" t="s">
-        <v>17</v>
-      </c>
-      <c r="U1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>150</v>
-      </c>
-      <c r="K2" t="s">
-        <v>29</v>
-      </c>
-      <c r="L2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="K3" t="s">
-        <v>60</v>
-      </c>
-      <c r="L3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:U4"/>
   <sheetViews>
@@ -11356,7 +11348,150 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="U1" sqref="U1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" t="s">
+        <v>25</v>
+      </c>
+      <c r="P1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R1" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1" t="s">
+        <v>24</v>
+      </c>
+      <c r="T1" t="s">
+        <v>17</v>
+      </c>
+      <c r="U1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>150</v>
+      </c>
+      <c r="K2" t="s">
+        <v>29</v>
+      </c>
+      <c r="L2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="K3" t="s">
+        <v>60</v>
+      </c>
+      <c r="L3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11496,8 +11631,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11616,8 +11751,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11736,8 +11871,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11916,8 +12051,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12055,8 +12190,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12175,8 +12310,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12295,8 +12430,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12415,8 +12550,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12535,128 +12670,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
-  <dimension ref="A1:U3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="U1" sqref="U1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L1" t="s">
-        <v>16</v>
-      </c>
-      <c r="M1" t="s">
-        <v>26</v>
-      </c>
-      <c r="N1" t="s">
-        <v>21</v>
-      </c>
-      <c r="O1" t="s">
-        <v>25</v>
-      </c>
-      <c r="P1" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>22</v>
-      </c>
-      <c r="R1" t="s">
-        <v>23</v>
-      </c>
-      <c r="S1" t="s">
-        <v>24</v>
-      </c>
-      <c r="T1" t="s">
-        <v>17</v>
-      </c>
-      <c r="U1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="K2" t="s">
-        <v>122</v>
-      </c>
-      <c r="L2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>123</v>
-      </c>
-      <c r="B3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12808,7 +12823,7 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12893,7 +12908,7 @@
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>93</v>
+        <v>68</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
@@ -12905,18 +12920,21 @@
         <v>1</v>
       </c>
       <c r="K2" t="s">
-        <v>124</v>
+        <v>122</v>
+      </c>
+      <c r="L2" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B3" t="s">
         <v>19</v>
       </c>
       <c r="C3">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -12925,7 +12943,7 @@
 </file>
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13010,7 +13028,7 @@
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>93</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
@@ -13022,18 +13040,18 @@
         <v>1</v>
       </c>
       <c r="K2" t="s">
-        <v>80</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>125</v>
       </c>
       <c r="B3" t="s">
         <v>19</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -13042,7 +13060,124 @@
 </file>
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="U1" sqref="U1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" t="s">
+        <v>25</v>
+      </c>
+      <c r="P1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R1" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1" t="s">
+        <v>24</v>
+      </c>
+      <c r="T1" t="s">
+        <v>17</v>
+      </c>
+      <c r="U1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="K2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13159,8 +13294,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2000-000000000000}">
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13294,8 +13429,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2100-000000000000}">
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13415,8 +13550,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2200-000000000000}">
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13536,8 +13671,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2300-000000000000}">
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13657,8 +13792,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2400-000000000000}">
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13778,8 +13913,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2500-000000000000}">
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13913,205 +14048,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2600-000000000000}">
-  <dimension ref="A1:U7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="U2" sqref="U2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L1" t="s">
-        <v>16</v>
-      </c>
-      <c r="M1" t="s">
-        <v>26</v>
-      </c>
-      <c r="N1" t="s">
-        <v>21</v>
-      </c>
-      <c r="O1" t="s">
-        <v>25</v>
-      </c>
-      <c r="P1" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>22</v>
-      </c>
-      <c r="R1" t="s">
-        <v>23</v>
-      </c>
-      <c r="S1" t="s">
-        <v>24</v>
-      </c>
-      <c r="T1" t="s">
-        <v>17</v>
-      </c>
-      <c r="U1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="K2" t="s">
-        <v>53</v>
-      </c>
-      <c r="L2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="K3" t="s">
-        <v>29</v>
-      </c>
-      <c r="L3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>3</v>
-      </c>
-      <c r="K4" t="s">
-        <v>3</v>
-      </c>
-      <c r="L4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5">
-        <v>4</v>
-      </c>
-      <c r="K5" t="s">
-        <v>58</v>
-      </c>
-      <c r="L5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>105</v>
-      </c>
-      <c r="B6" t="s">
-        <v>128</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6">
-        <v>5</v>
-      </c>
-      <c r="K6" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -14231,8 +14169,205 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="U2" sqref="U2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" t="s">
+        <v>25</v>
+      </c>
+      <c r="P1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R1" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1" t="s">
+        <v>24</v>
+      </c>
+      <c r="T1" t="s">
+        <v>17</v>
+      </c>
+      <c r="U1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="K2" t="s">
+        <v>53</v>
+      </c>
+      <c r="L2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="K3" t="s">
+        <v>29</v>
+      </c>
+      <c r="L3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="K4" t="s">
+        <v>3</v>
+      </c>
+      <c r="L4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="K5" t="s">
+        <v>58</v>
+      </c>
+      <c r="L5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>105</v>
+      </c>
+      <c r="B6" t="s">
+        <v>128</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="K6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -14350,7 +14485,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:U3"/>
   <sheetViews>
@@ -14471,7 +14606,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -14591,7 +14726,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -14711,7 +14846,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:U3"/>
   <sheetViews>

</xml_diff>